<commit_message>
add problem 189 and update 209
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2661A4-5381-4557-9FA7-8AEDE849980D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F42E796-03DD-4953-9287-8A1B63FC80EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3521" uniqueCount="1857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3522" uniqueCount="1858">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -5604,6 +5604,9 @@
   </si>
   <si>
     <t>2020.5.14(self)</t>
+  </si>
+  <si>
+    <t>2020.5.18</t>
   </si>
 </sst>
 </file>
@@ -6076,7 +6079,7 @@
   <dimension ref="A1:E1656"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1467" sqref="I1467"/>
+      <selection activeCell="D1190" sqref="D1190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8386,7 +8389,9 @@
       <c r="C190" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D190" s="3"/>
+      <c r="D190" s="3" t="s">
+        <v>1857</v>
+      </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="4">

</xml_diff>

<commit_message>
add problem 141 and update 707
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A8F8F5-EF7D-4F90-84DA-A512896E4B13}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF7AAE4-2E75-4FA5-A6AD-0974DCEC63CA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3883" uniqueCount="2195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3884" uniqueCount="2196">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -6619,6 +6619,9 @@
   </si>
   <si>
     <t>2020.5.25</t>
+  </si>
+  <si>
+    <t>2020.5.26</t>
   </si>
 </sst>
 </file>
@@ -7229,8 +7232,8 @@
   <dimension ref="A1:E1655"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1471" sqref="D1471"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8962,7 +8965,9 @@
       <c r="C142" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D142" s="3"/>
+      <c r="D142" s="3" t="s">
+        <v>2195</v>
+      </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="19">

</xml_diff>

<commit_message>
add problem 160 and update 141 and 142(add photo)
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF100579-471F-4787-8A63-A0260EE76BB3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF205697-3E9E-4362-A00B-A82972F25C85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2220" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="2197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3887" uniqueCount="2198">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -6625,6 +6625,9 @@
   </si>
   <si>
     <t>2020.5.27</t>
+  </si>
+  <si>
+    <t>2020.5.28</t>
   </si>
 </sst>
 </file>
@@ -7236,7 +7239,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9208,7 +9211,9 @@
       <c r="C161" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D161" s="4"/>
+      <c r="D161" s="4" t="s">
+        <v>2197</v>
+      </c>
     </row>
     <row r="162" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="20" t="s">

</xml_diff>

<commit_message>
add problem 19(third self solve)
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF205697-3E9E-4362-A00B-A82972F25C85}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7CEC36-76D2-48D9-ACA1-7689CDEFD694}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2220" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3887" uniqueCount="2198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3888" uniqueCount="2199">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -5601,9 +5601,6 @@
     <t>2020.5.16</t>
   </si>
   <si>
-    <t>2020.5.17（self)</t>
-  </si>
-  <si>
     <t>2020.5.14(self)</t>
   </si>
   <si>
@@ -6628,6 +6625,12 @@
   </si>
   <si>
     <t>2020.5.28</t>
+  </si>
+  <si>
+    <t>2020.5.17(self)</t>
+  </si>
+  <si>
+    <t>2020.5.29(self)</t>
   </si>
 </sst>
 </file>
@@ -7239,7 +7242,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7284,7 +7287,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7503,7 +7506,9 @@
       <c r="C21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>2198</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
@@ -7576,7 +7581,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8708,7 +8713,7 @@
         <v>5</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8974,7 +8979,7 @@
         <v>5</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8988,7 +8993,7 @@
         <v>7</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9102,7 +9107,7 @@
         <v>7</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9155,7 +9160,7 @@
     </row>
     <row r="157" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="20" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="B157" s="14" t="s">
         <v>171</v>
@@ -9167,7 +9172,7 @@
     </row>
     <row r="158" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="20" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="B158" s="13" t="s">
         <v>172</v>
@@ -9179,7 +9184,7 @@
     </row>
     <row r="159" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="20" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B159" s="14" t="s">
         <v>173</v>
@@ -9191,7 +9196,7 @@
     </row>
     <row r="160" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A160" s="20" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B160" s="13" t="s">
         <v>174</v>
@@ -9212,12 +9217,12 @@
         <v>5</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="20" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="B162" s="13" t="s">
         <v>176</v>
@@ -9241,7 +9246,7 @@
     </row>
     <row r="164" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="20" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B164" s="13" t="s">
         <v>178</v>
@@ -9298,7 +9303,7 @@
         <v>5</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>1856</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9327,7 +9332,7 @@
     </row>
     <row r="171" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="20" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="B171" s="14" t="s">
         <v>185</v>
@@ -9519,7 +9524,7 @@
     </row>
     <row r="187" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="20" t="s">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="B187" s="14" t="s">
         <v>201</v>
@@ -9564,7 +9569,7 @@
         <v>5</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>1857</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="191" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9806,7 +9811,7 @@
         <v>7</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>1855</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10207,7 +10212,7 @@
     </row>
     <row r="244" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="20" t="s">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B244" s="13" t="s">
         <v>258</v>
@@ -10219,7 +10224,7 @@
     </row>
     <row r="245" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="20" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B245" s="14" t="s">
         <v>259</v>
@@ -10231,7 +10236,7 @@
     </row>
     <row r="246" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="20" t="s">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B246" s="13" t="s">
         <v>260</v>
@@ -10243,7 +10248,7 @@
     </row>
     <row r="247" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="20" t="s">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B247" s="14" t="s">
         <v>261</v>
@@ -10255,7 +10260,7 @@
     </row>
     <row r="248" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="20" t="s">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B248" s="13" t="s">
         <v>262</v>
@@ -10267,7 +10272,7 @@
     </row>
     <row r="249" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="20" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B249" s="14" t="s">
         <v>263</v>
@@ -10279,7 +10284,7 @@
     </row>
     <row r="250" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="20" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B250" s="13" t="s">
         <v>264</v>
@@ -10291,7 +10296,7 @@
     </row>
     <row r="251" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="20" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B251" s="14" t="s">
         <v>265</v>
@@ -10303,7 +10308,7 @@
     </row>
     <row r="252" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="20" t="s">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B252" s="13" t="s">
         <v>266</v>
@@ -10315,7 +10320,7 @@
     </row>
     <row r="253" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="20" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B253" s="14" t="s">
         <v>267</v>
@@ -10327,7 +10332,7 @@
     </row>
     <row r="254" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="20" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B254" s="13" t="s">
         <v>268</v>
@@ -10339,7 +10344,7 @@
     </row>
     <row r="255" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="20" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B255" s="14" t="s">
         <v>269</v>
@@ -10351,7 +10356,7 @@
     </row>
     <row r="256" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="20" t="s">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B256" s="13" t="s">
         <v>270</v>
@@ -10363,7 +10368,7 @@
     </row>
     <row r="257" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A257" s="20" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B257" s="14" t="s">
         <v>271</v>
@@ -10399,7 +10404,7 @@
     </row>
     <row r="260" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A260" s="20" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B260" s="13" t="s">
         <v>274</v>
@@ -10423,7 +10428,7 @@
     </row>
     <row r="262" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A262" s="20" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B262" s="13" t="s">
         <v>276</v>
@@ -10471,7 +10476,7 @@
     </row>
     <row r="266" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="20" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B266" s="13" t="s">
         <v>280</v>
@@ -10483,7 +10488,7 @@
     </row>
     <row r="267" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A267" s="20" t="s">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B267" s="14" t="s">
         <v>281</v>
@@ -10495,7 +10500,7 @@
     </row>
     <row r="268" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A268" s="20" t="s">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B268" s="13" t="s">
         <v>282</v>
@@ -10507,7 +10512,7 @@
     </row>
     <row r="269" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="18" t="s">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B269" s="14" t="s">
         <v>283</v>
@@ -10519,7 +10524,7 @@
     </row>
     <row r="270" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="20" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B270" s="13" t="s">
         <v>284</v>
@@ -10531,7 +10536,7 @@
     </row>
     <row r="271" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A271" s="20" t="s">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="B271" s="14" t="s">
         <v>285</v>
@@ -10543,7 +10548,7 @@
     </row>
     <row r="272" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A272" s="20" t="s">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B272" s="13" t="s">
         <v>286</v>
@@ -10555,7 +10560,7 @@
     </row>
     <row r="273" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="20" t="s">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B273" s="14" t="s">
         <v>287</v>
@@ -10603,7 +10608,7 @@
     </row>
     <row r="277" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="20" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B277" s="14" t="s">
         <v>291</v>
@@ -10615,7 +10620,7 @@
     </row>
     <row r="278" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A278" s="20" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B278" s="13" t="s">
         <v>292</v>
@@ -10651,7 +10656,7 @@
     </row>
     <row r="281" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A281" s="20" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B281" s="14" t="s">
         <v>295</v>
@@ -10663,7 +10668,7 @@
     </row>
     <row r="282" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A282" s="20" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B282" s="13" t="s">
         <v>296</v>
@@ -10696,7 +10701,7 @@
         <v>5</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10713,7 +10718,7 @@
     </row>
     <row r="286" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A286" s="20" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B286" s="13" t="s">
         <v>300</v>
@@ -10725,7 +10730,7 @@
     </row>
     <row r="287" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A287" s="20" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B287" s="14" t="s">
         <v>301</v>
@@ -10749,7 +10754,7 @@
     </row>
     <row r="289" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="20" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B289" s="14" t="s">
         <v>303</v>
@@ -10785,7 +10790,7 @@
     </row>
     <row r="292" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="20" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B292" s="13" t="s">
         <v>306</v>
@@ -10809,7 +10814,7 @@
     </row>
     <row r="294" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A294" s="20" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B294" s="13" t="s">
         <v>308</v>
@@ -10821,7 +10826,7 @@
     </row>
     <row r="295" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="20" t="s">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B295" s="14" t="s">
         <v>309</v>
@@ -10833,7 +10838,7 @@
     </row>
     <row r="296" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="18" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B296" s="13" t="s">
         <v>310</v>
@@ -10845,7 +10850,7 @@
     </row>
     <row r="297" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="20" t="s">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B297" s="14" t="s">
         <v>311</v>
@@ -10869,7 +10874,7 @@
     </row>
     <row r="299" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="20" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B299" s="14" t="s">
         <v>313</v>
@@ -10917,7 +10922,7 @@
     </row>
     <row r="303" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="20" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B303" s="14" t="s">
         <v>317</v>
@@ -10953,7 +10958,7 @@
     </row>
     <row r="306" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="20" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B306" s="13" t="s">
         <v>320</v>
@@ -10989,7 +10994,7 @@
     </row>
     <row r="309" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="20" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B309" s="14" t="s">
         <v>323</v>
@@ -11025,7 +11030,7 @@
     </row>
     <row r="312" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A312" s="20" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B312" s="13" t="s">
         <v>326</v>
@@ -11061,7 +11066,7 @@
     </row>
     <row r="315" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A315" s="20" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B315" s="14" t="s">
         <v>329</v>
@@ -11097,7 +11102,7 @@
     </row>
     <row r="318" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="20" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B318" s="13" t="s">
         <v>332</v>
@@ -11133,7 +11138,7 @@
     </row>
     <row r="321" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A321" s="20" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B321" s="14" t="s">
         <v>335</v>
@@ -11169,7 +11174,7 @@
     </row>
     <row r="324" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A324" s="20" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B324" s="13" t="s">
         <v>338</v>
@@ -11193,7 +11198,7 @@
     </row>
     <row r="326" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A326" s="20" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B326" s="13" t="s">
         <v>340</v>
@@ -11289,7 +11294,7 @@
     </row>
     <row r="334" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A334" s="20" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B334" s="13" t="s">
         <v>348</v>
@@ -11361,7 +11366,7 @@
     </row>
     <row r="340" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A340" s="20" t="s">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B340" s="13" t="s">
         <v>354</v>
@@ -11373,7 +11378,7 @@
     </row>
     <row r="341" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="20" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B341" s="14" t="s">
         <v>355</v>
@@ -11447,7 +11452,7 @@
     </row>
     <row r="347" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A347" s="20" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B347" s="14" t="s">
         <v>362</v>
@@ -11471,7 +11476,7 @@
     </row>
     <row r="349" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A349" s="20" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B349" s="14" t="s">
         <v>364</v>
@@ -11507,7 +11512,7 @@
     </row>
     <row r="352" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A352" s="20" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B352" s="13" t="s">
         <v>367</v>
@@ -11531,7 +11536,7 @@
     </row>
     <row r="354" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A354" s="20" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B354" s="13" t="s">
         <v>369</v>
@@ -11567,7 +11572,7 @@
     </row>
     <row r="357" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A357" s="20" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B357" s="14" t="s">
         <v>372</v>
@@ -11591,7 +11596,7 @@
     </row>
     <row r="359" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="20" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B359" s="14" t="s">
         <v>374</v>
@@ -11603,7 +11608,7 @@
     </row>
     <row r="360" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A360" s="20" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B360" s="13" t="s">
         <v>375</v>
@@ -11615,7 +11620,7 @@
     </row>
     <row r="361" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A361" s="20" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B361" s="14" t="s">
         <v>376</v>
@@ -11627,7 +11632,7 @@
     </row>
     <row r="362" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A362" s="20" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B362" s="13" t="s">
         <v>377</v>
@@ -11639,7 +11644,7 @@
     </row>
     <row r="363" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A363" s="20" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B363" s="14" t="s">
         <v>378</v>
@@ -11651,7 +11656,7 @@
     </row>
     <row r="364" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="19" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B364" s="13" t="s">
         <v>379</v>
@@ -11663,7 +11668,7 @@
     </row>
     <row r="365" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A365" s="20" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B365" s="14" t="s">
         <v>380</v>
@@ -11675,7 +11680,7 @@
     </row>
     <row r="366" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A366" s="19" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B366" s="13" t="s">
         <v>381</v>
@@ -11687,7 +11692,7 @@
     </row>
     <row r="367" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A367" s="20" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B367" s="14" t="s">
         <v>382</v>
@@ -11723,7 +11728,7 @@
     </row>
     <row r="370" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A370" s="20" t="s">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B370" s="13" t="s">
         <v>385</v>
@@ -11735,7 +11740,7 @@
     </row>
     <row r="371" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A371" s="20" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B371" s="14" t="s">
         <v>386</v>
@@ -11843,7 +11848,7 @@
     </row>
     <row r="380" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A380" s="20" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B380" s="13" t="s">
         <v>395</v>
@@ -12191,7 +12196,7 @@
     </row>
     <row r="409" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A409" s="20" t="s">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B409" s="14" t="s">
         <v>424</v>
@@ -12227,7 +12232,7 @@
     </row>
     <row r="412" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="20" t="s">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B412" s="13" t="s">
         <v>427</v>
@@ -12311,7 +12316,7 @@
     </row>
     <row r="419" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A419" s="20" t="s">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B419" s="14" t="s">
         <v>434</v>
@@ -12359,7 +12364,7 @@
     </row>
     <row r="423" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A423" s="20" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B423" s="14" t="s">
         <v>438</v>
@@ -12395,7 +12400,7 @@
     </row>
     <row r="426" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="20" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B426" s="13" t="s">
         <v>441</v>
@@ -12407,7 +12412,7 @@
     </row>
     <row r="427" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A427" s="20" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B427" s="14" t="s">
         <v>442</v>
@@ -12419,7 +12424,7 @@
     </row>
     <row r="428" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A428" s="18" t="s">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B428" s="13" t="s">
         <v>443</v>
@@ -12431,7 +12436,7 @@
     </row>
     <row r="429" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="20" t="s">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B429" s="14" t="s">
         <v>444</v>
@@ -12467,7 +12472,7 @@
     </row>
     <row r="432" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" s="20" t="s">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B432" s="13" t="s">
         <v>447</v>
@@ -12563,7 +12568,7 @@
     </row>
     <row r="440" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A440" s="20" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B440" s="13" t="s">
         <v>455</v>
@@ -12623,7 +12628,7 @@
     </row>
     <row r="445" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A445" s="20" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B445" s="14" t="s">
         <v>460</v>
@@ -12875,7 +12880,7 @@
     </row>
     <row r="466" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A466" s="20" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B466" s="13" t="s">
         <v>481</v>
@@ -12923,7 +12928,7 @@
     </row>
     <row r="470" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A470" s="20" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B470" s="13" t="s">
         <v>485</v>
@@ -12947,7 +12952,7 @@
     </row>
     <row r="472" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A472" s="20" t="s">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B472" s="13" t="s">
         <v>487</v>
@@ -13103,7 +13108,7 @@
     </row>
     <row r="485" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A485" s="20" t="s">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B485" s="14" t="s">
         <v>500</v>
@@ -13141,7 +13146,7 @@
     </row>
     <row r="488" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A488" s="20" t="s">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B488" s="13" t="s">
         <v>503</v>
@@ -13165,7 +13170,7 @@
     </row>
     <row r="490" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A490" s="20" t="s">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B490" s="13" t="s">
         <v>505</v>
@@ -13177,7 +13182,7 @@
     </row>
     <row r="491" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A491" s="20" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B491" s="14" t="s">
         <v>506</v>
@@ -13287,7 +13292,7 @@
     </row>
     <row r="500" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A500" s="20" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B500" s="13" t="s">
         <v>516</v>
@@ -13359,7 +13364,7 @@
     </row>
     <row r="506" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A506" s="20" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B506" s="13" t="s">
         <v>522</v>
@@ -13419,7 +13424,7 @@
     </row>
     <row r="511" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A511" s="20" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B511" s="14" t="s">
         <v>527</v>
@@ -13431,7 +13436,7 @@
     </row>
     <row r="512" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A512" s="20" t="s">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B512" s="13" t="s">
         <v>528</v>
@@ -13443,7 +13448,7 @@
     </row>
     <row r="513" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A513" s="20" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B513" s="14" t="s">
         <v>529</v>
@@ -13623,7 +13628,7 @@
     </row>
     <row r="528" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A528" s="20" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B528" s="13" t="s">
         <v>544</v>
@@ -13671,7 +13676,7 @@
     </row>
     <row r="532" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A532" s="20" t="s">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B532" s="13" t="s">
         <v>548</v>
@@ -13695,7 +13700,7 @@
     </row>
     <row r="534" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A534" s="20" t="s">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B534" s="13" t="s">
         <v>550</v>
@@ -13707,7 +13712,7 @@
     </row>
     <row r="535" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A535" s="20" t="s">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="B535" s="14" t="s">
         <v>551</v>
@@ -13731,7 +13736,7 @@
     </row>
     <row r="537" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A537" s="20" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="B537" s="14" t="s">
         <v>553</v>
@@ -13827,7 +13832,7 @@
     </row>
     <row r="545" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A545" s="20" t="s">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B545" s="14" t="s">
         <v>561</v>
@@ -13839,7 +13844,7 @@
     </row>
     <row r="546" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A546" s="20" t="s">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="B546" s="13" t="s">
         <v>562</v>
@@ -13875,7 +13880,7 @@
     </row>
     <row r="549" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A549" s="20" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="B549" s="14" t="s">
         <v>565</v>
@@ -13887,7 +13892,7 @@
     </row>
     <row r="550" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A550" s="20" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B550" s="13" t="s">
         <v>566</v>
@@ -13899,7 +13904,7 @@
     </row>
     <row r="551" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A551" s="20" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B551" s="14" t="s">
         <v>567</v>
@@ -13959,7 +13964,7 @@
     </row>
     <row r="556" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A556" s="20" t="s">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B556" s="13" t="s">
         <v>572</v>
@@ -13992,7 +13997,7 @@
         <v>5</v>
       </c>
       <c r="D558" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="559" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14047,7 +14052,7 @@
     </row>
     <row r="563" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A563" s="20" t="s">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B563" s="14" t="s">
         <v>580</v>
@@ -14119,7 +14124,7 @@
     </row>
     <row r="569" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A569" s="20" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="B569" s="14" t="s">
         <v>586</v>
@@ -14131,7 +14136,7 @@
     </row>
     <row r="570" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A570" s="20" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="B570" s="13" t="s">
         <v>587</v>
@@ -14143,7 +14148,7 @@
     </row>
     <row r="571" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A571" s="20" t="s">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="B571" s="14" t="s">
         <v>588</v>
@@ -14155,7 +14160,7 @@
     </row>
     <row r="572" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A572" s="20" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B572" s="13" t="s">
         <v>589</v>
@@ -14167,7 +14172,7 @@
     </row>
     <row r="573" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A573" s="19" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B573" s="14" t="s">
         <v>590</v>
@@ -14179,7 +14184,7 @@
     </row>
     <row r="574" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A574" s="20" t="s">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B574" s="13" t="s">
         <v>591</v>
@@ -14191,7 +14196,7 @@
     </row>
     <row r="575" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A575" s="20" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B575" s="14" t="s">
         <v>592</v>
@@ -14203,7 +14208,7 @@
     </row>
     <row r="576" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A576" s="18" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B576" s="13" t="s">
         <v>593</v>
@@ -14227,7 +14232,7 @@
     </row>
     <row r="578" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A578" s="20" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B578" s="13" t="s">
         <v>595</v>
@@ -14239,7 +14244,7 @@
     </row>
     <row r="579" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A579" s="20" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B579" s="14" t="s">
         <v>596</v>
@@ -14251,7 +14256,7 @@
     </row>
     <row r="580" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A580" s="20" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B580" s="13" t="s">
         <v>597</v>
@@ -14263,7 +14268,7 @@
     </row>
     <row r="581" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A581" s="20" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B581" s="14" t="s">
         <v>598</v>
@@ -14275,7 +14280,7 @@
     </row>
     <row r="582" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A582" s="18" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B582" s="13" t="s">
         <v>599</v>
@@ -14287,7 +14292,7 @@
     </row>
     <row r="583" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A583" s="20" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B583" s="14" t="s">
         <v>600</v>
@@ -14299,7 +14304,7 @@
     </row>
     <row r="584" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A584" s="18" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B584" s="13" t="s">
         <v>601</v>
@@ -14311,7 +14316,7 @@
     </row>
     <row r="585" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A585" s="20" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B585" s="14" t="s">
         <v>602</v>
@@ -14323,7 +14328,7 @@
     </row>
     <row r="586" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A586" s="20" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B586" s="13" t="s">
         <v>603</v>
@@ -14335,7 +14340,7 @@
     </row>
     <row r="587" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A587" s="20" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B587" s="14" t="s">
         <v>604</v>
@@ -14347,7 +14352,7 @@
     </row>
     <row r="588" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A588" s="18" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B588" s="13" t="s">
         <v>605</v>
@@ -14359,7 +14364,7 @@
     </row>
     <row r="589" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A589" s="20" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B589" s="14" t="s">
         <v>606</v>
@@ -14467,7 +14472,7 @@
     </row>
     <row r="598" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A598" s="20" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B598" s="13" t="s">
         <v>615</v>
@@ -14527,7 +14532,7 @@
     </row>
     <row r="603" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A603" s="20" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B603" s="14" t="s">
         <v>620</v>
@@ -14539,7 +14544,7 @@
     </row>
     <row r="604" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A604" s="20" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B604" s="13" t="s">
         <v>621</v>
@@ -14551,7 +14556,7 @@
     </row>
     <row r="605" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A605" s="20" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B605" s="14" t="s">
         <v>622</v>
@@ -14587,7 +14592,7 @@
     </row>
     <row r="608" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A608" s="20" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B608" s="13" t="s">
         <v>625</v>
@@ -14599,7 +14604,7 @@
     </row>
     <row r="609" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A609" s="20" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B609" s="14" t="s">
         <v>626</v>
@@ -14623,7 +14628,7 @@
     </row>
     <row r="611" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A611" s="20" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B611" s="14" t="s">
         <v>628</v>
@@ -14635,7 +14640,7 @@
     </row>
     <row r="612" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A612" s="19" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B612" s="13" t="s">
         <v>629</v>
@@ -14647,7 +14652,7 @@
     </row>
     <row r="613" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A613" s="20" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B613" s="14" t="s">
         <v>630</v>
@@ -14659,7 +14664,7 @@
     </row>
     <row r="614" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A614" s="20" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B614" s="13" t="s">
         <v>631</v>
@@ -14671,7 +14676,7 @@
     </row>
     <row r="615" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A615" s="20" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B615" s="14" t="s">
         <v>632</v>
@@ -14683,7 +14688,7 @@
     </row>
     <row r="616" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A616" s="20" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B616" s="13" t="s">
         <v>633</v>
@@ -14695,7 +14700,7 @@
     </row>
     <row r="617" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A617" s="20" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B617" s="14" t="s">
         <v>634</v>
@@ -14707,7 +14712,7 @@
     </row>
     <row r="618" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A618" s="19" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B618" s="13" t="s">
         <v>635</v>
@@ -14719,7 +14724,7 @@
     </row>
     <row r="619" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A619" s="20" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B619" s="14" t="s">
         <v>636</v>
@@ -14731,7 +14736,7 @@
     </row>
     <row r="620" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A620" s="20" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B620" s="13" t="s">
         <v>637</v>
@@ -14791,7 +14796,7 @@
     </row>
     <row r="625" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A625" s="20" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B625" s="14" t="s">
         <v>642</v>
@@ -14803,7 +14808,7 @@
     </row>
     <row r="626" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A626" s="20" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B626" s="13" t="s">
         <v>643</v>
@@ -14875,7 +14880,7 @@
     </row>
     <row r="632" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A632" s="20" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B632" s="13" t="s">
         <v>649</v>
@@ -14911,7 +14916,7 @@
     </row>
     <row r="635" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A635" s="20" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B635" s="14" t="s">
         <v>652</v>
@@ -14923,7 +14928,7 @@
     </row>
     <row r="636" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A636" s="20" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B636" s="13" t="s">
         <v>653</v>
@@ -15007,7 +15012,7 @@
     </row>
     <row r="643" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A643" s="20" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B643" s="14" t="s">
         <v>660</v>
@@ -15019,7 +15024,7 @@
     </row>
     <row r="644" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A644" s="19" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B644" s="13" t="s">
         <v>661</v>
@@ -15031,7 +15036,7 @@
     </row>
     <row r="645" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A645" s="20" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B645" s="14" t="s">
         <v>662</v>
@@ -15115,7 +15120,7 @@
     </row>
     <row r="652" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A652" s="20" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B652" s="13" t="s">
         <v>669</v>
@@ -15175,7 +15180,7 @@
     </row>
     <row r="657" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A657" s="20" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B657" s="14" t="s">
         <v>674</v>
@@ -15223,7 +15228,7 @@
     </row>
     <row r="661" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A661" s="20" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B661" s="14" t="s">
         <v>678</v>
@@ -15259,7 +15264,7 @@
     </row>
     <row r="664" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A664" s="20" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B664" s="13" t="s">
         <v>681</v>
@@ -15295,7 +15300,7 @@
     </row>
     <row r="667" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A667" s="20" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B667" s="14" t="s">
         <v>684</v>
@@ -15475,7 +15480,7 @@
     </row>
     <row r="682" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A682" s="20" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B682" s="13" t="s">
         <v>699</v>
@@ -15487,7 +15492,7 @@
     </row>
     <row r="683" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A683" s="18" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B683" s="14" t="s">
         <v>700</v>
@@ -15499,7 +15504,7 @@
     </row>
     <row r="684" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A684" s="20" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B684" s="13" t="s">
         <v>701</v>
@@ -15631,7 +15636,7 @@
     </row>
     <row r="695" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A695" s="20" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B695" s="14" t="s">
         <v>712</v>
@@ -15727,7 +15732,7 @@
     </row>
     <row r="703" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A703" s="20" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B703" s="14" t="s">
         <v>720</v>
@@ -15796,12 +15801,12 @@
         <v>7</v>
       </c>
       <c r="D708" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="709" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A709" s="20" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B709" s="14" t="s">
         <v>726</v>
@@ -15837,7 +15842,7 @@
     </row>
     <row r="712" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A712" s="20" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B712" s="13" t="s">
         <v>729</v>
@@ -15897,7 +15902,7 @@
     </row>
     <row r="717" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A717" s="20" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B717" s="14" t="s">
         <v>734</v>
@@ -15981,7 +15986,7 @@
     </row>
     <row r="724" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A724" s="20" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B724" s="13" t="s">
         <v>741</v>
@@ -16031,7 +16036,7 @@
     </row>
     <row r="728" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A728" s="20" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="B728" s="13" t="s">
         <v>744</v>
@@ -16115,7 +16120,7 @@
     </row>
     <row r="735" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A735" s="20" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="B735" s="14" t="s">
         <v>751</v>
@@ -16151,7 +16156,7 @@
     </row>
     <row r="738" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A738" s="20" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="B738" s="13" t="s">
         <v>754</v>
@@ -16211,7 +16216,7 @@
     </row>
     <row r="743" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A743" s="20" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B743" s="14" t="s">
         <v>759</v>
@@ -16309,7 +16314,7 @@
     </row>
     <row r="751" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A751" s="20" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="B751" s="14" t="s">
         <v>767</v>
@@ -16321,7 +16326,7 @@
     </row>
     <row r="752" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A752" s="20" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="B752" s="13" t="s">
         <v>768</v>
@@ -16369,7 +16374,7 @@
     </row>
     <row r="756" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A756" s="20" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="B756" s="13" t="s">
         <v>772</v>
@@ -16405,7 +16410,7 @@
     </row>
     <row r="759" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A759" s="20" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="B759" s="14" t="s">
         <v>775</v>
@@ -16417,7 +16422,7 @@
     </row>
     <row r="760" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A760" s="20" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="B760" s="13" t="s">
         <v>776</v>
@@ -16429,7 +16434,7 @@
     </row>
     <row r="761" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A761" s="20" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B761" s="14" t="s">
         <v>777</v>
@@ -16573,7 +16578,7 @@
     </row>
     <row r="773" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A773" s="20" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B773" s="14" t="s">
         <v>789</v>
@@ -16597,7 +16602,7 @@
     </row>
     <row r="775" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A775" s="20" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B775" s="14" t="s">
         <v>791</v>
@@ -16621,7 +16626,7 @@
     </row>
     <row r="777" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A777" s="20" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B777" s="14" t="s">
         <v>793</v>
@@ -16909,7 +16914,7 @@
     </row>
     <row r="801" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A801" s="20" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B801" s="14" t="s">
         <v>817</v>
@@ -19849,7 +19854,7 @@
     </row>
     <row r="1046" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1046" s="20" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B1046" s="13" t="s">
         <v>1062</v>
@@ -19909,7 +19914,7 @@
     </row>
     <row r="1051" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1051" s="20" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B1051" s="14" t="s">
         <v>1067</v>
@@ -19969,7 +19974,7 @@
     </row>
     <row r="1056" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1056" s="20" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B1056" s="13" t="s">
         <v>1072</v>
@@ -19981,7 +19986,7 @@
     </row>
     <row r="1057" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1057" s="20" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B1057" s="14" t="s">
         <v>1073</v>
@@ -19993,7 +19998,7 @@
     </row>
     <row r="1058" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1058" s="20" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B1058" s="13" t="s">
         <v>1074</v>
@@ -20005,7 +20010,7 @@
     </row>
     <row r="1059" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1059" s="20" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B1059" s="14" t="s">
         <v>1075</v>
@@ -20017,7 +20022,7 @@
     </row>
     <row r="1060" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1060" s="20" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B1060" s="13" t="s">
         <v>1076</v>
@@ -20029,7 +20034,7 @@
     </row>
     <row r="1061" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1061" s="20" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B1061" s="14" t="s">
         <v>1077</v>
@@ -20041,7 +20046,7 @@
     </row>
     <row r="1062" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1062" s="20" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B1062" s="13" t="s">
         <v>1078</v>
@@ -20053,7 +20058,7 @@
     </row>
     <row r="1063" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1063" s="20" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
       <c r="B1063" s="14" t="s">
         <v>1061</v>
@@ -20065,7 +20070,7 @@
     </row>
     <row r="1064" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1064" s="20" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="B1064" s="13" t="s">
         <v>1079</v>
@@ -20077,7 +20082,7 @@
     </row>
     <row r="1065" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1065" s="20" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="B1065" s="14" t="s">
         <v>1080</v>
@@ -20089,7 +20094,7 @@
     </row>
     <row r="1066" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1066" s="20" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
       <c r="B1066" s="13" t="s">
         <v>1081</v>
@@ -20101,7 +20106,7 @@
     </row>
     <row r="1067" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1067" s="20" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="B1067" s="14" t="s">
         <v>1082</v>
@@ -20113,7 +20118,7 @@
     </row>
     <row r="1068" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1068" s="20" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="B1068" s="13" t="s">
         <v>1083</v>
@@ -20125,7 +20130,7 @@
     </row>
     <row r="1069" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1069" s="20" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="B1069" s="14" t="s">
         <v>1084</v>
@@ -20137,7 +20142,7 @@
     </row>
     <row r="1070" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1070" s="20" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="B1070" s="13" t="s">
         <v>1085</v>
@@ -20149,7 +20154,7 @@
     </row>
     <row r="1071" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1071" s="20" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="B1071" s="14" t="s">
         <v>1086</v>
@@ -20209,7 +20214,7 @@
     </row>
     <row r="1076" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1076" s="20" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="B1076" s="13" t="s">
         <v>1091</v>
@@ -20221,7 +20226,7 @@
     </row>
     <row r="1077" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1077" s="20" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="B1077" s="14" t="s">
         <v>1092</v>
@@ -20233,7 +20238,7 @@
     </row>
     <row r="1078" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1078" s="20" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="B1078" s="13" t="s">
         <v>1093</v>
@@ -20293,7 +20298,7 @@
     </row>
     <row r="1083" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1083" s="20" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="B1083" s="14" t="s">
         <v>1098</v>
@@ -20305,7 +20310,7 @@
     </row>
     <row r="1084" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1084" s="20" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="B1084" s="13" t="s">
         <v>1099</v>
@@ -20317,7 +20322,7 @@
     </row>
     <row r="1085" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1085" s="20" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="B1085" s="14" t="s">
         <v>1100</v>
@@ -20329,7 +20334,7 @@
     </row>
     <row r="1086" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1086" s="20" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="B1086" s="13" t="s">
         <v>1101</v>
@@ -20341,7 +20346,7 @@
     </row>
     <row r="1087" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1087" s="20" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="B1087" s="14" t="s">
         <v>1102</v>
@@ -20353,7 +20358,7 @@
     </row>
     <row r="1088" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1088" s="20" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="B1088" s="13" t="s">
         <v>1103</v>
@@ -20365,7 +20370,7 @@
     </row>
     <row r="1089" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1089" s="20" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="B1089" s="14" t="s">
         <v>1104</v>
@@ -20473,7 +20478,7 @@
     </row>
     <row r="1098" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1098" s="20" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="B1098" s="13" t="s">
         <v>1113</v>
@@ -20485,7 +20490,7 @@
     </row>
     <row r="1099" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1099" s="20" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="B1099" s="14" t="s">
         <v>1114</v>
@@ -20497,7 +20502,7 @@
     </row>
     <row r="1100" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1100" s="20" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="B1100" s="13" t="s">
         <v>1115</v>
@@ -20509,7 +20514,7 @@
     </row>
     <row r="1101" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1101" s="20" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="B1101" s="14" t="s">
         <v>1116</v>
@@ -20521,7 +20526,7 @@
     </row>
     <row r="1102" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1102" s="20" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="B1102" s="13" t="s">
         <v>1117</v>
@@ -20533,7 +20538,7 @@
     </row>
     <row r="1103" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1103" s="20" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="B1103" s="14" t="s">
         <v>1118</v>
@@ -20593,7 +20598,7 @@
     </row>
     <row r="1108" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1108" s="20" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="B1108" s="13" t="s">
         <v>1123</v>
@@ -20653,7 +20658,7 @@
     </row>
     <row r="1113" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1113" s="20" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="B1113" s="14" t="s">
         <v>1128</v>
@@ -20665,7 +20670,7 @@
     </row>
     <row r="1114" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1114" s="20" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="B1114" s="13" t="s">
         <v>1129</v>
@@ -20725,7 +20730,7 @@
     </row>
     <row r="1119" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1119" s="20" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="B1119" s="14" t="s">
         <v>1134</v>
@@ -20737,7 +20742,7 @@
     </row>
     <row r="1120" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1120" s="20" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="B1120" s="13" t="s">
         <v>1135</v>
@@ -20749,7 +20754,7 @@
     </row>
     <row r="1121" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1121" s="20" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="B1121" s="14" t="s">
         <v>1136</v>
@@ -20761,7 +20766,7 @@
     </row>
     <row r="1122" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1122" s="20" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="B1122" s="13" t="s">
         <v>1137</v>
@@ -20821,7 +20826,7 @@
     </row>
     <row r="1127" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1127" s="20" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="B1127" s="14" t="s">
         <v>1142</v>
@@ -20833,7 +20838,7 @@
     </row>
     <row r="1128" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1128" s="20" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="B1128" s="13" t="s">
         <v>1143</v>
@@ -20893,7 +20898,7 @@
     </row>
     <row r="1133" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1133" s="20" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
       <c r="B1133" s="14" t="s">
         <v>1148</v>
@@ -20905,7 +20910,7 @@
     </row>
     <row r="1134" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1134" s="20" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
       <c r="B1134" s="13" t="s">
         <v>1149</v>
@@ -20917,7 +20922,7 @@
     </row>
     <row r="1135" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1135" s="20" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
       <c r="B1135" s="14" t="s">
         <v>1150</v>
@@ -20929,7 +20934,7 @@
     </row>
     <row r="1136" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1136" s="20" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
       <c r="B1136" s="13" t="s">
         <v>1151</v>
@@ -20941,7 +20946,7 @@
     </row>
     <row r="1137" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1137" s="20" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
       <c r="B1137" s="14" t="s">
         <v>1152</v>
@@ -21001,7 +21006,7 @@
     </row>
     <row r="1142" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1142" s="20" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="B1142" s="13" t="s">
         <v>1157</v>
@@ -21013,7 +21018,7 @@
     </row>
     <row r="1143" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1143" s="20" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
       <c r="B1143" s="14" t="s">
         <v>1158</v>
@@ -21085,7 +21090,7 @@
     </row>
     <row r="1149" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1149" s="20" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
       <c r="B1149" s="14" t="s">
         <v>1164</v>
@@ -21097,7 +21102,7 @@
     </row>
     <row r="1150" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1150" s="20" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
       <c r="B1150" s="13" t="s">
         <v>1165</v>
@@ -21109,7 +21114,7 @@
     </row>
     <row r="1151" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1151" s="20" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
       <c r="B1151" s="14" t="s">
         <v>1166</v>
@@ -21121,7 +21126,7 @@
     </row>
     <row r="1152" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1152" s="20" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
       <c r="B1152" s="13" t="s">
         <v>1167</v>
@@ -21133,7 +21138,7 @@
     </row>
     <row r="1153" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1153" s="20" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
       <c r="B1153" s="14" t="s">
         <v>1168</v>
@@ -21145,7 +21150,7 @@
     </row>
     <row r="1154" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1154" s="20" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="B1154" s="13" t="s">
         <v>1169</v>
@@ -21205,7 +21210,7 @@
     </row>
     <row r="1159" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1159" s="20" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
       <c r="B1159" s="14" t="s">
         <v>1174</v>
@@ -21217,7 +21222,7 @@
     </row>
     <row r="1160" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1160" s="20" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
       <c r="B1160" s="13" t="s">
         <v>1175</v>
@@ -21277,7 +21282,7 @@
     </row>
     <row r="1165" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1165" s="20" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="B1165" s="14" t="s">
         <v>1180</v>
@@ -21289,7 +21294,7 @@
     </row>
     <row r="1166" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1166" s="20" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="B1166" s="13" t="s">
         <v>1181</v>
@@ -21301,7 +21306,7 @@
     </row>
     <row r="1167" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1167" s="20" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="B1167" s="14" t="s">
         <v>1182</v>
@@ -21313,7 +21318,7 @@
     </row>
     <row r="1168" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1168" s="20" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="B1168" s="13" t="s">
         <v>1183</v>
@@ -21325,7 +21330,7 @@
     </row>
     <row r="1169" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1169" s="20" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="B1169" s="14" t="s">
         <v>1184</v>
@@ -21385,7 +21390,7 @@
     </row>
     <row r="1174" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1174" s="20" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="B1174" s="13" t="s">
         <v>1189</v>
@@ -21397,7 +21402,7 @@
     </row>
     <row r="1175" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1175" s="20" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="B1175" s="14" t="s">
         <v>1190</v>
@@ -21409,7 +21414,7 @@
     </row>
     <row r="1176" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1176" s="18" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="B1176" s="13" t="s">
         <v>1191</v>
@@ -21421,7 +21426,7 @@
     </row>
     <row r="1177" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1177" s="20" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="B1177" s="14" t="s">
         <v>1192</v>
@@ -21469,7 +21474,7 @@
     </row>
     <row r="1181" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1181" s="20" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="B1181" s="14" t="s">
         <v>1196</v>
@@ -21481,7 +21486,7 @@
     </row>
     <row r="1182" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1182" s="20" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="B1182" s="13" t="s">
         <v>1197</v>
@@ -21493,7 +21498,7 @@
     </row>
     <row r="1183" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1183" s="20" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="B1183" s="14" t="s">
         <v>1198</v>
@@ -21505,7 +21510,7 @@
     </row>
     <row r="1184" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1184" s="20" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="B1184" s="13" t="s">
         <v>1199</v>
@@ -21565,7 +21570,7 @@
     </row>
     <row r="1189" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1189" s="20" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="B1189" s="14" t="s">
         <v>1204</v>
@@ -21625,7 +21630,7 @@
     </row>
     <row r="1194" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1194" s="20" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="B1194" s="13" t="s">
         <v>1209</v>
@@ -21637,7 +21642,7 @@
     </row>
     <row r="1195" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1195" s="20" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="B1195" s="14" t="s">
         <v>1210</v>
@@ -21649,7 +21654,7 @@
     </row>
     <row r="1196" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1196" s="18" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="B1196" s="13" t="s">
         <v>1211</v>
@@ -21661,7 +21666,7 @@
     </row>
     <row r="1197" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1197" s="20" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="B1197" s="14" t="s">
         <v>1212</v>
@@ -21673,7 +21678,7 @@
     </row>
     <row r="1198" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1198" s="20" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="B1198" s="13" t="s">
         <v>1213</v>
@@ -21685,7 +21690,7 @@
     </row>
     <row r="1199" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1199" s="20" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="B1199" s="14" t="s">
         <v>1214</v>
@@ -21697,7 +21702,7 @@
     </row>
     <row r="1200" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1200" s="20" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="B1200" s="13" t="s">
         <v>1215</v>
@@ -21757,7 +21762,7 @@
     </row>
     <row r="1205" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1205" s="20" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
       <c r="B1205" s="14" t="s">
         <v>1220</v>
@@ -21769,7 +21774,7 @@
     </row>
     <row r="1206" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1206" s="20" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
       <c r="B1206" s="13" t="s">
         <v>1221</v>
@@ -21841,7 +21846,7 @@
     </row>
     <row r="1212" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1212" s="20" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
       <c r="B1212" s="13" t="s">
         <v>1227</v>
@@ -21853,7 +21858,7 @@
     </row>
     <row r="1213" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1213" s="20" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
       <c r="B1213" s="14" t="s">
         <v>1228</v>
@@ -21865,7 +21870,7 @@
     </row>
     <row r="1214" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1214" s="20" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="B1214" s="13" t="s">
         <v>1229</v>
@@ -21877,7 +21882,7 @@
     </row>
     <row r="1215" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1215" s="20" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
       <c r="B1215" s="14" t="s">
         <v>1230</v>
@@ -21889,7 +21894,7 @@
     </row>
     <row r="1216" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1216" s="20" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
       <c r="B1216" s="13" t="s">
         <v>1231</v>
@@ -21901,7 +21906,7 @@
     </row>
     <row r="1217" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1217" s="20" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
       <c r="B1217" s="14" t="s">
         <v>1232</v>
@@ -22009,7 +22014,7 @@
     </row>
     <row r="1226" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1226" s="20" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
       <c r="B1226" s="13" t="s">
         <v>1241</v>
@@ -22045,7 +22050,7 @@
     </row>
     <row r="1229" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1229" s="20" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="B1229" s="14" t="s">
         <v>1244</v>
@@ -22057,7 +22062,7 @@
     </row>
     <row r="1230" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1230" s="20" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
       <c r="B1230" s="13" t="s">
         <v>1245</v>
@@ -22069,7 +22074,7 @@
     </row>
     <row r="1231" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1231" s="20" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="B1231" s="14" t="s">
         <v>1246</v>
@@ -22081,7 +22086,7 @@
     </row>
     <row r="1232" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1232" s="20" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="B1232" s="13" t="s">
         <v>1247</v>
@@ -22141,7 +22146,7 @@
     </row>
     <row r="1237" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1237" s="20" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="B1237" s="14" t="s">
         <v>1252</v>
@@ -22201,7 +22206,7 @@
     </row>
     <row r="1242" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1242" s="20" t="s">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="B1242" s="13" t="s">
         <v>1257</v>
@@ -22213,7 +22218,7 @@
     </row>
     <row r="1243" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1243" s="20" t="s">
-        <v>2135</v>
+        <v>2134</v>
       </c>
       <c r="B1243" s="14" t="s">
         <v>1258</v>
@@ -22225,7 +22230,7 @@
     </row>
     <row r="1244" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1244" s="20" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="B1244" s="13" t="s">
         <v>1259</v>
@@ -22237,7 +22242,7 @@
     </row>
     <row r="1245" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1245" s="20" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="B1245" s="14" t="s">
         <v>1260</v>
@@ -22249,7 +22254,7 @@
     </row>
     <row r="1246" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1246" s="20" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="B1246" s="13" t="s">
         <v>1261</v>
@@ -22261,7 +22266,7 @@
     </row>
     <row r="1247" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1247" s="20" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="B1247" s="14" t="s">
         <v>1262</v>
@@ -22321,7 +22326,7 @@
     </row>
     <row r="1252" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1252" s="20" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="B1252" s="13" t="s">
         <v>1267</v>
@@ -22381,7 +22386,7 @@
     </row>
     <row r="1257" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1257" s="20" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
       <c r="B1257" s="14" t="s">
         <v>1272</v>
@@ -22393,7 +22398,7 @@
     </row>
     <row r="1258" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1258" s="20" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="B1258" s="13" t="s">
         <v>1273</v>
@@ -22405,7 +22410,7 @@
     </row>
     <row r="1259" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1259" s="20" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
       <c r="B1259" s="14" t="s">
         <v>1274</v>
@@ -22417,7 +22422,7 @@
     </row>
     <row r="1260" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1260" s="20" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="B1260" s="13" t="s">
         <v>1275</v>
@@ -22477,7 +22482,7 @@
     </row>
     <row r="1265" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1265" s="20" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="B1265" s="14" t="s">
         <v>1280</v>
@@ -22489,7 +22494,7 @@
     </row>
     <row r="1266" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1266" s="20" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B1266" s="13" t="s">
         <v>1281</v>
@@ -22549,7 +22554,7 @@
     </row>
     <row r="1271" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1271" s="20" t="s">
-        <v>2147</v>
+        <v>2146</v>
       </c>
       <c r="B1271" s="14" t="s">
         <v>1286</v>
@@ -22561,7 +22566,7 @@
     </row>
     <row r="1272" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1272" s="20" t="s">
-        <v>2148</v>
+        <v>2147</v>
       </c>
       <c r="B1272" s="13" t="s">
         <v>1287</v>
@@ -22573,7 +22578,7 @@
     </row>
     <row r="1273" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1273" s="20" t="s">
-        <v>2149</v>
+        <v>2148</v>
       </c>
       <c r="B1273" s="14" t="s">
         <v>1288</v>
@@ -22585,7 +22590,7 @@
     </row>
     <row r="1274" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1274" s="20" t="s">
-        <v>2150</v>
+        <v>2149</v>
       </c>
       <c r="B1274" s="13" t="s">
         <v>1289</v>
@@ -22597,7 +22602,7 @@
     </row>
     <row r="1275" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1275" s="20" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
       <c r="B1275" s="14" t="s">
         <v>1290</v>
@@ -22657,7 +22662,7 @@
     </row>
     <row r="1280" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1280" s="20" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="B1280" s="13" t="s">
         <v>1295</v>
@@ -22669,7 +22674,7 @@
     </row>
     <row r="1281" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1281" s="20" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="B1281" s="14" t="s">
         <v>1296</v>
@@ -22729,7 +22734,7 @@
     </row>
     <row r="1286" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1286" s="20" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="B1286" s="13" t="s">
         <v>1301</v>
@@ -22837,7 +22842,7 @@
     </row>
     <row r="1295" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1295" s="20" t="s">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="B1295" s="14" t="s">
         <v>1310</v>
@@ -22945,7 +22950,7 @@
     </row>
     <row r="1304" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1304" s="20" t="s">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="B1304" s="13" t="s">
         <v>1319</v>
@@ -23005,7 +23010,7 @@
     </row>
     <row r="1309" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1309" s="20" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="B1309" s="14" t="s">
         <v>1324</v>
@@ -23161,7 +23166,7 @@
     </row>
     <row r="1322" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1322" s="20" t="s">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="B1322" s="13" t="s">
         <v>1337</v>
@@ -23173,7 +23178,7 @@
     </row>
     <row r="1323" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1323" s="20" t="s">
-        <v>2159</v>
+        <v>2158</v>
       </c>
       <c r="B1323" s="14" t="s">
         <v>1338</v>
@@ -23233,7 +23238,7 @@
     </row>
     <row r="1328" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1328" s="20" t="s">
-        <v>2160</v>
+        <v>2159</v>
       </c>
       <c r="B1328" s="13" t="s">
         <v>1343</v>
@@ -23341,7 +23346,7 @@
     </row>
     <row r="1337" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1337" s="20" t="s">
-        <v>2161</v>
+        <v>2160</v>
       </c>
       <c r="B1337" s="14" t="s">
         <v>1352</v>
@@ -23401,7 +23406,7 @@
     </row>
     <row r="1342" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1342" s="20" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
       <c r="B1342" s="13" t="s">
         <v>1357</v>
@@ -23509,7 +23514,7 @@
     </row>
     <row r="1351" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1351" s="20" t="s">
-        <v>2163</v>
+        <v>2162</v>
       </c>
       <c r="B1351" s="14" t="s">
         <v>1366</v>
@@ -23569,7 +23574,7 @@
     </row>
     <row r="1356" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1356" s="20" t="s">
-        <v>2164</v>
+        <v>2163</v>
       </c>
       <c r="B1356" s="13" t="s">
         <v>1371</v>
@@ -23677,7 +23682,7 @@
     </row>
     <row r="1365" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1365" s="20" t="s">
-        <v>2165</v>
+        <v>2164</v>
       </c>
       <c r="B1365" s="14" t="s">
         <v>1380</v>
@@ -23737,7 +23742,7 @@
     </row>
     <row r="1370" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1370" s="20" t="s">
-        <v>2166</v>
+        <v>2165</v>
       </c>
       <c r="B1370" s="13" t="s">
         <v>1385</v>
@@ -23845,7 +23850,7 @@
     </row>
     <row r="1379" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1379" s="20" t="s">
-        <v>2167</v>
+        <v>2166</v>
       </c>
       <c r="B1379" s="14" t="s">
         <v>1394</v>
@@ -23917,7 +23922,7 @@
     </row>
     <row r="1385" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1385" s="20" t="s">
-        <v>2168</v>
+        <v>2167</v>
       </c>
       <c r="B1385" s="14" t="s">
         <v>1400</v>
@@ -24025,7 +24030,7 @@
     </row>
     <row r="1394" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1394" s="20" t="s">
-        <v>2169</v>
+        <v>2168</v>
       </c>
       <c r="B1394" s="13" t="s">
         <v>1409</v>
@@ -24085,7 +24090,7 @@
     </row>
     <row r="1399" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1399" s="20" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B1399" s="14" t="s">
         <v>1414</v>
@@ -24193,7 +24198,7 @@
     </row>
     <row r="1408" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1408" s="20" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="B1408" s="13" t="s">
         <v>1423</v>
@@ -24253,7 +24258,7 @@
     </row>
     <row r="1413" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1413" s="20" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="B1413" s="14" t="s">
         <v>1428</v>
@@ -24361,7 +24366,7 @@
     </row>
     <row r="1422" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1422" s="20" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="B1422" s="13" t="s">
         <v>1437</v>
@@ -24421,7 +24426,7 @@
     </row>
     <row r="1427" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1427" s="20" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
       <c r="B1427" s="14" t="s">
         <v>1442</v>
@@ -24433,7 +24438,7 @@
     </row>
     <row r="1428" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1428" s="20" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
       <c r="B1428" s="13" t="s">
         <v>1443</v>
@@ -24445,7 +24450,7 @@
     </row>
     <row r="1429" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1429" s="20" t="s">
-        <v>2176</v>
+        <v>2175</v>
       </c>
       <c r="B1429" s="14" t="s">
         <v>1444</v>
@@ -24457,7 +24462,7 @@
     </row>
     <row r="1430" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1430" s="20" t="s">
-        <v>2177</v>
+        <v>2176</v>
       </c>
       <c r="B1430" s="13" t="s">
         <v>1445</v>
@@ -24469,7 +24474,7 @@
     </row>
     <row r="1431" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1431" s="20" t="s">
-        <v>2178</v>
+        <v>2177</v>
       </c>
       <c r="B1431" s="14" t="s">
         <v>1446</v>
@@ -24529,7 +24534,7 @@
     </row>
     <row r="1436" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1436" s="20" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="B1436" s="13" t="s">
         <v>1451</v>
@@ -24589,7 +24594,7 @@
     </row>
     <row r="1441" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1441" s="20" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="B1441" s="14" t="s">
         <v>1456</v>
@@ -24649,7 +24654,7 @@
     </row>
     <row r="1446" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1446" s="20" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="B1446" s="13" t="s">
         <v>1461</v>
@@ -24664,7 +24669,7 @@
         <v>1446</v>
       </c>
       <c r="B1447" s="14" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="C1447" s="3" t="s">
         <v>5</v>
@@ -24676,7 +24681,7 @@
         <v>1447</v>
       </c>
       <c r="B1448" s="14" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="C1448" s="3" t="s">
         <v>7</v>
@@ -24688,7 +24693,7 @@
         <v>1448</v>
       </c>
       <c r="B1449" s="14" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="C1449" s="3" t="s">
         <v>7</v>
@@ -24700,7 +24705,7 @@
         <v>1449</v>
       </c>
       <c r="B1450" s="14" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="C1450" s="3" t="s">
         <v>10</v>
@@ -24712,7 +24717,7 @@
         <v>1450</v>
       </c>
       <c r="B1451" s="14" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="C1451" s="3" t="s">
         <v>5</v>
@@ -24724,7 +24729,7 @@
         <v>1451</v>
       </c>
       <c r="B1452" s="14" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="C1452" s="3" t="s">
         <v>7</v>
@@ -24736,7 +24741,7 @@
         <v>1452</v>
       </c>
       <c r="B1453" s="14" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="C1453" s="3" t="s">
         <v>7</v>
@@ -24748,7 +24753,7 @@
         <v>1453</v>
       </c>
       <c r="B1454" s="14" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="C1454" s="3" t="s">
         <v>10</v>
@@ -26994,7 +26999,7 @@
         <v>1445</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="D1" s="39" t="s">
         <v>7</v>
@@ -27007,7 +27012,7 @@
         <v>1446</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>2182</v>
+        <v>2181</v>
       </c>
       <c r="D2" s="39"/>
       <c r="E2" s="30"/>
@@ -27018,7 +27023,7 @@
         <v>1447</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>2183</v>
+        <v>2182</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>7</v>
@@ -27031,7 +27036,7 @@
         <v>1448</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>2184</v>
+        <v>2183</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>7</v>
@@ -27044,7 +27049,7 @@
         <v>1449</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>2185</v>
+        <v>2184</v>
       </c>
       <c r="D5" s="33" t="s">
         <v>10</v>
@@ -27057,7 +27062,7 @@
         <v>1450</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="D6" s="29" t="s">
         <v>5</v>
@@ -27070,7 +27075,7 @@
         <v>1451</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>2187</v>
+        <v>2186</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>7</v>
@@ -27083,7 +27088,7 @@
         <v>1452</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>2188</v>
+        <v>2187</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>7</v>
@@ -27096,7 +27101,7 @@
         <v>1453</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="D9" s="37" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
add problem 21(5th self done)
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A79309-D223-4A93-A50F-66459F16A288}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D94437E-22F5-4133-9D7C-F3C4FF73DAF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2220" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1290" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="剑指Offer" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode 题目'!$A$2:$D$1470</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode 题目'!$A$2:$D$1486</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">剑指Offer!$A$3:$D$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">程序员面试题金典!$A$3:$D$3</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3892" uniqueCount="2203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="2223">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -6603,9 +6603,6 @@
     <t>圆形靶内的最大飞镖数量  </t>
   </si>
   <si>
-    <t>Apples &amp; Oranges  </t>
-  </si>
-  <si>
     <t>2020.5.22</t>
   </si>
   <si>
@@ -6643,13 +6640,79 @@
   </si>
   <si>
     <t>2020.6.3</t>
+  </si>
+  <si>
+    <t> 活跃用户  </t>
+  </si>
+  <si>
+    <t>检查单词是否为句中其他单词的前缀  </t>
+  </si>
+  <si>
+    <t>定长子串中元音的最大数目  </t>
+  </si>
+  <si>
+    <t>二叉树中的伪回文路径  </t>
+  </si>
+  <si>
+    <t>两个子序列的最大点积  </t>
+  </si>
+  <si>
+    <t>矩形面积  新</t>
+  </si>
+  <si>
+    <t>通过翻转子数组使两个数组相等  </t>
+  </si>
+  <si>
+    <t>检查一个字符串是否包含所有长度为 K 的二进制子串  </t>
+  </si>
+  <si>
+    <t>课程安排 IV  </t>
+  </si>
+  <si>
+    <t>摘樱桃 II  </t>
+  </si>
+  <si>
+    <t>数组中两元素的最大乘积  </t>
+  </si>
+  <si>
+    <t>切割后面积最大的蛋糕  </t>
+  </si>
+  <si>
+    <t>重新规划路线  </t>
+  </si>
+  <si>
+    <t>两个盒子中球的颜色数相同的概率  </t>
+  </si>
+  <si>
+    <t>Calculate Salaries  新</t>
+  </si>
+  <si>
+    <t>Find All the Lonely Nodes  新</t>
+  </si>
+  <si>
+    <t>$1469</t>
+  </si>
+  <si>
+    <t>$1468</t>
+  </si>
+  <si>
+    <t>$1459</t>
+  </si>
+  <si>
+    <t>$1454</t>
+  </si>
+  <si>
+    <t>2020.6.5(slef5)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6710,27 +6773,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFED7336"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF009975"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFEC4C47"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -6849,7 +6894,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6917,9 +6962,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -6931,20 +6973,11 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -6955,14 +6988,29 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -7249,12 +7297,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36439EE-948F-4B95-AA31-6B4987F28A76}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E1655"/>
+  <dimension ref="A1:E1653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I238" sqref="I238"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7262,17 +7309,17 @@
     <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="70.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
@@ -7299,7 +7346,7 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7326,7 +7373,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>4</v>
       </c>
@@ -7398,7 +7445,7 @@
       </c>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>10</v>
       </c>
@@ -7519,7 +7566,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7544,7 +7591,9 @@
       <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>2222</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
@@ -7558,7 +7607,7 @@
       </c>
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18">
         <v>23</v>
       </c>
@@ -7593,7 +7642,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7636,7 +7685,7 @@
       </c>
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18">
         <v>30</v>
       </c>
@@ -7660,7 +7709,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <v>32</v>
       </c>
@@ -7720,7 +7769,7 @@
       </c>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>37</v>
       </c>
@@ -7768,7 +7817,7 @@
       </c>
       <c r="D41" s="3"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>41</v>
       </c>
@@ -7780,7 +7829,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
         <v>42</v>
       </c>
@@ -7804,7 +7853,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="18">
         <v>44</v>
       </c>
@@ -7816,7 +7865,7 @@
       </c>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>45</v>
       </c>
@@ -7888,7 +7937,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="18">
         <v>51</v>
       </c>
@@ -7900,7 +7949,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -7962,7 +8011,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18">
         <v>57</v>
       </c>
@@ -8058,7 +8107,7 @@
       </c>
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18">
         <v>65</v>
       </c>
@@ -8098,7 +8147,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>68</v>
       </c>
@@ -8146,7 +8195,7 @@
       </c>
       <c r="D72" s="3"/>
     </row>
-    <row r="73" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>72</v>
       </c>
@@ -8194,7 +8243,7 @@
       </c>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>76</v>
       </c>
@@ -8290,7 +8339,7 @@
       </c>
       <c r="D84" s="3"/>
     </row>
-    <row r="85" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>84</v>
       </c>
@@ -8302,7 +8351,7 @@
       </c>
       <c r="D85" s="4"/>
     </row>
-    <row r="86" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="18">
         <v>85</v>
       </c>
@@ -8326,7 +8375,7 @@
       </c>
       <c r="D87" s="4"/>
     </row>
-    <row r="88" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="18">
         <v>87</v>
       </c>
@@ -8448,7 +8497,7 @@
       </c>
       <c r="D97" s="4"/>
     </row>
-    <row r="98" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="18">
         <v>97</v>
       </c>
@@ -8472,7 +8521,7 @@
       </c>
       <c r="D99" s="4"/>
     </row>
-    <row r="100" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="18">
         <v>99</v>
       </c>
@@ -8664,7 +8713,7 @@
       </c>
       <c r="D115" s="4"/>
     </row>
-    <row r="116" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="18">
         <v>115</v>
       </c>
@@ -8764,7 +8813,7 @@
       </c>
       <c r="D123" s="4"/>
     </row>
-    <row r="124" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="18">
         <v>123</v>
       </c>
@@ -8776,7 +8825,7 @@
       </c>
       <c r="D124" s="3"/>
     </row>
-    <row r="125" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="19">
         <v>124</v>
       </c>
@@ -8800,7 +8849,7 @@
       </c>
       <c r="D126" s="3"/>
     </row>
-    <row r="127" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="19">
         <v>126</v>
       </c>
@@ -8824,7 +8873,7 @@
       </c>
       <c r="D128" s="3"/>
     </row>
-    <row r="129" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="19">
         <v>128</v>
       </c>
@@ -8872,7 +8921,7 @@
       </c>
       <c r="D132" s="3"/>
     </row>
-    <row r="133" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="19">
         <v>132</v>
       </c>
@@ -8908,7 +8957,7 @@
       </c>
       <c r="D135" s="4"/>
     </row>
-    <row r="136" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="18">
         <v>135</v>
       </c>
@@ -8968,7 +9017,7 @@
       </c>
       <c r="D140" s="3"/>
     </row>
-    <row r="141" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="19">
         <v>140</v>
       </c>
@@ -8991,7 +9040,7 @@
         <v>5</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9005,7 +9054,7 @@
         <v>7</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9034,7 +9083,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="18">
         <v>145</v>
       </c>
@@ -9084,7 +9133,7 @@
       </c>
       <c r="D149" s="4"/>
     </row>
-    <row r="150" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="18">
         <v>149</v>
       </c>
@@ -9146,7 +9195,7 @@
       </c>
       <c r="D154" s="3"/>
     </row>
-    <row r="155" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="19">
         <v>154</v>
       </c>
@@ -9194,7 +9243,7 @@
       </c>
       <c r="D158" s="3"/>
     </row>
-    <row r="159" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="20" t="s">
         <v>1861</v>
       </c>
@@ -9229,7 +9278,7 @@
         <v>5</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -9268,7 +9317,7 @@
       </c>
       <c r="D164" s="3"/>
     </row>
-    <row r="165" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="19">
         <v>164</v>
       </c>
@@ -9280,7 +9329,7 @@
       </c>
       <c r="D165" s="4"/>
     </row>
-    <row r="166" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="18">
         <v>165</v>
       </c>
@@ -9390,7 +9439,7 @@
       </c>
       <c r="D174" s="3"/>
     </row>
-    <row r="175" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="19">
         <v>174</v>
       </c>
@@ -9522,7 +9571,7 @@
       </c>
       <c r="D185" s="4"/>
     </row>
-    <row r="186" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="18">
         <v>185</v>
       </c>
@@ -9558,7 +9607,7 @@
       </c>
       <c r="D188" s="3"/>
     </row>
-    <row r="189" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="19">
         <v>188</v>
       </c>
@@ -9751,7 +9800,7 @@
         <v>5</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
     </row>
     <row r="205" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9789,7 +9838,7 @@
         <v>5</v>
       </c>
       <c r="D207" s="4" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9827,7 +9876,7 @@
         <v>7</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
     </row>
     <row r="211" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9854,7 +9903,7 @@
       </c>
       <c r="D212" s="3"/>
     </row>
-    <row r="213" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="19">
         <v>212</v>
       </c>
@@ -9878,7 +9927,7 @@
       </c>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="19">
         <v>214</v>
       </c>
@@ -9926,7 +9975,7 @@
       </c>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="19">
         <v>218</v>
       </c>
@@ -9998,7 +10047,7 @@
       </c>
       <c r="D224" s="3"/>
     </row>
-    <row r="225" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="19">
         <v>224</v>
       </c>
@@ -10106,7 +10155,7 @@
       </c>
       <c r="D233" s="4"/>
     </row>
-    <row r="234" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="18">
         <v>233</v>
       </c>
@@ -10129,7 +10178,7 @@
         <v>5</v>
       </c>
       <c r="D235" s="4" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
     </row>
     <row r="236" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10180,7 +10229,7 @@
       </c>
       <c r="D239" s="4"/>
     </row>
-    <row r="240" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="18">
         <v>239</v>
       </c>
@@ -10288,7 +10337,7 @@
       </c>
       <c r="D248" s="3"/>
     </row>
-    <row r="249" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="20" t="s">
         <v>1872</v>
       </c>
@@ -10456,7 +10505,7 @@
       </c>
       <c r="D262" s="3"/>
     </row>
-    <row r="263" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A263" s="19">
         <v>262</v>
       </c>
@@ -10468,7 +10517,7 @@
       </c>
       <c r="D263" s="4"/>
     </row>
-    <row r="264" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A264" s="18">
         <v>263</v>
       </c>
@@ -10492,7 +10541,7 @@
       </c>
       <c r="D265" s="4"/>
     </row>
-    <row r="266" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A266" s="20" t="s">
         <v>1883</v>
       </c>
@@ -10540,7 +10589,7 @@
       </c>
       <c r="D269" s="4"/>
     </row>
-    <row r="270" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A270" s="20" t="s">
         <v>1886</v>
       </c>
@@ -10576,7 +10625,7 @@
       </c>
       <c r="D272" s="3"/>
     </row>
-    <row r="273" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A273" s="20" t="s">
         <v>1889</v>
       </c>
@@ -10588,7 +10637,7 @@
       </c>
       <c r="D273" s="4"/>
     </row>
-    <row r="274" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A274" s="18">
         <v>273</v>
       </c>
@@ -10600,7 +10649,7 @@
       </c>
       <c r="D274" s="3"/>
     </row>
-    <row r="275" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A275" s="19">
         <v>274</v>
       </c>
@@ -10696,7 +10745,7 @@
       </c>
       <c r="D282" s="3"/>
     </row>
-    <row r="283" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A283" s="19">
         <v>282</v>
       </c>
@@ -10708,7 +10757,7 @@
       </c>
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="18">
         <v>283</v>
       </c>
@@ -10719,7 +10768,7 @@
         <v>5</v>
       </c>
       <c r="D284" s="3" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10806,7 +10855,7 @@
       </c>
       <c r="D291" s="4"/>
     </row>
-    <row r="292" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A292" s="20" t="s">
         <v>1898</v>
       </c>
@@ -10818,7 +10867,7 @@
       </c>
       <c r="D292" s="3"/>
     </row>
-    <row r="293" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A293" s="19">
         <v>292</v>
       </c>
@@ -10854,7 +10903,7 @@
       </c>
       <c r="D295" s="4"/>
     </row>
-    <row r="296" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A296" s="18" t="s">
         <v>1902</v>
       </c>
@@ -10866,7 +10915,7 @@
       </c>
       <c r="D296" s="3"/>
     </row>
-    <row r="297" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A297" s="20" t="s">
         <v>1901</v>
       </c>
@@ -10878,7 +10927,7 @@
       </c>
       <c r="D297" s="4"/>
     </row>
-    <row r="298" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A298" s="18">
         <v>297</v>
       </c>
@@ -10926,7 +10975,7 @@
       </c>
       <c r="D301" s="4"/>
     </row>
-    <row r="302" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A302" s="18">
         <v>301</v>
       </c>
@@ -10938,7 +10987,7 @@
       </c>
       <c r="D302" s="3"/>
     </row>
-    <row r="303" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="20" t="s">
         <v>1904</v>
       </c>
@@ -10950,7 +10999,7 @@
       </c>
       <c r="D303" s="4"/>
     </row>
-    <row r="304" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A304" s="18">
         <v>303</v>
       </c>
@@ -10974,7 +11023,7 @@
       </c>
       <c r="D305" s="4"/>
     </row>
-    <row r="306" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A306" s="20" t="s">
         <v>1905</v>
       </c>
@@ -10986,7 +11035,7 @@
       </c>
       <c r="D306" s="3"/>
     </row>
-    <row r="307" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A307" s="19">
         <v>306</v>
       </c>
@@ -11010,7 +11059,7 @@
       </c>
       <c r="D308" s="3"/>
     </row>
-    <row r="309" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A309" s="20" t="s">
         <v>1906</v>
       </c>
@@ -11022,7 +11071,7 @@
       </c>
       <c r="D309" s="4"/>
     </row>
-    <row r="310" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="18">
         <v>309</v>
       </c>
@@ -11058,7 +11107,7 @@
       </c>
       <c r="D312" s="3"/>
     </row>
-    <row r="313" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A313" s="19">
         <v>312</v>
       </c>
@@ -11070,7 +11119,7 @@
       </c>
       <c r="D313" s="4"/>
     </row>
-    <row r="314" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A314" s="18">
         <v>313</v>
       </c>
@@ -11094,7 +11143,7 @@
       </c>
       <c r="D315" s="4"/>
     </row>
-    <row r="316" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A316" s="18">
         <v>315</v>
       </c>
@@ -11106,7 +11155,7 @@
       </c>
       <c r="D316" s="3"/>
     </row>
-    <row r="317" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="19">
         <v>316</v>
       </c>
@@ -11118,7 +11167,7 @@
       </c>
       <c r="D317" s="4"/>
     </row>
-    <row r="318" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A318" s="20" t="s">
         <v>1909</v>
       </c>
@@ -11166,7 +11215,7 @@
       </c>
       <c r="D321" s="4"/>
     </row>
-    <row r="322" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A322" s="18">
         <v>321</v>
       </c>
@@ -11178,7 +11227,7 @@
       </c>
       <c r="D322" s="3"/>
     </row>
-    <row r="323" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A323" s="19">
         <v>322</v>
       </c>
@@ -11238,7 +11287,7 @@
       </c>
       <c r="D327" s="4"/>
     </row>
-    <row r="328" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A328" s="18">
         <v>327</v>
       </c>
@@ -11261,10 +11310,10 @@
         <v>7</v>
       </c>
       <c r="D329" s="4" t="s">
-        <v>2201</v>
-      </c>
-    </row>
-    <row r="330" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A330" s="18">
         <v>329</v>
       </c>
@@ -11276,7 +11325,7 @@
       </c>
       <c r="D330" s="3"/>
     </row>
-    <row r="331" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A331" s="19">
         <v>330</v>
       </c>
@@ -11336,7 +11385,7 @@
       </c>
       <c r="D335" s="4"/>
     </row>
-    <row r="336" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A336" s="18">
         <v>335</v>
       </c>
@@ -11348,7 +11397,7 @@
       </c>
       <c r="D336" s="3"/>
     </row>
-    <row r="337" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A337" s="19">
         <v>336</v>
       </c>
@@ -11396,7 +11445,7 @@
       </c>
       <c r="D340" s="3"/>
     </row>
-    <row r="341" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A341" s="20" t="s">
         <v>1915</v>
       </c>
@@ -11542,7 +11591,7 @@
       </c>
       <c r="D352" s="3"/>
     </row>
-    <row r="353" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A353" s="19">
         <v>352</v>
       </c>
@@ -11566,7 +11615,7 @@
       </c>
       <c r="D354" s="3"/>
     </row>
-    <row r="355" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A355" s="19">
         <v>354</v>
       </c>
@@ -11578,7 +11627,7 @@
       </c>
       <c r="D355" s="4"/>
     </row>
-    <row r="356" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A356" s="18">
         <v>355</v>
       </c>
@@ -11614,7 +11663,7 @@
       </c>
       <c r="D358" s="3"/>
     </row>
-    <row r="359" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="20" t="s">
         <v>1921</v>
       </c>
@@ -11674,7 +11723,7 @@
       </c>
       <c r="D363" s="4"/>
     </row>
-    <row r="364" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A364" s="19" t="s">
         <v>1929</v>
       </c>
@@ -11890,7 +11939,7 @@
       </c>
       <c r="D381" s="4"/>
     </row>
-    <row r="382" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A382" s="18">
         <v>381</v>
       </c>
@@ -12010,7 +12059,7 @@
       </c>
       <c r="D391" s="4"/>
     </row>
-    <row r="392" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A392" s="18">
         <v>391</v>
       </c>
@@ -12154,7 +12203,7 @@
       </c>
       <c r="D403" s="4"/>
     </row>
-    <row r="404" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A404" s="18">
         <v>403</v>
       </c>
@@ -12202,7 +12251,7 @@
       </c>
       <c r="D407" s="4"/>
     </row>
-    <row r="408" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A408" s="18">
         <v>407</v>
       </c>
@@ -12238,7 +12287,7 @@
       </c>
       <c r="D410" s="3"/>
     </row>
-    <row r="411" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A411" s="19">
         <v>410</v>
       </c>
@@ -12250,7 +12299,7 @@
       </c>
       <c r="D411" s="4"/>
     </row>
-    <row r="412" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="20" t="s">
         <v>1934</v>
       </c>
@@ -12262,7 +12311,7 @@
       </c>
       <c r="D412" s="3"/>
     </row>
-    <row r="413" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A413" s="19">
         <v>412</v>
       </c>
@@ -12358,7 +12407,7 @@
       </c>
       <c r="D420" s="3"/>
     </row>
-    <row r="421" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A421" s="19">
         <v>420</v>
       </c>
@@ -12418,7 +12467,7 @@
       </c>
       <c r="D425" s="4"/>
     </row>
-    <row r="426" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A426" s="20" t="s">
         <v>1937</v>
       </c>
@@ -12454,7 +12503,7 @@
       </c>
       <c r="D428" s="3"/>
     </row>
-    <row r="429" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A429" s="20" t="s">
         <v>1939</v>
       </c>
@@ -12466,7 +12515,7 @@
       </c>
       <c r="D429" s="4"/>
     </row>
-    <row r="430" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A430" s="18">
         <v>429</v>
       </c>
@@ -12490,7 +12539,7 @@
       </c>
       <c r="D431" s="4"/>
     </row>
-    <row r="432" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A432" s="20" t="s">
         <v>1941</v>
       </c>
@@ -12502,7 +12551,7 @@
       </c>
       <c r="D432" s="3"/>
     </row>
-    <row r="433" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A433" s="19">
         <v>432</v>
       </c>
@@ -12598,7 +12647,7 @@
       </c>
       <c r="D440" s="3"/>
     </row>
-    <row r="441" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A441" s="19">
         <v>440</v>
       </c>
@@ -12610,7 +12659,7 @@
       </c>
       <c r="D441" s="4"/>
     </row>
-    <row r="442" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A442" s="18">
         <v>441</v>
       </c>
@@ -12670,7 +12719,7 @@
       </c>
       <c r="D446" s="3"/>
     </row>
-    <row r="447" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A447" s="19">
         <v>446</v>
       </c>
@@ -12814,7 +12863,7 @@
       </c>
       <c r="D458" s="3"/>
     </row>
-    <row r="459" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A459" s="19">
         <v>458</v>
       </c>
@@ -12838,7 +12887,7 @@
       </c>
       <c r="D460" s="3"/>
     </row>
-    <row r="461" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A461" s="19">
         <v>460</v>
       </c>
@@ -12898,7 +12947,7 @@
       </c>
       <c r="D465" s="4"/>
     </row>
-    <row r="466" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A466" s="20" t="s">
         <v>1944</v>
       </c>
@@ -12910,7 +12959,7 @@
       </c>
       <c r="D466" s="3"/>
     </row>
-    <row r="467" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A467" s="19">
         <v>466</v>
       </c>
@@ -12970,7 +13019,7 @@
       </c>
       <c r="D471" s="4"/>
     </row>
-    <row r="472" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A472" s="20" t="s">
         <v>1946</v>
       </c>
@@ -12982,7 +13031,7 @@
       </c>
       <c r="D472" s="3"/>
     </row>
-    <row r="473" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A473" s="19">
         <v>472</v>
       </c>
@@ -13066,7 +13115,7 @@
       </c>
       <c r="D479" s="4"/>
     </row>
-    <row r="480" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A480" s="18">
         <v>479</v>
       </c>
@@ -13078,7 +13127,7 @@
       </c>
       <c r="D480" s="3"/>
     </row>
-    <row r="481" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A481" s="19">
         <v>480</v>
       </c>
@@ -13114,7 +13163,7 @@
       </c>
       <c r="D483" s="4"/>
     </row>
-    <row r="484" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A484" s="18">
         <v>483</v>
       </c>
@@ -13176,7 +13225,7 @@
       </c>
       <c r="D488" s="3"/>
     </row>
-    <row r="489" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A489" s="19">
         <v>488</v>
       </c>
@@ -13188,7 +13237,7 @@
       </c>
       <c r="D489" s="4"/>
     </row>
-    <row r="490" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A490" s="20" t="s">
         <v>1949</v>
       </c>
@@ -13236,7 +13285,7 @@
       </c>
       <c r="D493" s="4"/>
     </row>
-    <row r="494" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A494" s="18">
         <v>493</v>
       </c>
@@ -13310,7 +13359,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="500" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A500" s="20" t="s">
         <v>1951</v>
       </c>
@@ -13322,7 +13371,7 @@
       </c>
       <c r="D500" s="3"/>
     </row>
-    <row r="501" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A501" s="19">
         <v>500</v>
       </c>
@@ -13346,7 +13395,7 @@
       </c>
       <c r="D502" s="3"/>
     </row>
-    <row r="503" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A503" s="19">
         <v>502</v>
       </c>
@@ -13490,7 +13539,7 @@
       </c>
       <c r="D514" s="3"/>
     </row>
-    <row r="515" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A515" s="19">
         <v>514</v>
       </c>
@@ -13526,7 +13575,7 @@
       </c>
       <c r="D517" s="4"/>
     </row>
-    <row r="518" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A518" s="18">
         <v>517</v>
       </c>
@@ -13646,7 +13695,7 @@
       </c>
       <c r="D527" s="4"/>
     </row>
-    <row r="528" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A528" s="20" t="s">
         <v>1956</v>
       </c>
@@ -13658,7 +13707,7 @@
       </c>
       <c r="D528" s="3"/>
     </row>
-    <row r="529" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A529" s="19">
         <v>528</v>
       </c>
@@ -13874,7 +13923,7 @@
       </c>
       <c r="D546" s="3"/>
     </row>
-    <row r="547" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A547" s="19">
         <v>546</v>
       </c>
@@ -13886,7 +13935,7 @@
       </c>
       <c r="D547" s="4"/>
     </row>
-    <row r="548" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="18">
         <v>547</v>
       </c>
@@ -13946,7 +13995,7 @@
       </c>
       <c r="D552" s="3"/>
     </row>
-    <row r="553" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A553" s="19">
         <v>552</v>
       </c>
@@ -14017,7 +14066,7 @@
         <v>5</v>
       </c>
       <c r="D558" s="3" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="559" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14094,7 +14143,7 @@
       </c>
       <c r="D564" s="3"/>
     </row>
-    <row r="565" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A565" s="19">
         <v>564</v>
       </c>
@@ -14142,7 +14191,7 @@
       </c>
       <c r="D568" s="3"/>
     </row>
-    <row r="569" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A569" s="20" t="s">
         <v>1968</v>
       </c>
@@ -14154,7 +14203,7 @@
       </c>
       <c r="D569" s="4"/>
     </row>
-    <row r="570" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A570" s="20" t="s">
         <v>1969</v>
       </c>
@@ -14178,7 +14227,7 @@
       </c>
       <c r="D571" s="4"/>
     </row>
-    <row r="572" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A572" s="20" t="s">
         <v>1971</v>
       </c>
@@ -14274,7 +14323,7 @@
       </c>
       <c r="D579" s="4"/>
     </row>
-    <row r="580" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A580" s="20" t="s">
         <v>1978</v>
       </c>
@@ -14370,7 +14419,7 @@
       </c>
       <c r="D587" s="4"/>
     </row>
-    <row r="588" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A588" s="18" t="s">
         <v>1985</v>
       </c>
@@ -14382,7 +14431,7 @@
       </c>
       <c r="D588" s="3"/>
     </row>
-    <row r="589" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="589" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A589" s="20" t="s">
         <v>1984</v>
       </c>
@@ -14418,7 +14467,7 @@
       </c>
       <c r="D591" s="4"/>
     </row>
-    <row r="592" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="592" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A592" s="18">
         <v>591</v>
       </c>
@@ -14526,7 +14575,7 @@
       </c>
       <c r="D600" s="3"/>
     </row>
-    <row r="601" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A601" s="19">
         <v>600</v>
       </c>
@@ -14538,7 +14587,7 @@
       </c>
       <c r="D601" s="4"/>
     </row>
-    <row r="602" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A602" s="18">
         <v>601</v>
       </c>
@@ -14706,7 +14755,7 @@
       </c>
       <c r="D615" s="4"/>
     </row>
-    <row r="616" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A616" s="20" t="s">
         <v>1998</v>
       </c>
@@ -14742,7 +14791,7 @@
       </c>
       <c r="D618" s="3"/>
     </row>
-    <row r="619" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A619" s="20" t="s">
         <v>2000</v>
       </c>
@@ -14874,7 +14923,7 @@
       </c>
       <c r="D629" s="4"/>
     </row>
-    <row r="630" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A630" s="18">
         <v>629</v>
       </c>
@@ -14886,7 +14935,7 @@
       </c>
       <c r="D630" s="3"/>
     </row>
-    <row r="631" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A631" s="19">
         <v>630</v>
       </c>
@@ -14898,7 +14947,7 @@
       </c>
       <c r="D631" s="4"/>
     </row>
-    <row r="632" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A632" s="20" t="s">
         <v>2006</v>
       </c>
@@ -14910,7 +14959,7 @@
       </c>
       <c r="D632" s="3"/>
     </row>
-    <row r="633" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A633" s="19">
         <v>632</v>
       </c>
@@ -14994,7 +15043,7 @@
       </c>
       <c r="D639" s="4"/>
     </row>
-    <row r="640" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A640" s="18">
         <v>639</v>
       </c>
@@ -15030,7 +15079,7 @@
       </c>
       <c r="D642" s="3"/>
     </row>
-    <row r="643" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="643" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A643" s="20" t="s">
         <v>2009</v>
       </c>
@@ -15042,7 +15091,7 @@
       </c>
       <c r="D643" s="4"/>
     </row>
-    <row r="644" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="644" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A644" s="19" t="s">
         <v>2011</v>
       </c>
@@ -15054,7 +15103,7 @@
       </c>
       <c r="D644" s="3"/>
     </row>
-    <row r="645" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="645" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A645" s="20" t="s">
         <v>2010</v>
       </c>
@@ -15066,7 +15115,7 @@
       </c>
       <c r="D645" s="4"/>
     </row>
-    <row r="646" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="646" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A646" s="18">
         <v>645</v>
       </c>
@@ -15198,7 +15247,7 @@
       </c>
       <c r="D656" s="3"/>
     </row>
-    <row r="657" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="657" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A657" s="20" t="s">
         <v>2013</v>
       </c>
@@ -15210,7 +15259,7 @@
       </c>
       <c r="D657" s="4"/>
     </row>
-    <row r="658" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="658" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A658" s="18">
         <v>657</v>
       </c>
@@ -15246,7 +15295,7 @@
       </c>
       <c r="D660" s="3"/>
     </row>
-    <row r="661" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="661" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A661" s="20" t="s">
         <v>2014</v>
       </c>
@@ -15258,7 +15307,7 @@
       </c>
       <c r="D661" s="4"/>
     </row>
-    <row r="662" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="662" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A662" s="18">
         <v>661</v>
       </c>
@@ -15294,7 +15343,7 @@
       </c>
       <c r="D664" s="3"/>
     </row>
-    <row r="665" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="665" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A665" s="19">
         <v>664</v>
       </c>
@@ -15306,7 +15355,7 @@
       </c>
       <c r="D665" s="4"/>
     </row>
-    <row r="666" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="666" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A666" s="18">
         <v>665</v>
       </c>
@@ -15342,7 +15391,7 @@
       </c>
       <c r="D668" s="3"/>
     </row>
-    <row r="669" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="669" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A669" s="19">
         <v>668</v>
       </c>
@@ -15426,7 +15475,7 @@
       </c>
       <c r="D675" s="4"/>
     </row>
-    <row r="676" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="676" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A676" s="18">
         <v>675</v>
       </c>
@@ -15474,7 +15523,7 @@
       </c>
       <c r="D679" s="4"/>
     </row>
-    <row r="680" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="680" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A680" s="18">
         <v>679</v>
       </c>
@@ -15522,7 +15571,7 @@
       </c>
       <c r="D683" s="4"/>
     </row>
-    <row r="684" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="684" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A684" s="20" t="s">
         <v>2018</v>
       </c>
@@ -15534,7 +15583,7 @@
       </c>
       <c r="D684" s="3"/>
     </row>
-    <row r="685" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="685" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A685" s="19">
         <v>684</v>
       </c>
@@ -15546,7 +15595,7 @@
       </c>
       <c r="D685" s="4"/>
     </row>
-    <row r="686" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="686" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A686" s="18">
         <v>685</v>
       </c>
@@ -15594,7 +15643,7 @@
       </c>
       <c r="D689" s="4"/>
     </row>
-    <row r="690" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="690" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A690" s="18">
         <v>689</v>
       </c>
@@ -15618,7 +15667,7 @@
       </c>
       <c r="D691" s="4"/>
     </row>
-    <row r="692" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="692" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A692" s="18">
         <v>691</v>
       </c>
@@ -15714,7 +15763,7 @@
       </c>
       <c r="D699" s="4"/>
     </row>
-    <row r="700" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="700" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A700" s="18">
         <v>699</v>
       </c>
@@ -15821,7 +15870,7 @@
         <v>7</v>
       </c>
       <c r="D708" s="3" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
     </row>
     <row r="709" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -15848,7 +15897,7 @@
       </c>
       <c r="D710" s="3"/>
     </row>
-    <row r="711" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="711" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A711" s="19">
         <v>710</v>
       </c>
@@ -15860,7 +15909,7 @@
       </c>
       <c r="D711" s="4"/>
     </row>
-    <row r="712" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="712" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A712" s="20" t="s">
         <v>2023</v>
       </c>
@@ -15872,7 +15921,7 @@
       </c>
       <c r="D712" s="3"/>
     </row>
-    <row r="713" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="713" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A713" s="19">
         <v>712</v>
       </c>
@@ -15908,7 +15957,7 @@
       </c>
       <c r="D715" s="4"/>
     </row>
-    <row r="716" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="716" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A716" s="18">
         <v>715</v>
       </c>
@@ -15956,7 +16005,7 @@
       </c>
       <c r="D719" s="4"/>
     </row>
-    <row r="720" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="720" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A720" s="18">
         <v>719</v>
       </c>
@@ -16042,7 +16091,7 @@
       </c>
       <c r="D726" s="3"/>
     </row>
-    <row r="727" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="727" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A727" s="19">
         <v>726</v>
       </c>
@@ -16054,7 +16103,7 @@
       </c>
       <c r="D727" s="4"/>
     </row>
-    <row r="728" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="728" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A728" s="20" t="s">
         <v>2026</v>
       </c>
@@ -16066,7 +16115,7 @@
       </c>
       <c r="D728" s="3"/>
     </row>
-    <row r="729" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="729" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A729" s="19">
         <v>728</v>
       </c>
@@ -16090,7 +16139,7 @@
       </c>
       <c r="D730" s="3"/>
     </row>
-    <row r="731" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="731" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A731" s="19">
         <v>730</v>
       </c>
@@ -16114,7 +16163,7 @@
       </c>
       <c r="D732" s="3"/>
     </row>
-    <row r="733" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="733" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A733" s="19">
         <v>732</v>
       </c>
@@ -16162,7 +16211,7 @@
       </c>
       <c r="D736" s="3"/>
     </row>
-    <row r="737" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="737" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A737" s="19">
         <v>736</v>
       </c>
@@ -16222,7 +16271,7 @@
       </c>
       <c r="D741" s="4"/>
     </row>
-    <row r="742" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="742" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A742" s="18">
         <v>741</v>
       </c>
@@ -16270,7 +16319,7 @@
       </c>
       <c r="D745" s="4"/>
     </row>
-    <row r="746" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="746" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A746" s="18">
         <v>745</v>
       </c>
@@ -16320,7 +16369,7 @@
       </c>
       <c r="D749" s="4"/>
     </row>
-    <row r="750" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="750" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A750" s="18">
         <v>749</v>
       </c>
@@ -16368,7 +16417,7 @@
       </c>
       <c r="D753" s="4"/>
     </row>
-    <row r="754" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="754" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A754" s="18">
         <v>753</v>
       </c>
@@ -16416,7 +16465,7 @@
       </c>
       <c r="D757" s="4"/>
     </row>
-    <row r="758" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="758" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A758" s="18">
         <v>757</v>
       </c>
@@ -16440,7 +16489,7 @@
       </c>
       <c r="D759" s="4"/>
     </row>
-    <row r="760" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="760" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A760" s="20" t="s">
         <v>2034</v>
       </c>
@@ -16464,7 +16513,7 @@
       </c>
       <c r="D761" s="4"/>
     </row>
-    <row r="762" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="762" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A762" s="18">
         <v>761</v>
       </c>
@@ -16476,7 +16525,7 @@
       </c>
       <c r="D762" s="3"/>
     </row>
-    <row r="763" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="763" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A763" s="19">
         <v>762</v>
       </c>
@@ -16512,7 +16561,7 @@
       </c>
       <c r="D765" s="4"/>
     </row>
-    <row r="766" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="766" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A766" s="18">
         <v>765</v>
       </c>
@@ -16548,7 +16597,7 @@
       </c>
       <c r="D768" s="3"/>
     </row>
-    <row r="769" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="769" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A769" s="19">
         <v>768</v>
       </c>
@@ -16572,7 +16621,7 @@
       </c>
       <c r="D770" s="3"/>
     </row>
-    <row r="771" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="771" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A771" s="19">
         <v>770</v>
       </c>
@@ -16596,7 +16645,7 @@
       </c>
       <c r="D772" s="3"/>
     </row>
-    <row r="773" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="773" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A773" s="20" t="s">
         <v>2036</v>
       </c>
@@ -16608,7 +16657,7 @@
       </c>
       <c r="D773" s="4"/>
     </row>
-    <row r="774" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="774" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A774" s="18">
         <v>773</v>
       </c>
@@ -16620,7 +16669,7 @@
       </c>
       <c r="D774" s="3"/>
     </row>
-    <row r="775" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="775" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A775" s="20" t="s">
         <v>2037</v>
       </c>
@@ -16632,7 +16681,7 @@
       </c>
       <c r="D775" s="4"/>
     </row>
-    <row r="776" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="776" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A776" s="18">
         <v>775</v>
       </c>
@@ -16668,7 +16717,7 @@
       </c>
       <c r="D778" s="3"/>
     </row>
-    <row r="779" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="779" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A779" s="19">
         <v>778</v>
       </c>
@@ -16692,7 +16741,7 @@
       </c>
       <c r="D780" s="3"/>
     </row>
-    <row r="781" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="781" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A781" s="19">
         <v>780</v>
       </c>
@@ -16716,7 +16765,7 @@
       </c>
       <c r="D782" s="3"/>
     </row>
-    <row r="783" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="783" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A783" s="19">
         <v>782</v>
       </c>
@@ -16764,7 +16813,7 @@
       </c>
       <c r="D786" s="3"/>
     </row>
-    <row r="787" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="787" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A787" s="19">
         <v>786</v>
       </c>
@@ -16848,7 +16897,7 @@
       </c>
       <c r="D793" s="4"/>
     </row>
-    <row r="794" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="794" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A794" s="18">
         <v>793</v>
       </c>
@@ -16908,7 +16957,7 @@
       </c>
       <c r="D798" s="3"/>
     </row>
-    <row r="799" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="799" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A799" s="19">
         <v>798</v>
       </c>
@@ -16968,7 +17017,7 @@
       </c>
       <c r="D803" s="4"/>
     </row>
-    <row r="804" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="804" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A804" s="18">
         <v>803</v>
       </c>
@@ -16992,7 +17041,7 @@
       </c>
       <c r="D805" s="4"/>
     </row>
-    <row r="806" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="806" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A806" s="18">
         <v>805</v>
       </c>
@@ -17052,7 +17101,7 @@
       </c>
       <c r="D810" s="3"/>
     </row>
-    <row r="811" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="811" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A811" s="19">
         <v>810</v>
       </c>
@@ -17112,7 +17161,7 @@
       </c>
       <c r="D815" s="4"/>
     </row>
-    <row r="816" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="816" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A816" s="18">
         <v>815</v>
       </c>
@@ -17148,7 +17197,7 @@
       </c>
       <c r="D818" s="3"/>
     </row>
-    <row r="819" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="819" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A819" s="19">
         <v>818</v>
       </c>
@@ -17256,7 +17305,7 @@
       </c>
       <c r="D827" s="4"/>
     </row>
-    <row r="828" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="828" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A828" s="18">
         <v>827</v>
       </c>
@@ -17268,7 +17317,7 @@
       </c>
       <c r="D828" s="3"/>
     </row>
-    <row r="829" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="829" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A829" s="19">
         <v>828</v>
       </c>
@@ -17280,7 +17329,7 @@
       </c>
       <c r="D829" s="4"/>
     </row>
-    <row r="830" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="830" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A830" s="18">
         <v>829</v>
       </c>
@@ -17340,7 +17389,7 @@
       </c>
       <c r="D834" s="3"/>
     </row>
-    <row r="835" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="835" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A835" s="19">
         <v>834</v>
       </c>
@@ -17400,7 +17449,7 @@
       </c>
       <c r="D839" s="4"/>
     </row>
-    <row r="840" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="840" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A840" s="18">
         <v>839</v>
       </c>
@@ -17448,7 +17497,7 @@
       </c>
       <c r="D843" s="4"/>
     </row>
-    <row r="844" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="844" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A844" s="18">
         <v>843</v>
       </c>
@@ -17496,7 +17545,7 @@
       </c>
       <c r="D847" s="4"/>
     </row>
-    <row r="848" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="848" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A848" s="18">
         <v>847</v>
       </c>
@@ -17532,7 +17581,7 @@
       </c>
       <c r="D850" s="3"/>
     </row>
-    <row r="851" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="851" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A851" s="19">
         <v>850</v>
       </c>
@@ -17580,7 +17629,7 @@
       </c>
       <c r="D854" s="3"/>
     </row>
-    <row r="855" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="855" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A855" s="19">
         <v>854</v>
       </c>
@@ -17616,7 +17665,7 @@
       </c>
       <c r="D857" s="4"/>
     </row>
-    <row r="858" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="858" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A858" s="18">
         <v>857</v>
       </c>
@@ -17676,7 +17725,7 @@
       </c>
       <c r="D862" s="3"/>
     </row>
-    <row r="863" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="863" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A863" s="19">
         <v>862</v>
       </c>
@@ -17700,7 +17749,7 @@
       </c>
       <c r="D864" s="3"/>
     </row>
-    <row r="865" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="865" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A865" s="19">
         <v>864</v>
       </c>
@@ -17784,7 +17833,7 @@
       </c>
       <c r="D871" s="4"/>
     </row>
-    <row r="872" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="872" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A872" s="18">
         <v>871</v>
       </c>
@@ -17868,7 +17917,7 @@
       </c>
       <c r="D878" s="3"/>
     </row>
-    <row r="879" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="879" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A879" s="19">
         <v>878</v>
       </c>
@@ -17880,7 +17929,7 @@
       </c>
       <c r="D879" s="4"/>
     </row>
-    <row r="880" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="880" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A880" s="18">
         <v>879</v>
       </c>
@@ -17916,7 +17965,7 @@
       </c>
       <c r="D882" s="3"/>
     </row>
-    <row r="883" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="883" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A883" s="19">
         <v>882</v>
       </c>
@@ -17976,7 +18025,7 @@
       </c>
       <c r="D887" s="4"/>
     </row>
-    <row r="888" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="888" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A888" s="18">
         <v>887</v>
       </c>
@@ -18024,7 +18073,7 @@
       </c>
       <c r="D891" s="4"/>
     </row>
-    <row r="892" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="892" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A892" s="18">
         <v>891</v>
       </c>
@@ -18072,7 +18121,7 @@
       </c>
       <c r="D895" s="4"/>
     </row>
-    <row r="896" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="896" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A896" s="18">
         <v>895</v>
       </c>
@@ -18120,7 +18169,7 @@
       </c>
       <c r="D899" s="4"/>
     </row>
-    <row r="900" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="900" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A900" s="18">
         <v>899</v>
       </c>
@@ -18156,7 +18205,7 @@
       </c>
       <c r="D902" s="3"/>
     </row>
-    <row r="903" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="903" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A903" s="19">
         <v>902</v>
       </c>
@@ -18168,7 +18217,7 @@
       </c>
       <c r="D903" s="4"/>
     </row>
-    <row r="904" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="904" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A904" s="18">
         <v>903</v>
       </c>
@@ -18204,7 +18253,7 @@
       </c>
       <c r="D906" s="3"/>
     </row>
-    <row r="907" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="907" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A907" s="19">
         <v>906</v>
       </c>
@@ -18288,7 +18337,7 @@
       </c>
       <c r="D913" s="4"/>
     </row>
-    <row r="914" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="914" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A914" s="18">
         <v>913</v>
       </c>
@@ -18372,7 +18421,7 @@
       </c>
       <c r="D920" s="3"/>
     </row>
-    <row r="921" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="921" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A921" s="19">
         <v>920</v>
       </c>
@@ -18420,7 +18469,7 @@
       </c>
       <c r="D924" s="3"/>
     </row>
-    <row r="925" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="925" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A925" s="19">
         <v>924</v>
       </c>
@@ -18456,7 +18505,7 @@
       </c>
       <c r="D927" s="4"/>
     </row>
-    <row r="928" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="928" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A928" s="18">
         <v>927</v>
       </c>
@@ -18468,7 +18517,7 @@
       </c>
       <c r="D928" s="3"/>
     </row>
-    <row r="929" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="929" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A929" s="19">
         <v>928</v>
       </c>
@@ -18564,7 +18613,7 @@
       </c>
       <c r="D936" s="3"/>
     </row>
-    <row r="937" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="937" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A937" s="19">
         <v>936</v>
       </c>
@@ -18612,7 +18661,7 @@
       </c>
       <c r="D940" s="3"/>
     </row>
-    <row r="941" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="941" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A941" s="19">
         <v>940</v>
       </c>
@@ -18648,7 +18697,7 @@
       </c>
       <c r="D943" s="4"/>
     </row>
-    <row r="944" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="944" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A944" s="18">
         <v>943</v>
       </c>
@@ -18756,7 +18805,7 @@
       </c>
       <c r="D952" s="3"/>
     </row>
-    <row r="953" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="953" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A953" s="19">
         <v>952</v>
       </c>
@@ -18804,7 +18853,7 @@
       </c>
       <c r="D956" s="3"/>
     </row>
-    <row r="957" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="957" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A957" s="19">
         <v>956</v>
       </c>
@@ -18852,7 +18901,7 @@
       </c>
       <c r="D960" s="3"/>
     </row>
-    <row r="961" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="961" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A961" s="19">
         <v>960</v>
       </c>
@@ -18900,7 +18949,7 @@
       </c>
       <c r="D964" s="3"/>
     </row>
-    <row r="965" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="965" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A965" s="19">
         <v>964</v>
       </c>
@@ -18948,7 +18997,7 @@
       </c>
       <c r="D968" s="3"/>
     </row>
-    <row r="969" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="969" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A969" s="19">
         <v>968</v>
       </c>
@@ -18996,7 +19045,7 @@
       </c>
       <c r="D972" s="3"/>
     </row>
-    <row r="973" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="973" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A973" s="19">
         <v>972</v>
       </c>
@@ -19032,7 +19081,7 @@
       </c>
       <c r="D975" s="4"/>
     </row>
-    <row r="976" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="976" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A976" s="18">
         <v>975</v>
       </c>
@@ -19092,7 +19141,7 @@
       </c>
       <c r="D980" s="3"/>
     </row>
-    <row r="981" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="981" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A981" s="19">
         <v>980</v>
       </c>
@@ -19116,7 +19165,7 @@
       </c>
       <c r="D982" s="3"/>
     </row>
-    <row r="983" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="983" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A983" s="19">
         <v>982</v>
       </c>
@@ -19236,7 +19285,7 @@
       </c>
       <c r="D992" s="3"/>
     </row>
-    <row r="993" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="993" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A993" s="19">
         <v>992</v>
       </c>
@@ -19272,7 +19321,7 @@
       </c>
       <c r="D995" s="4"/>
     </row>
-    <row r="996" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="996" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A996" s="18">
         <v>995</v>
       </c>
@@ -19284,7 +19333,7 @@
       </c>
       <c r="D996" s="3"/>
     </row>
-    <row r="997" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="997" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A997" s="19">
         <v>996</v>
       </c>
@@ -19332,7 +19381,7 @@
       </c>
       <c r="D1000" s="3"/>
     </row>
-    <row r="1001" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1001" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1001" s="19">
         <v>1000</v>
       </c>
@@ -19344,7 +19393,7 @@
       </c>
       <c r="D1001" s="4"/>
     </row>
-    <row r="1002" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1002" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1002" s="18">
         <v>1001</v>
       </c>
@@ -19476,7 +19525,7 @@
       </c>
       <c r="D1012" s="3"/>
     </row>
-    <row r="1013" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1013" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1013" s="19">
         <v>1012</v>
       </c>
@@ -19668,7 +19717,7 @@
       </c>
       <c r="D1028" s="3"/>
     </row>
-    <row r="1029" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1029" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1029" s="19">
         <v>1028</v>
       </c>
@@ -19716,7 +19765,7 @@
       </c>
       <c r="D1032" s="3"/>
     </row>
-    <row r="1033" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1033" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1033" s="19">
         <v>1032</v>
       </c>
@@ -19764,7 +19813,7 @@
       </c>
       <c r="D1036" s="3"/>
     </row>
-    <row r="1037" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1037" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1037" s="19">
         <v>1036</v>
       </c>
@@ -19860,7 +19909,7 @@
       </c>
       <c r="D1044" s="3"/>
     </row>
-    <row r="1045" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1045" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1045" s="19">
         <v>1044</v>
       </c>
@@ -20088,7 +20137,7 @@
       </c>
       <c r="D1063" s="4"/>
     </row>
-    <row r="1064" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1064" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1064" s="20" t="s">
         <v>2050</v>
       </c>
@@ -20136,7 +20185,7 @@
       </c>
       <c r="D1067" s="4"/>
     </row>
-    <row r="1068" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1068" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1068" s="20" t="s">
         <v>2054</v>
       </c>
@@ -20220,7 +20269,7 @@
       </c>
       <c r="D1074" s="3"/>
     </row>
-    <row r="1075" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1075" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1075" s="19">
         <v>1074</v>
       </c>
@@ -20388,7 +20437,7 @@
       </c>
       <c r="D1088" s="3"/>
     </row>
-    <row r="1089" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1089" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1089" s="20" t="s">
         <v>2067</v>
       </c>
@@ -20436,7 +20485,7 @@
       </c>
       <c r="D1092" s="3"/>
     </row>
-    <row r="1093" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1093" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1093" s="19">
         <v>1092</v>
       </c>
@@ -20472,7 +20521,7 @@
       </c>
       <c r="D1095" s="4"/>
     </row>
-    <row r="1096" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1096" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1096" s="18">
         <v>1095</v>
       </c>
@@ -20484,7 +20533,7 @@
       </c>
       <c r="D1096" s="3"/>
     </row>
-    <row r="1097" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1097" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1097" s="19">
         <v>1096</v>
       </c>
@@ -20496,7 +20545,7 @@
       </c>
       <c r="D1097" s="4"/>
     </row>
-    <row r="1098" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1098" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1098" s="20" t="s">
         <v>2068</v>
       </c>
@@ -20604,7 +20653,7 @@
       </c>
       <c r="D1106" s="3"/>
     </row>
-    <row r="1107" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1107" s="19">
         <v>1106</v>
       </c>
@@ -20784,7 +20833,7 @@
       </c>
       <c r="D1121" s="4"/>
     </row>
-    <row r="1122" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1122" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1122" s="20" t="s">
         <v>2080</v>
       </c>
@@ -20832,7 +20881,7 @@
       </c>
       <c r="D1125" s="4"/>
     </row>
-    <row r="1126" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1126" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1126" s="18">
         <v>1125</v>
       </c>
@@ -20856,7 +20905,7 @@
       </c>
       <c r="D1127" s="4"/>
     </row>
-    <row r="1128" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1128" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1128" s="20" t="s">
         <v>2082</v>
       </c>
@@ -20964,7 +21013,7 @@
       </c>
       <c r="D1136" s="3"/>
     </row>
-    <row r="1137" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1137" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1137" s="20" t="s">
         <v>2087</v>
       </c>
@@ -21096,7 +21145,7 @@
       </c>
       <c r="D1147" s="4"/>
     </row>
-    <row r="1148" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1148" s="18">
         <v>1147</v>
       </c>
@@ -21168,7 +21217,7 @@
       </c>
       <c r="D1153" s="4"/>
     </row>
-    <row r="1154" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1154" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1154" s="20" t="s">
         <v>2095</v>
       </c>
@@ -21216,7 +21265,7 @@
       </c>
       <c r="D1157" s="4"/>
     </row>
-    <row r="1158" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1158" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1158" s="18">
         <v>1157</v>
       </c>
@@ -21240,7 +21289,7 @@
       </c>
       <c r="D1159" s="4"/>
     </row>
-    <row r="1160" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1160" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1160" s="20" t="s">
         <v>2097</v>
       </c>
@@ -21288,7 +21337,7 @@
       </c>
       <c r="D1163" s="4"/>
     </row>
-    <row r="1164" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1164" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1164" s="18">
         <v>1163</v>
       </c>
@@ -21348,7 +21397,7 @@
       </c>
       <c r="D1168" s="3"/>
     </row>
-    <row r="1169" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1169" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1169" s="20" t="s">
         <v>2102</v>
       </c>
@@ -21396,7 +21445,7 @@
       </c>
       <c r="D1172" s="3"/>
     </row>
-    <row r="1173" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1173" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1173" s="19">
         <v>1172</v>
       </c>
@@ -21468,7 +21517,7 @@
       </c>
       <c r="D1178" s="3"/>
     </row>
-    <row r="1179" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1179" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1179" s="19">
         <v>1178</v>
       </c>
@@ -21528,7 +21577,7 @@
       </c>
       <c r="D1183" s="4"/>
     </row>
-    <row r="1184" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1184" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1184" s="20" t="s">
         <v>2110</v>
       </c>
@@ -21576,7 +21625,7 @@
       </c>
       <c r="D1187" s="4"/>
     </row>
-    <row r="1188" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1188" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1188" s="18">
         <v>1187</v>
       </c>
@@ -21636,7 +21685,7 @@
       </c>
       <c r="D1192" s="3"/>
     </row>
-    <row r="1193" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1193" s="19">
         <v>1192</v>
       </c>
@@ -21660,7 +21709,7 @@
       </c>
       <c r="D1194" s="3"/>
     </row>
-    <row r="1195" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1195" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1195" s="20" t="s">
         <v>2113</v>
       </c>
@@ -21720,7 +21769,7 @@
       </c>
       <c r="D1199" s="4"/>
     </row>
-    <row r="1200" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1200" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1200" s="20" t="s">
         <v>2117</v>
       </c>
@@ -21768,7 +21817,7 @@
       </c>
       <c r="D1203" s="4"/>
     </row>
-    <row r="1204" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1204" s="18">
         <v>1203</v>
       </c>
@@ -21804,7 +21853,7 @@
       </c>
       <c r="D1206" s="3"/>
     </row>
-    <row r="1207" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1207" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1207" s="19">
         <v>1206</v>
       </c>
@@ -21816,7 +21865,7 @@
       </c>
       <c r="D1207" s="4"/>
     </row>
-    <row r="1208" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1208" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1208" s="18">
         <v>1207</v>
       </c>
@@ -21852,7 +21901,7 @@
       </c>
       <c r="D1210" s="3"/>
     </row>
-    <row r="1211" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1211" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1211" s="19">
         <v>1210</v>
       </c>
@@ -21924,7 +21973,7 @@
       </c>
       <c r="D1216" s="3"/>
     </row>
-    <row r="1217" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1217" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1217" s="20" t="s">
         <v>2126</v>
       </c>
@@ -21972,7 +22021,7 @@
       </c>
       <c r="D1220" s="3"/>
     </row>
-    <row r="1221" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1221" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1221" s="19">
         <v>1220</v>
       </c>
@@ -22020,7 +22069,7 @@
       </c>
       <c r="D1224" s="3"/>
     </row>
-    <row r="1225" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1225" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1225" s="19">
         <v>1224</v>
       </c>
@@ -22032,7 +22081,7 @@
       </c>
       <c r="D1225" s="4"/>
     </row>
-    <row r="1226" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1226" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1226" s="20" t="s">
         <v>2127</v>
       </c>
@@ -22044,7 +22093,7 @@
       </c>
       <c r="D1226" s="3"/>
     </row>
-    <row r="1227" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1227" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1227" s="19">
         <v>1226</v>
       </c>
@@ -22104,7 +22153,7 @@
       </c>
       <c r="D1231" s="4"/>
     </row>
-    <row r="1232" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1232" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1232" s="20" t="s">
         <v>2131</v>
       </c>
@@ -22152,7 +22201,7 @@
       </c>
       <c r="D1235" s="4"/>
     </row>
-    <row r="1236" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1236" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1236" s="18">
         <v>1235</v>
       </c>
@@ -22212,7 +22261,7 @@
       </c>
       <c r="D1240" s="3"/>
     </row>
-    <row r="1241" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1241" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1241" s="19">
         <v>1240</v>
       </c>
@@ -22284,7 +22333,7 @@
       </c>
       <c r="D1246" s="3"/>
     </row>
-    <row r="1247" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1247" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1247" s="20" t="s">
         <v>2138</v>
       </c>
@@ -22332,7 +22381,7 @@
       </c>
       <c r="D1250" s="3"/>
     </row>
-    <row r="1251" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1251" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1251" s="19">
         <v>1250</v>
       </c>
@@ -22392,7 +22441,7 @@
       </c>
       <c r="D1255" s="4"/>
     </row>
-    <row r="1256" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1256" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1256" s="18">
         <v>1255</v>
       </c>
@@ -22440,7 +22489,7 @@
       </c>
       <c r="D1259" s="4"/>
     </row>
-    <row r="1260" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1260" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1260" s="20" t="s">
         <v>2143</v>
       </c>
@@ -22488,7 +22537,7 @@
       </c>
       <c r="D1263" s="4"/>
     </row>
-    <row r="1264" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1264" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1264" s="18">
         <v>1263</v>
       </c>
@@ -22560,7 +22609,7 @@
       </c>
       <c r="D1269" s="4"/>
     </row>
-    <row r="1270" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1270" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1270" s="18">
         <v>1269</v>
       </c>
@@ -22620,7 +22669,7 @@
       </c>
       <c r="D1274" s="3"/>
     </row>
-    <row r="1275" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1275" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1275" s="20" t="s">
         <v>2150</v>
       </c>
@@ -22668,7 +22717,7 @@
       </c>
       <c r="D1278" s="3"/>
     </row>
-    <row r="1279" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1279" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1279" s="19">
         <v>1278</v>
       </c>
@@ -22740,7 +22789,7 @@
       </c>
       <c r="D1284" s="3"/>
     </row>
-    <row r="1285" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1285" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1285" s="19">
         <v>1284</v>
       </c>
@@ -22800,7 +22849,7 @@
       </c>
       <c r="D1289" s="4"/>
     </row>
-    <row r="1290" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1290" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1290" s="18">
         <v>1289</v>
       </c>
@@ -22848,7 +22897,7 @@
       </c>
       <c r="D1293" s="4"/>
     </row>
-    <row r="1294" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1294" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1294" s="18">
         <v>1293</v>
       </c>
@@ -22908,7 +22957,7 @@
       </c>
       <c r="D1298" s="3"/>
     </row>
-    <row r="1299" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1299" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1299" s="19">
         <v>1298</v>
       </c>
@@ -22944,7 +22993,7 @@
       </c>
       <c r="D1301" s="4"/>
     </row>
-    <row r="1302" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1302" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1302" s="18">
         <v>1301</v>
       </c>
@@ -23016,7 +23065,7 @@
       </c>
       <c r="D1307" s="4"/>
     </row>
-    <row r="1308" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1308" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1308" s="18">
         <v>1307</v>
       </c>
@@ -23076,7 +23125,7 @@
       </c>
       <c r="D1312" s="3"/>
     </row>
-    <row r="1313" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1313" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1313" s="19">
         <v>1312</v>
       </c>
@@ -23124,7 +23173,7 @@
       </c>
       <c r="D1316" s="3"/>
     </row>
-    <row r="1317" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1317" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1317" s="19">
         <v>1316</v>
       </c>
@@ -23172,7 +23221,7 @@
       </c>
       <c r="D1320" s="3"/>
     </row>
-    <row r="1321" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1321" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1321" s="19">
         <v>1320</v>
       </c>
@@ -23244,7 +23293,7 @@
       </c>
       <c r="D1326" s="3"/>
     </row>
-    <row r="1327" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1327" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1327" s="19">
         <v>1326</v>
       </c>
@@ -23292,7 +23341,7 @@
       </c>
       <c r="D1330" s="3"/>
     </row>
-    <row r="1331" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1331" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1331" s="19">
         <v>1330</v>
       </c>
@@ -23352,7 +23401,7 @@
       </c>
       <c r="D1335" s="4"/>
     </row>
-    <row r="1336" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1336" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1336" s="18">
         <v>1335</v>
       </c>
@@ -23364,7 +23413,7 @@
       </c>
       <c r="D1336" s="3"/>
     </row>
-    <row r="1337" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1337" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1337" s="20" t="s">
         <v>2160</v>
       </c>
@@ -23376,7 +23425,7 @@
       </c>
       <c r="D1337" s="4"/>
     </row>
-    <row r="1338" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1338" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1338" s="18">
         <v>1337</v>
       </c>
@@ -23412,7 +23461,7 @@
       </c>
       <c r="D1340" s="3"/>
     </row>
-    <row r="1341" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1341" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1341" s="19">
         <v>1340</v>
       </c>
@@ -23472,7 +23521,7 @@
       </c>
       <c r="D1345" s="4"/>
     </row>
-    <row r="1346" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1346" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1346" s="18">
         <v>1345</v>
       </c>
@@ -23520,7 +23569,7 @@
       </c>
       <c r="D1349" s="4"/>
     </row>
-    <row r="1350" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1350" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1350" s="18">
         <v>1349</v>
       </c>
@@ -23580,7 +23629,7 @@
       </c>
       <c r="D1354" s="3"/>
     </row>
-    <row r="1355" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1355" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1355" s="19">
         <v>1354</v>
       </c>
@@ -23640,7 +23689,7 @@
       </c>
       <c r="D1359" s="4"/>
     </row>
-    <row r="1360" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1360" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1360" s="18">
         <v>1359</v>
       </c>
@@ -23688,7 +23737,7 @@
       </c>
       <c r="D1363" s="4"/>
     </row>
-    <row r="1364" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1364" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1364" s="18">
         <v>1363</v>
       </c>
@@ -23748,7 +23797,7 @@
       </c>
       <c r="D1368" s="3"/>
     </row>
-    <row r="1369" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1369" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1369" s="19">
         <v>1368</v>
       </c>
@@ -23760,7 +23809,7 @@
       </c>
       <c r="D1369" s="4"/>
     </row>
-    <row r="1370" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1370" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1370" s="20" t="s">
         <v>2165</v>
       </c>
@@ -23772,7 +23821,7 @@
       </c>
       <c r="D1370" s="3"/>
     </row>
-    <row r="1371" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1371" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1371" s="19">
         <v>1370</v>
       </c>
@@ -23808,7 +23857,7 @@
       </c>
       <c r="D1373" s="4"/>
     </row>
-    <row r="1374" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1374" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1374" s="18">
         <v>1373</v>
       </c>
@@ -23856,7 +23905,7 @@
       </c>
       <c r="D1377" s="4"/>
     </row>
-    <row r="1378" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1378" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1378" s="18">
         <v>1377</v>
       </c>
@@ -23928,7 +23977,7 @@
       </c>
       <c r="D1383" s="4"/>
     </row>
-    <row r="1384" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1384" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1384" s="18">
         <v>1383</v>
       </c>
@@ -23940,7 +23989,7 @@
       </c>
       <c r="D1384" s="3"/>
     </row>
-    <row r="1385" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1385" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1385" s="20" t="s">
         <v>2167</v>
       </c>
@@ -23952,7 +24001,7 @@
       </c>
       <c r="D1385" s="4"/>
     </row>
-    <row r="1386" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1386" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1386" s="18">
         <v>1385</v>
       </c>
@@ -23988,7 +24037,7 @@
       </c>
       <c r="D1388" s="3"/>
     </row>
-    <row r="1389" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1389" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1389" s="19">
         <v>1388</v>
       </c>
@@ -24036,7 +24085,7 @@
       </c>
       <c r="D1392" s="3"/>
     </row>
-    <row r="1393" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1393" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1393" s="19">
         <v>1392</v>
       </c>
@@ -24096,7 +24145,7 @@
       </c>
       <c r="D1397" s="4"/>
     </row>
-    <row r="1398" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1398" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1398" s="18">
         <v>1397</v>
       </c>
@@ -24156,7 +24205,7 @@
       </c>
       <c r="D1402" s="3"/>
     </row>
-    <row r="1403" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1403" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1403" s="19">
         <v>1402</v>
       </c>
@@ -24204,7 +24253,7 @@
       </c>
       <c r="D1406" s="3"/>
     </row>
-    <row r="1407" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1407" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1407" s="19">
         <v>1406</v>
       </c>
@@ -24264,7 +24313,7 @@
       </c>
       <c r="D1411" s="4"/>
     </row>
-    <row r="1412" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1412" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1412" s="18">
         <v>1411</v>
       </c>
@@ -24276,7 +24325,7 @@
       </c>
       <c r="D1412" s="3"/>
     </row>
-    <row r="1413" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1413" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1413" s="20" t="s">
         <v>2171</v>
       </c>
@@ -24288,7 +24337,7 @@
       </c>
       <c r="D1413" s="4"/>
     </row>
-    <row r="1414" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1414" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1414" s="18">
         <v>1413</v>
       </c>
@@ -24324,7 +24373,7 @@
       </c>
       <c r="D1416" s="3"/>
     </row>
-    <row r="1417" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1417" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1417" s="19">
         <v>1416</v>
       </c>
@@ -24372,7 +24421,7 @@
       </c>
       <c r="D1420" s="3"/>
     </row>
-    <row r="1421" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1421" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1421" s="19">
         <v>1420</v>
       </c>
@@ -24432,7 +24481,7 @@
       </c>
       <c r="D1425" s="4"/>
     </row>
-    <row r="1426" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1426" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1426" s="18">
         <v>1425</v>
       </c>
@@ -24540,7 +24589,7 @@
       </c>
       <c r="D1434" s="3"/>
     </row>
-    <row r="1435" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1435" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1435" s="19">
         <v>1434</v>
       </c>
@@ -24600,7 +24649,7 @@
       </c>
       <c r="D1439" s="4"/>
     </row>
-    <row r="1440" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1440" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1440" s="18">
         <v>1439</v>
       </c>
@@ -24660,7 +24709,7 @@
       </c>
       <c r="D1444" s="3"/>
     </row>
-    <row r="1445" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1445" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1445" s="19">
         <v>1444</v>
       </c>
@@ -24720,7 +24769,7 @@
       </c>
       <c r="D1449" s="3"/>
     </row>
-    <row r="1450" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1450" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1450" s="18">
         <v>1449</v>
       </c>
@@ -24768,7 +24817,7 @@
       </c>
       <c r="D1453" s="3"/>
     </row>
-    <row r="1454" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1454" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1454" s="18">
         <v>1453</v>
       </c>
@@ -24781,245 +24830,389 @@
       <c r="D1454" s="4"/>
     </row>
     <row r="1455" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1455" s="19" t="s">
-        <v>1462</v>
+      <c r="A1455" s="18" t="s">
+        <v>2221</v>
       </c>
       <c r="B1455" s="14" t="s">
-        <v>1463</v>
-      </c>
-      <c r="C1455" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1455" s="3"/>
+        <v>2202</v>
+      </c>
+      <c r="C1455" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1455" s="4"/>
     </row>
     <row r="1456" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1456" s="18" t="s">
-        <v>1464</v>
-      </c>
-      <c r="B1456" s="13" t="s">
-        <v>1465</v>
+      <c r="A1456" s="18">
+        <v>1455</v>
+      </c>
+      <c r="B1456" s="14" t="s">
+        <v>2203</v>
       </c>
       <c r="C1456" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1456" s="4"/>
+      <c r="D1456" s="3"/>
     </row>
     <row r="1457" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1457" s="19" t="s">
-        <v>1466</v>
+      <c r="A1457" s="18">
+        <v>1456</v>
       </c>
       <c r="B1457" s="14" t="s">
-        <v>1467</v>
-      </c>
-      <c r="C1457" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1457" s="3"/>
-    </row>
-    <row r="1458" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1458" s="18" t="s">
-        <v>1468</v>
-      </c>
-      <c r="B1458" s="13" t="s">
-        <v>1469</v>
+        <v>2204</v>
+      </c>
+      <c r="C1457" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1457" s="4"/>
+    </row>
+    <row r="1458" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1458" s="18">
+        <v>1457</v>
+      </c>
+      <c r="B1458" s="14" t="s">
+        <v>2205</v>
       </c>
       <c r="C1458" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1458" s="4"/>
-    </row>
-    <row r="1459" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1459" s="19" t="s">
-        <v>1470</v>
+        <v>7</v>
+      </c>
+      <c r="D1458" s="3"/>
+    </row>
+    <row r="1459" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1459" s="18">
+        <v>1458</v>
       </c>
       <c r="B1459" s="14" t="s">
-        <v>1471</v>
-      </c>
-      <c r="C1459" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1459" s="3"/>
+        <v>2206</v>
+      </c>
+      <c r="C1459" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1459" s="4"/>
     </row>
     <row r="1460" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1460" s="18" t="s">
+        <v>2220</v>
+      </c>
+      <c r="B1460" s="14" t="s">
+        <v>2207</v>
+      </c>
+      <c r="C1460" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1460" s="3"/>
+    </row>
+    <row r="1461" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1461" s="18">
+        <v>1460</v>
+      </c>
+      <c r="B1461" s="14" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C1461" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1462" s="18">
+        <v>1461</v>
+      </c>
+      <c r="B1462" s="14" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C1462" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1463" s="18">
+        <v>1462</v>
+      </c>
+      <c r="B1463" s="14" t="s">
+        <v>2210</v>
+      </c>
+      <c r="C1463" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1464" s="18">
+        <v>1463</v>
+      </c>
+      <c r="B1464" s="14" t="s">
+        <v>2211</v>
+      </c>
+      <c r="C1464" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1465" s="18">
+        <v>1464</v>
+      </c>
+      <c r="B1465" s="14" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C1465" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1465" s="2"/>
+    </row>
+    <row r="1466" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1466" s="18">
+        <v>1465</v>
+      </c>
+      <c r="B1466" s="14" t="s">
+        <v>2213</v>
+      </c>
+      <c r="C1466" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1466" s="3"/>
+    </row>
+    <row r="1467" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1467" s="18">
+        <v>1466</v>
+      </c>
+      <c r="B1467" s="14" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C1467" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1467" s="4"/>
+    </row>
+    <row r="1468" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1468" s="18">
+        <v>1467</v>
+      </c>
+      <c r="B1468" s="14" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C1468" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1468" s="3"/>
+    </row>
+    <row r="1469" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1469" s="18" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B1469" s="14" t="s">
+        <v>2216</v>
+      </c>
+      <c r="C1469" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1469" s="3"/>
+    </row>
+    <row r="1470" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1470" s="18" t="s">
+        <v>2218</v>
+      </c>
+      <c r="B1470" s="14" t="s">
+        <v>2217</v>
+      </c>
+      <c r="C1470" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1470" s="4"/>
+    </row>
+    <row r="1471" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1471" s="19" t="s">
+        <v>1462</v>
+      </c>
+      <c r="B1471" s="14" t="s">
+        <v>1463</v>
+      </c>
+      <c r="C1471" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1471" s="3"/>
+    </row>
+    <row r="1472" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1472" s="18" t="s">
+        <v>1464</v>
+      </c>
+      <c r="B1472" s="13" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C1472" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1472" s="4"/>
+    </row>
+    <row r="1473" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1473" s="19" t="s">
+        <v>1466</v>
+      </c>
+      <c r="B1473" s="14" t="s">
+        <v>1467</v>
+      </c>
+      <c r="C1473" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1473" s="3"/>
+    </row>
+    <row r="1474" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1474" s="18" t="s">
+        <v>1468</v>
+      </c>
+      <c r="B1474" s="13" t="s">
+        <v>1469</v>
+      </c>
+      <c r="C1474" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1474" s="4"/>
+    </row>
+    <row r="1475" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1475" s="19" t="s">
+        <v>1470</v>
+      </c>
+      <c r="B1475" s="14" t="s">
+        <v>1471</v>
+      </c>
+      <c r="C1475" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1475" s="3"/>
+    </row>
+    <row r="1476" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1476" s="18" t="s">
         <v>1472</v>
       </c>
-      <c r="B1460" s="13" t="s">
+      <c r="B1476" s="13" t="s">
         <v>1473</v>
       </c>
-      <c r="C1460" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1460" s="4"/>
-    </row>
-    <row r="1461" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1461" s="19" t="s">
+      <c r="C1476" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1476" s="4"/>
+    </row>
+    <row r="1477" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1477" s="19" t="s">
         <v>1474</v>
       </c>
-      <c r="B1461" s="14" t="s">
+      <c r="B1477" s="14" t="s">
         <v>1475</v>
       </c>
-      <c r="C1461" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1461" s="3"/>
-    </row>
-    <row r="1462" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1462" s="18" t="s">
+      <c r="C1477" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1477" s="3"/>
+    </row>
+    <row r="1478" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1478" s="18" t="s">
         <v>1476</v>
       </c>
-      <c r="B1462" s="13" t="s">
+      <c r="B1478" s="13" t="s">
         <v>1477</v>
       </c>
-      <c r="C1462" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="1463" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1463" s="19" t="s">
+      <c r="C1478" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1478" s="4"/>
+    </row>
+    <row r="1479" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1479" s="19" t="s">
         <v>1478</v>
       </c>
-      <c r="B1463" s="14" t="s">
+      <c r="B1479" s="14" t="s">
         <v>1479</v>
       </c>
-      <c r="C1463" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1464" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1464" s="18" t="s">
+      <c r="C1479" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1479" s="3"/>
+    </row>
+    <row r="1480" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1480" s="18" t="s">
         <v>1480</v>
       </c>
-      <c r="B1464" s="13" t="s">
+      <c r="B1480" s="13" t="s">
         <v>1481</v>
       </c>
-      <c r="C1464" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="1465" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1465" s="19" t="s">
+      <c r="C1480" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1480" s="4"/>
+    </row>
+    <row r="1481" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1481" s="19" t="s">
         <v>1482</v>
       </c>
-      <c r="B1465" s="14" t="s">
+      <c r="B1481" s="14" t="s">
         <v>1483</v>
       </c>
-      <c r="C1465" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="1466" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1466" s="18" t="s">
+      <c r="C1481" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1481" s="3"/>
+    </row>
+    <row r="1482" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1482" s="18" t="s">
         <v>1484</v>
       </c>
-      <c r="B1466" s="13" t="s">
+      <c r="B1482" s="13" t="s">
         <v>1485</v>
       </c>
-      <c r="C1466" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1466" s="2"/>
-    </row>
-    <row r="1467" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1467" s="19" t="s">
+      <c r="C1482" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1482" s="4"/>
+    </row>
+    <row r="1483" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1483" s="19" t="s">
         <v>1486</v>
       </c>
-      <c r="B1467" s="14" t="s">
+      <c r="B1483" s="14" t="s">
         <v>1487</v>
       </c>
-      <c r="C1467" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1467" s="3"/>
-    </row>
-    <row r="1468" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1468" s="18" t="s">
+      <c r="C1483" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1483" s="3"/>
+    </row>
+    <row r="1484" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1484" s="18" t="s">
         <v>1488</v>
       </c>
-      <c r="B1468" s="13" t="s">
+      <c r="B1484" s="13" t="s">
         <v>1489</v>
       </c>
-      <c r="C1468" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1468" s="4"/>
-    </row>
-    <row r="1469" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1469" s="19" t="s">
+      <c r="C1484" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1484" s="4"/>
+    </row>
+    <row r="1485" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1485" s="19" t="s">
         <v>1490</v>
       </c>
-      <c r="B1469" s="14" t="s">
+      <c r="B1485" s="14" t="s">
         <v>1491</v>
       </c>
-      <c r="C1469" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1469" s="3"/>
-    </row>
-    <row r="1470" spans="1:5" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1470" s="18" t="s">
+      <c r="C1485" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1485" s="3"/>
+    </row>
+    <row r="1486" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1486" s="18" t="s">
         <v>1492</v>
       </c>
-      <c r="B1470" s="13" t="s">
+      <c r="B1486" s="13" t="s">
         <v>1493</v>
       </c>
-      <c r="C1470" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1470" s="4"/>
-    </row>
-    <row r="1471" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1471" s="3"/>
-    </row>
-    <row r="1472" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1472" s="4"/>
-    </row>
-    <row r="1473" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1473" s="3"/>
-    </row>
-    <row r="1474" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1474" s="4"/>
-    </row>
-    <row r="1475" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1475" s="3"/>
-    </row>
-    <row r="1476" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1476" s="4"/>
-    </row>
-    <row r="1477" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1477" s="3"/>
-    </row>
-    <row r="1478" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1478" s="4"/>
-    </row>
-    <row r="1479" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1479" s="3"/>
-    </row>
-    <row r="1480" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1480" s="4"/>
-    </row>
-    <row r="1481" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1481" s="3"/>
-    </row>
-    <row r="1482" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1482" s="4"/>
-    </row>
-    <row r="1483" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1483" s="3"/>
-    </row>
-    <row r="1484" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1484" s="4"/>
-    </row>
-    <row r="1485" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1485" s="3"/>
-    </row>
-    <row r="1486" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1486" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E1486" s="4"/>
     </row>
-    <row r="1487" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1487" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1487" s="3"/>
     </row>
-    <row r="1488" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1488" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1488" s="4"/>
     </row>
     <row r="1489" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25277,15 +25470,15 @@
     <row r="1573" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1573" s="3"/>
     </row>
-    <row r="1574" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1574" s="4"/>
-    </row>
-    <row r="1575" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1575" s="3"/>
-    </row>
-    <row r="1579" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1577" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1578" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1578" s="2"/>
+    </row>
+    <row r="1579" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1579" s="3"/>
+    </row>
     <row r="1580" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1580" s="2"/>
+      <c r="E1580" s="4"/>
     </row>
     <row r="1581" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1581" s="3"/>
@@ -25503,24 +25696,11 @@
     <row r="1652" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1652" s="4"/>
     </row>
-    <row r="1653" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1653" s="3"/>
-    </row>
-    <row r="1654" spans="5:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1654" s="4"/>
-    </row>
-    <row r="1655" spans="5:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1655" s="7"/>
+    <row r="1653" spans="5:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1653" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D1470" xr:uid="{AA2808F7-94D6-4788-B7C2-AA20F53DB078}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="中等"/>
-        <filter val="简单"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:D1486" xr:uid="{AA2808F7-94D6-4788-B7C2-AA20F53DB078}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -26969,22 +27149,22 @@
     <hyperlink ref="B1444" r:id="rId1442" display="https://leetcode-cn.com/problems/minimum-time-to-collect-all-apples-in-a-tree" xr:uid="{26C99996-EF95-41E0-AC28-7ACC44E27D73}"/>
     <hyperlink ref="B1445" r:id="rId1443" display="https://leetcode-cn.com/problems/number-of-ways-of-cutting-a-pizza" xr:uid="{399F5F11-C4D3-4E4E-B284-B30210CDDC71}"/>
     <hyperlink ref="B1446" r:id="rId1444" display="https://leetcode-cn.com/problems/apples-oranges" xr:uid="{4EA7D115-D121-4BCC-99F9-CD083ECA09C8}"/>
-    <hyperlink ref="B1455" r:id="rId1445" display="https://leetcode-cn.com/problems/guess-numbers" xr:uid="{69087C18-FA9C-40B3-AF17-043A96496574}"/>
-    <hyperlink ref="B1456" r:id="rId1446" display="https://leetcode-cn.com/problems/deep-dark-fraction" xr:uid="{114BD6E4-01F4-4B7F-A39C-5F005CAF496A}"/>
-    <hyperlink ref="B1457" r:id="rId1447" display="https://leetcode-cn.com/problems/programmable-robot" xr:uid="{5AB364F8-5855-443C-BF25-0AAD6261A637}"/>
-    <hyperlink ref="B1458" r:id="rId1448" display="https://leetcode-cn.com/problems/broken-board-dominoes" xr:uid="{F4A53F44-AA5A-483F-9C5B-6D3834B9E37D}"/>
-    <hyperlink ref="B1459" r:id="rId1449" display="https://leetcode-cn.com/problems/coin-bonus" xr:uid="{F83EFE64-1C11-462B-BAED-11146005F3A9}"/>
-    <hyperlink ref="B1460" r:id="rId1450" display="https://leetcode-cn.com/problems/na-ying-bi" xr:uid="{A76A66F5-E848-44C7-B3DA-9E7DD8A8C044}"/>
-    <hyperlink ref="B1461" r:id="rId1451" display="https://leetcode-cn.com/problems/chuan-di-xin-xi" xr:uid="{92733632-EA18-4A8A-8FF7-FF778E2296C5}"/>
-    <hyperlink ref="B1462" r:id="rId1452" display="https://leetcode-cn.com/problems/ju-qing-hong-fa-shi-jian" xr:uid="{180831C5-B17B-47C8-96E5-BD6168FE5F93}"/>
-    <hyperlink ref="B1463" r:id="rId1453" display="https://leetcode-cn.com/problems/zui-xiao-tiao-yue-ci-shu" xr:uid="{43E72EB8-A0E0-4323-A2F1-445E96866D3B}"/>
-    <hyperlink ref="B1464" r:id="rId1454" display="https://leetcode-cn.com/problems/er-cha-shu-ren-wu-diao-du" xr:uid="{362A3653-8A6F-4C30-AC3C-F3F60DB66B09}"/>
-    <hyperlink ref="B1465" r:id="rId1455" display="https://leetcode-cn.com/problems/qi-wang-ge-shu-tong-ji" xr:uid="{9CA6765F-77AE-48E9-96CE-211D96171ADE}"/>
-    <hyperlink ref="B1466" r:id="rId1456" display="https://leetcode-cn.com/problems/xiao-zhang-shua-ti-ji-hua" xr:uid="{64E0E543-DA06-49F5-ABA0-93AFBC6AE494}"/>
-    <hyperlink ref="B1467" r:id="rId1457" display="https://leetcode-cn.com/problems/xun-bao" xr:uid="{D7038CDA-E564-465B-9BE5-F87650501858}"/>
-    <hyperlink ref="B1468" r:id="rId1458" display="https://leetcode-cn.com/problems/qie-fen-shu-zu" xr:uid="{9812E229-7AF3-488C-A910-903A3CEB1C27}"/>
-    <hyperlink ref="B1469" r:id="rId1459" display="https://leetcode-cn.com/problems/you-le-yuan-de-mi-gong" xr:uid="{83653B12-D1CB-40CE-85A9-7080941CA862}"/>
-    <hyperlink ref="B1470" r:id="rId1460" display="https://leetcode-cn.com/problems/you-le-yuan-de-you-lan-ji-hua" xr:uid="{FEFCF74B-B5BC-42D7-88BE-EFDE007579B8}"/>
+    <hyperlink ref="B1471" r:id="rId1445" display="https://leetcode-cn.com/problems/guess-numbers" xr:uid="{69087C18-FA9C-40B3-AF17-043A96496574}"/>
+    <hyperlink ref="B1472" r:id="rId1446" display="https://leetcode-cn.com/problems/deep-dark-fraction" xr:uid="{114BD6E4-01F4-4B7F-A39C-5F005CAF496A}"/>
+    <hyperlink ref="B1473" r:id="rId1447" display="https://leetcode-cn.com/problems/programmable-robot" xr:uid="{5AB364F8-5855-443C-BF25-0AAD6261A637}"/>
+    <hyperlink ref="B1474" r:id="rId1448" display="https://leetcode-cn.com/problems/broken-board-dominoes" xr:uid="{F4A53F44-AA5A-483F-9C5B-6D3834B9E37D}"/>
+    <hyperlink ref="B1475" r:id="rId1449" display="https://leetcode-cn.com/problems/coin-bonus" xr:uid="{F83EFE64-1C11-462B-BAED-11146005F3A9}"/>
+    <hyperlink ref="B1476" r:id="rId1450" display="https://leetcode-cn.com/problems/na-ying-bi" xr:uid="{A76A66F5-E848-44C7-B3DA-9E7DD8A8C044}"/>
+    <hyperlink ref="B1477" r:id="rId1451" display="https://leetcode-cn.com/problems/chuan-di-xin-xi" xr:uid="{92733632-EA18-4A8A-8FF7-FF778E2296C5}"/>
+    <hyperlink ref="B1478" r:id="rId1452" display="https://leetcode-cn.com/problems/ju-qing-hong-fa-shi-jian" xr:uid="{180831C5-B17B-47C8-96E5-BD6168FE5F93}"/>
+    <hyperlink ref="B1479" r:id="rId1453" display="https://leetcode-cn.com/problems/zui-xiao-tiao-yue-ci-shu" xr:uid="{43E72EB8-A0E0-4323-A2F1-445E96866D3B}"/>
+    <hyperlink ref="B1480" r:id="rId1454" display="https://leetcode-cn.com/problems/er-cha-shu-ren-wu-diao-du" xr:uid="{362A3653-8A6F-4C30-AC3C-F3F60DB66B09}"/>
+    <hyperlink ref="B1481" r:id="rId1455" display="https://leetcode-cn.com/problems/qi-wang-ge-shu-tong-ji" xr:uid="{9CA6765F-77AE-48E9-96CE-211D96171ADE}"/>
+    <hyperlink ref="B1482" r:id="rId1456" display="https://leetcode-cn.com/problems/xiao-zhang-shua-ti-ji-hua" xr:uid="{64E0E543-DA06-49F5-ABA0-93AFBC6AE494}"/>
+    <hyperlink ref="B1483" r:id="rId1457" display="https://leetcode-cn.com/problems/xun-bao" xr:uid="{D7038CDA-E564-465B-9BE5-F87650501858}"/>
+    <hyperlink ref="B1484" r:id="rId1458" display="https://leetcode-cn.com/problems/qie-fen-shu-zu" xr:uid="{9812E229-7AF3-488C-A910-903A3CEB1C27}"/>
+    <hyperlink ref="B1485" r:id="rId1459" display="https://leetcode-cn.com/problems/you-le-yuan-de-mi-gong" xr:uid="{83653B12-D1CB-40CE-85A9-7080941CA862}"/>
+    <hyperlink ref="B1486" r:id="rId1460" display="https://leetcode-cn.com/problems/you-le-yuan-de-you-lan-ji-hua" xr:uid="{FEFCF74B-B5BC-42D7-88BE-EFDE007579B8}"/>
     <hyperlink ref="B1447" r:id="rId1461" display="https://leetcode-cn.com/problems/consecutive-characters" xr:uid="{CF4321A1-6252-461C-9B12-23ED59AABFE8}"/>
     <hyperlink ref="B1448" r:id="rId1462" display="https://leetcode-cn.com/problems/simplified-fractions" xr:uid="{A5D3E664-F486-4799-AA04-2AE2496E698E}"/>
     <hyperlink ref="B1449" r:id="rId1463" display="https://leetcode-cn.com/problems/count-good-nodes-in-binary-tree" xr:uid="{EA7C1C01-25CB-4B93-B7B6-2D71007B3607}"/>
@@ -26993,158 +27173,296 @@
     <hyperlink ref="B1452" r:id="rId1466" display="https://leetcode-cn.com/problems/rearrange-words-in-a-sentence" xr:uid="{5664D24C-330E-46B0-B92C-81004FA950EF}"/>
     <hyperlink ref="B1453" r:id="rId1467" display="https://leetcode-cn.com/problems/people-whose-list-of-favorite-companies-is-not-a-subset-of-another-list" xr:uid="{A93AD622-DE4C-48B0-9FBA-7146E9A9BB19}"/>
     <hyperlink ref="B1454" r:id="rId1468" display="https://leetcode-cn.com/problems/maximum-number-of-darts-inside-of-a-circular-dartboard" xr:uid="{41DC97E6-01F8-4124-A47D-578AEAFFE838}"/>
+    <hyperlink ref="B1455" r:id="rId1469" display="https://leetcode-cn.com/problems/active-users" xr:uid="{54F5D417-1CA6-4BD5-A396-87B16007D290}"/>
+    <hyperlink ref="B1456" r:id="rId1470" display="https://leetcode-cn.com/problems/check-if-a-word-occurs-as-a-prefix-of-any-word-in-a-sentence" xr:uid="{C53CC06E-5412-4C68-AC73-28C3E8E6811A}"/>
+    <hyperlink ref="B1457" r:id="rId1471" display="https://leetcode-cn.com/problems/maximum-number-of-vowels-in-a-substring-of-given-length" xr:uid="{D16EA7AF-F62F-4095-9E46-B304570910FF}"/>
+    <hyperlink ref="B1458" r:id="rId1472" display="https://leetcode-cn.com/problems/pseudo-palindromic-paths-in-a-binary-tree" xr:uid="{72DF2597-9992-42E8-9FA6-3B635D878B2F}"/>
+    <hyperlink ref="B1459" r:id="rId1473" display="https://leetcode-cn.com/problems/max-dot-product-of-two-subsequences" xr:uid="{B25D4947-BA87-44E1-BE52-6D5DC4A6264D}"/>
+    <hyperlink ref="B1460" r:id="rId1474" display="https://leetcode-cn.com/problems/rectangles-area" xr:uid="{BCB05ED1-19F6-42BF-9474-3FFE55B33428}"/>
+    <hyperlink ref="B1461" r:id="rId1475" display="https://leetcode-cn.com/problems/make-two-arrays-equal-by-reversing-sub-arrays" xr:uid="{2CB7D8D4-9B1E-412F-AE31-B3D65678E710}"/>
+    <hyperlink ref="B1462" r:id="rId1476" display="https://leetcode-cn.com/problems/check-if-a-string-contains-all-binary-codes-of-size-k" xr:uid="{A152DB91-DEF2-49BE-A210-E56A69E56BCA}"/>
+    <hyperlink ref="B1463" r:id="rId1477" display="https://leetcode-cn.com/problems/course-schedule-iv" xr:uid="{7984C0B0-857D-4D2B-A546-AFA1E92EC9C5}"/>
+    <hyperlink ref="B1464" r:id="rId1478" display="https://leetcode-cn.com/problems/cherry-pickup-ii" xr:uid="{7327CB5B-E649-46A8-B1B9-B9C713F9AD4A}"/>
+    <hyperlink ref="B1465" r:id="rId1479" display="https://leetcode-cn.com/problems/maximum-product-of-two-elements-in-an-array" xr:uid="{554DC431-84AC-4AF4-AD13-DDE3813173AD}"/>
+    <hyperlink ref="B1466" r:id="rId1480" display="https://leetcode-cn.com/problems/maximum-area-of-a-piece-of-cake-after-horizontal-and-vertical-cuts" xr:uid="{582333F7-CC54-47DB-A752-354790FF47CF}"/>
+    <hyperlink ref="B1467" r:id="rId1481" display="https://leetcode-cn.com/problems/reorder-routes-to-make-all-paths-lead-to-the-city-zero" xr:uid="{1E0E5379-73FC-466B-AEBE-663D2324F1EE}"/>
+    <hyperlink ref="B1468" r:id="rId1482" display="https://leetcode-cn.com/problems/probability-of-a-two-boxes-having-the-same-number-of-distinct-balls" xr:uid="{A1E9C98B-76C7-4D4C-B60A-739959D5E001}"/>
+    <hyperlink ref="B1470" r:id="rId1483" display="https://leetcode-cn.com/problems/find-all-the-lonely-nodes" xr:uid="{028A4BFB-CBB9-4EB3-8262-5F5D20D3ABFE}"/>
+    <hyperlink ref="B1469" r:id="rId1484" display="https://leetcode-cn.com/problems/calculate-salaries" xr:uid="{9038CFCF-8600-427F-8E5D-CCF1CB281983}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId1469"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId1485"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD289D6F-A9EC-4855-93D2-FF7CAFD43BD4}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B2" sqref="B2:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="27">
-        <v>1445</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>2189</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>7</v>
-      </c>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="E1" s="21"/>
     </row>
-    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27">
-        <v>1446</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>2181</v>
-      </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="30"/>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23">
+        <v>1453</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>2188</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="23">
-        <v>1447</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>2182</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="25"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="36">
+        <v>1454</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>2202</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27">
-        <v>1448</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>2183</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="30"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="23">
+        <v>1455</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>2203</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="31"/>
-      <c r="B5" s="23">
-        <v>1449</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>2184</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="25"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26">
+        <v>1456</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>2204</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27">
-        <v>1450</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>2185</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="30"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="23">
+        <v>1457</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>2205</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="23">
-        <v>1451</v>
-      </c>
-      <c r="C7" s="22" t="s">
-        <v>2186</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="25"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="26">
+        <v>1458</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>2206</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27">
-        <v>1452</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>2187</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="30"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="37">
+        <v>1459</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>2207</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35">
-        <v>1453</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>2188</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="21"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26">
+        <v>1460</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>2208</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="28"/>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="23">
+        <v>1461</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>2209</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="24"/>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26">
+        <v>1462</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>2210</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="28"/>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="23">
+        <v>1463</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>2211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="24"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26">
+        <v>1464</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>2212</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="28"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="23">
+        <v>1465</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>2213</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="24"/>
+    </row>
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26">
+        <v>1466</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>2214</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="28"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31">
+        <v>1467</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>2215</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="36">
+        <v>1468</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>2216</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39">
+        <v>1469</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>2217</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:D2"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://leetcode-cn.com/problems/consecutive-characters" xr:uid="{B73FBE0D-DA7F-436B-9AB8-9481198B04B4}"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://leetcode-cn.com/problems/simplified-fractions" xr:uid="{638D7FEE-4EE4-4A76-94E8-1E50DDF25FDE}"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://leetcode-cn.com/problems/count-good-nodes-in-binary-tree" xr:uid="{990C7B67-64BE-414A-A005-664BD738A5AF}"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://leetcode-cn.com/problems/form-largest-integer-with-digits-that-add-up-to-target" xr:uid="{A4569765-BBBB-4D94-BC70-7AD1404E2384}"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://leetcode-cn.com/problems/number-of-students-doing-homework-at-a-given-time" xr:uid="{6734DDEC-1AB4-4F0E-B6BB-D057BF4FC803}"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://leetcode-cn.com/problems/rearrange-words-in-a-sentence" xr:uid="{BA63C63B-AA70-4BBF-AADB-437202138CA2}"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://leetcode-cn.com/problems/people-whose-list-of-favorite-companies-is-not-a-subset-of-another-list" xr:uid="{664FA6E3-AE26-4641-89E6-803C3FC4539A}"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://leetcode-cn.com/problems/maximum-number-of-darts-inside-of-a-circular-dartboard" xr:uid="{45C4C5FD-E0E6-4A1F-B042-E6F4929F3297}"/>
-    <hyperlink ref="C1" r:id="rId9" display="https://leetcode-cn.com/problems/apples-oranges" xr:uid="{97FB82E2-EDB0-4C25-B00C-2045AAE46BBD}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://leetcode-cn.com/problems/active-users" xr:uid="{8AAFF00E-F6D5-447B-95E8-12B63F9FE39D}"/>
+    <hyperlink ref="C4" r:id="rId2" display="https://leetcode-cn.com/problems/check-if-a-word-occurs-as-a-prefix-of-any-word-in-a-sentence" xr:uid="{21B714EA-1196-40F4-A6EC-A62FA950C8EC}"/>
+    <hyperlink ref="C5" r:id="rId3" display="https://leetcode-cn.com/problems/maximum-number-of-vowels-in-a-substring-of-given-length" xr:uid="{9913D8DB-788C-4056-AFE5-E55E9B32A7F4}"/>
+    <hyperlink ref="C6" r:id="rId4" display="https://leetcode-cn.com/problems/pseudo-palindromic-paths-in-a-binary-tree" xr:uid="{80C42D78-6277-413C-B37A-9E8A2C712DA2}"/>
+    <hyperlink ref="C7" r:id="rId5" display="https://leetcode-cn.com/problems/max-dot-product-of-two-subsequences" xr:uid="{C5AE739B-8470-45E2-8AD5-DF9B41129184}"/>
+    <hyperlink ref="C8" r:id="rId6" display="https://leetcode-cn.com/problems/rectangles-area" xr:uid="{3B2A8BD9-3AF7-40E4-BB9D-0D496713CF2D}"/>
+    <hyperlink ref="C9" r:id="rId7" display="https://leetcode-cn.com/problems/make-two-arrays-equal-by-reversing-sub-arrays" xr:uid="{103177AF-CD75-443C-9968-C4D6FCC384AD}"/>
+    <hyperlink ref="C10" r:id="rId8" display="https://leetcode-cn.com/problems/check-if-a-string-contains-all-binary-codes-of-size-k" xr:uid="{6435EEDD-4669-4F26-B013-A979FB3DDD3B}"/>
+    <hyperlink ref="C11" r:id="rId9" display="https://leetcode-cn.com/problems/course-schedule-iv" xr:uid="{9679AF77-2612-4F0E-A516-0EF8735CDD61}"/>
+    <hyperlink ref="C12" r:id="rId10" display="https://leetcode-cn.com/problems/cherry-pickup-ii" xr:uid="{7284B984-6B9D-45BB-819C-4E86591A390F}"/>
+    <hyperlink ref="C13" r:id="rId11" display="https://leetcode-cn.com/problems/maximum-product-of-two-elements-in-an-array" xr:uid="{CFD2C20F-E055-4926-96CF-F94DC5FD5E9B}"/>
+    <hyperlink ref="C14" r:id="rId12" display="https://leetcode-cn.com/problems/maximum-area-of-a-piece-of-cake-after-horizontal-and-vertical-cuts" xr:uid="{E2F1F5A7-6A3C-48E5-A67B-63B5FC2A9234}"/>
+    <hyperlink ref="C15" r:id="rId13" display="https://leetcode-cn.com/problems/reorder-routes-to-make-all-paths-lead-to-the-city-zero" xr:uid="{C1521F76-AC5C-4792-A9BF-1C64372FF864}"/>
+    <hyperlink ref="C16" r:id="rId14" display="https://leetcode-cn.com/problems/probability-of-a-two-boxes-having-the-same-number-of-distinct-balls" xr:uid="{AFAFD077-657D-47ED-BD4B-D37327D99FBF}"/>
+    <hyperlink ref="C2" r:id="rId15" display="https://leetcode-cn.com/problems/maximum-number-of-darts-inside-of-a-circular-dartboard" xr:uid="{77EFA145-2850-4ECB-85A6-6DFF9A25C79C}"/>
+    <hyperlink ref="C19" r:id="rId16" display="https://leetcode-cn.com/problems/find-all-the-lonely-nodes" xr:uid="{C02EA5AA-BE78-4F15-85DE-E667526F2E75}"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://leetcode-cn.com/problems/calculate-salaries" xr:uid="{47E9AFA0-347B-40C5-B8FD-BDD3802F9310}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -27165,11 +27483,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1494</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -28525,7 +28843,7 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:A1048576"/>
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28537,11 +28855,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>1710</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>

</xml_diff>

<commit_message>
add problem 2(6th self done)
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D94437E-22F5-4133-9D7C-F3C4FF73DAF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44AA8F62-7BD3-47CD-B354-FAD519343A19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1290" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="2223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3947" uniqueCount="2224">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -6703,6 +6703,9 @@
   </si>
   <si>
     <t>2020.6.5(slef5)</t>
+  </si>
+  <si>
+    <t>2020.6.6(self6)</t>
   </si>
 </sst>
 </file>
@@ -7301,7 +7304,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7359,7 +7362,9 @@
       <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4" t="s">
+        <v>2223</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18">

</xml_diff>

<commit_message>
add lcci 01.07 & 01.08
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D659B32E-3BBD-4879-976E-13DDA53B469D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0DD263-5922-408E-B54B-5D765E6CBB46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1650" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="4575" windowWidth="28800" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4322" uniqueCount="2499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="2500">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -7532,6 +7532,9 @@
   </si>
   <si>
     <t>2020.6.10</t>
+  </si>
+  <si>
+    <t>2020.6.11(self)</t>
   </si>
 </sst>
 </file>
@@ -8132,7 +8135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36439EE-948F-4B95-AA31-6B4987F28A76}">
   <dimension ref="A1:E1653"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
@@ -29966,8 +29969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A56D5E7-551D-4DA8-94DC-D98ED60B1AEE}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30080,6 +30083,9 @@
       <c r="C10" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D10" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -30090,6 +30096,9 @@
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2499</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add problem 5 & 15 & 24 & 153
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0DD263-5922-408E-B54B-5D765E6CBB46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172C8891-FA72-4034-97CF-BE9D5397D3BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="4575" windowWidth="28800" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2625" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4324" uniqueCount="2500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4328" uniqueCount="2502">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -7535,6 +7535,12 @@
   </si>
   <si>
     <t>2020.6.11(self)</t>
+  </si>
+  <si>
+    <t>2020.6.12</t>
+  </si>
+  <si>
+    <t>2020.5.10</t>
   </si>
 </sst>
 </file>
@@ -8135,9 +8141,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36439EE-948F-4B95-AA31-6B4987F28A76}">
   <dimension ref="A1:E1653"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8233,7 +8239,9 @@
       <c r="C7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>2500</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
@@ -8355,7 +8363,9 @@
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>2500</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
@@ -8467,7 +8477,9 @@
       <c r="C26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="s">
+        <v>2501</v>
+      </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
@@ -10039,7 +10051,9 @@
       <c r="C154" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D154" s="3"/>
+      <c r="D154" s="3" t="s">
+        <v>2499</v>
+      </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="19">
@@ -29969,7 +29983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A56D5E7-551D-4DA8-94DC-D98ED60B1AEE}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add problem 225 & 232& 494 & 133
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AC856-303D-4162-BF61-0E78A7AD2FC5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B39DA8-FA3C-4E9F-AE11-7444F7E2DA69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="945" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="450" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -16,8 +16,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode 题目'!$A$2:$D$1486</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$4:$D$137</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">剑指Offer!$A$3:$D$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">程序员面试题金典!$A$3:$D$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">剑指Offer!$A$2:$D$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">程序员面试题金典!$A$2:$D$111</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4337" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4341" uniqueCount="2505">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -7547,6 +7547,9 @@
   </si>
   <si>
     <t>2020.6.14</t>
+  </si>
+  <si>
+    <t>2020.6.15</t>
   </si>
 </sst>
 </file>
@@ -8145,11 +8148,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36439EE-948F-4B95-AA31-6B4987F28A76}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E1653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D233" sqref="D233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8183,7 +8187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18">
         <v>1</v>
       </c>
@@ -8197,7 +8201,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>2</v>
       </c>
@@ -8235,7 +8239,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
         <v>5</v>
       </c>
@@ -8345,7 +8349,7 @@
       </c>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>14</v>
       </c>
@@ -8359,7 +8363,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18">
         <v>15</v>
       </c>
@@ -8409,7 +8413,7 @@
       </c>
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>19</v>
       </c>
@@ -8423,7 +8427,7 @@
         <v>2197</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>20</v>
       </c>
@@ -8437,7 +8441,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>21</v>
       </c>
@@ -8475,7 +8479,7 @@
       </c>
       <c r="D25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>24</v>
       </c>
@@ -8489,7 +8493,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18">
         <v>26</v>
       </c>
@@ -8503,7 +8507,7 @@
         <v>2189</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>27</v>
       </c>
@@ -8517,7 +8521,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18">
         <v>28</v>
       </c>
@@ -8603,7 +8607,7 @@
       </c>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>35</v>
       </c>
@@ -8833,7 +8837,7 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>54</v>
       </c>
@@ -8859,7 +8863,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>56</v>
       </c>
@@ -8921,7 +8925,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18">
         <v>61</v>
       </c>
@@ -8983,7 +8987,7 @@
       </c>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>66</v>
       </c>
@@ -8997,7 +9001,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18">
         <v>67</v>
       </c>
@@ -9035,7 +9039,7 @@
       </c>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>70</v>
       </c>
@@ -9325,7 +9329,7 @@
       </c>
       <c r="D94" s="3"/>
     </row>
-    <row r="95" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>94</v>
       </c>
@@ -9615,7 +9619,7 @@
       </c>
       <c r="D118" s="3"/>
     </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="19">
         <v>118</v>
       </c>
@@ -9629,7 +9633,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="18">
         <v>119</v>
       </c>
@@ -9799,7 +9803,7 @@
       </c>
       <c r="D133" s="4"/>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="18">
         <v>133</v>
       </c>
@@ -9809,7 +9813,9 @@
       <c r="C134" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D134" s="3"/>
+      <c r="D134" s="3" t="s">
+        <v>2504</v>
+      </c>
     </row>
     <row r="135" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="19">
@@ -9859,7 +9865,7 @@
       </c>
       <c r="D138" s="3"/>
     </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="19">
         <v>138</v>
       </c>
@@ -9897,7 +9903,7 @@
       </c>
       <c r="D141" s="4"/>
     </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="18">
         <v>141</v>
       </c>
@@ -9911,7 +9917,7 @@
         <v>2193</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="19">
         <v>142</v>
       </c>
@@ -9937,7 +9943,7 @@
       </c>
       <c r="D144" s="3"/>
     </row>
-    <row r="145" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="19">
         <v>144</v>
       </c>
@@ -9951,7 +9957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="146" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="18">
         <v>145</v>
       </c>
@@ -10013,7 +10019,7 @@
       </c>
       <c r="D150" s="3"/>
     </row>
-    <row r="151" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="19">
         <v>150</v>
       </c>
@@ -10027,7 +10033,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="18">
         <v>151</v>
       </c>
@@ -10053,7 +10059,7 @@
       </c>
       <c r="D153" s="4"/>
     </row>
-    <row r="154" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="18">
         <v>153</v>
       </c>
@@ -10079,7 +10085,7 @@
       </c>
       <c r="D155" s="4"/>
     </row>
-    <row r="156" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="18">
         <v>155</v>
       </c>
@@ -10141,7 +10147,7 @@
       </c>
       <c r="D160" s="3"/>
     </row>
-    <row r="161" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="19">
         <v>160</v>
       </c>
@@ -10227,7 +10233,7 @@
       </c>
       <c r="D167" s="4"/>
     </row>
-    <row r="168" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A168" s="18">
         <v>167</v>
       </c>
@@ -10493,7 +10499,7 @@
       </c>
       <c r="D189" s="4"/>
     </row>
-    <row r="190" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="18">
         <v>189</v>
       </c>
@@ -10627,7 +10633,7 @@
       </c>
       <c r="D200" s="3"/>
     </row>
-    <row r="201" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="19">
         <v>200</v>
       </c>
@@ -10665,7 +10671,7 @@
       </c>
       <c r="D203" s="4"/>
     </row>
-    <row r="204" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A204" s="18">
         <v>203</v>
       </c>
@@ -10703,7 +10709,7 @@
       </c>
       <c r="D206" s="3"/>
     </row>
-    <row r="207" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="19">
         <v>206</v>
       </c>
@@ -10741,7 +10747,7 @@
       </c>
       <c r="D209" s="4"/>
     </row>
-    <row r="210" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="18">
         <v>209</v>
       </c>
@@ -10945,7 +10951,9 @@
       <c r="C226" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D226" s="3"/>
+      <c r="D226" s="3" t="s">
+        <v>2504</v>
+      </c>
     </row>
     <row r="227" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="19">
@@ -11029,7 +11037,9 @@
       <c r="C233" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D233" s="4"/>
+      <c r="D233" s="4" t="s">
+        <v>2504</v>
+      </c>
     </row>
     <row r="234" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="18">
@@ -11043,7 +11053,7 @@
       </c>
       <c r="D234" s="3"/>
     </row>
-    <row r="235" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="19">
         <v>234</v>
       </c>
@@ -11585,7 +11595,7 @@
       </c>
       <c r="D279" s="4"/>
     </row>
-    <row r="280" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="18">
         <v>279</v>
       </c>
@@ -11635,7 +11645,7 @@
       </c>
       <c r="D283" s="4"/>
     </row>
-    <row r="284" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="18">
         <v>283</v>
       </c>
@@ -12177,7 +12187,7 @@
       </c>
       <c r="D328" s="3"/>
     </row>
-    <row r="329" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A329" s="19">
         <v>328</v>
       </c>
@@ -12371,7 +12381,7 @@
       </c>
       <c r="D344" s="3"/>
     </row>
-    <row r="345" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A345" s="19">
         <v>344</v>
       </c>
@@ -13405,7 +13415,7 @@
       </c>
       <c r="D430" s="3"/>
     </row>
-    <row r="431" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A431" s="19">
         <v>430</v>
       </c>
@@ -14067,7 +14077,7 @@
       </c>
       <c r="D485" s="4"/>
     </row>
-    <row r="486" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A486" s="18">
         <v>485</v>
       </c>
@@ -14081,7 +14091,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="487" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A487" s="19">
         <v>486</v>
       </c>
@@ -14177,7 +14187,7 @@
       </c>
       <c r="D494" s="3"/>
     </row>
-    <row r="495" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A495" s="19">
         <v>494</v>
       </c>
@@ -14187,7 +14197,9 @@
       <c r="C495" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D495" s="4"/>
+      <c r="D495" s="4" t="s">
+        <v>2504</v>
+      </c>
     </row>
     <row r="496" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A496" s="18">
@@ -14225,7 +14237,7 @@
       </c>
       <c r="D498" s="3"/>
     </row>
-    <row r="499" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A499" s="19">
         <v>498</v>
       </c>
@@ -14935,7 +14947,7 @@
       </c>
       <c r="D557" s="4"/>
     </row>
-    <row r="558" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A558" s="18">
         <v>557</v>
       </c>
@@ -14985,7 +14997,7 @@
       </c>
       <c r="D561" s="4"/>
     </row>
-    <row r="562" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A562" s="18">
         <v>561</v>
       </c>
@@ -15719,7 +15731,7 @@
       </c>
       <c r="D622" s="3"/>
     </row>
-    <row r="623" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="623" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A623" s="19">
         <v>622</v>
       </c>
@@ -16741,7 +16753,7 @@
       </c>
       <c r="D707" s="4"/>
     </row>
-    <row r="708" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="708" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A708" s="18">
         <v>707</v>
       </c>
@@ -16947,7 +16959,7 @@
       </c>
       <c r="D724" s="3"/>
     </row>
-    <row r="725" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="725" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A725" s="19">
         <v>724</v>
       </c>
@@ -16961,7 +16973,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="726" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="726" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A726" s="18">
         <v>725</v>
       </c>
@@ -17129,7 +17141,7 @@
       </c>
       <c r="D739" s="4"/>
     </row>
-    <row r="740" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="740" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A740" s="18">
         <v>739</v>
       </c>
@@ -17227,7 +17239,7 @@
       </c>
       <c r="D747" s="4"/>
     </row>
-    <row r="748" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="748" spans="1:4" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A748" s="18">
         <v>747</v>
       </c>
@@ -17289,7 +17301,7 @@
       </c>
       <c r="D752" s="3"/>
     </row>
-    <row r="753" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="753" spans="1:4" ht="16.5" hidden="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A753" s="19">
         <v>752</v>
       </c>
@@ -17303,7 +17315,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="754" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="754" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A754" s="18">
         <v>753</v>
       </c>
@@ -26586,7 +26598,11 @@
       <c r="E1653" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:D1486" xr:uid="{AA2808F7-94D6-4788-B7C2-AA20F53DB078}"/>
+  <autoFilter ref="A2:D1486" xr:uid="{AA2808F7-94D6-4788-B7C2-AA20F53DB078}">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
@@ -30005,10 +30021,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A56D5E7-551D-4DA8-94DC-D98ED60B1AEE}">
-  <dimension ref="A1:D114"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30019,7 +30035,7 @@
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>1494</v>
       </c>
@@ -30027,98 +30043,107 @@
       <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>3</v>
+      <c r="A3" s="3" t="s">
+        <v>1495</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1496</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1495</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1496</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="4" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1498</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1497</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1498</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>1499</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1500</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1499</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>1500</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>1501</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>1501</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
+      <c r="A7" s="3" t="s">
+        <v>1502</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1503</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1502</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>1503</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>1504</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>1505</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>1504</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>1505</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>5</v>
+      <c r="A9" s="3" t="s">
+        <v>1506</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1507</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2499</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1506</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>1507</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="4" t="s">
+        <v>1508</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>1509</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
@@ -30126,1255 +30151,1241 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>1508</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>1509</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>2499</v>
+      <c r="A11" s="3" t="s">
+        <v>1510</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1511</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1510</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="A12" s="4" t="s">
+        <v>1512</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1513</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>1512</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1513</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1515</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>1515</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="4" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>1516</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1517</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
+      <c r="A15" s="3" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1518</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>1519</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="A16" s="4" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>1521</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>1521</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>7</v>
+      <c r="A17" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1522</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="A18" s="4" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>1524</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>1524</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
+      <c r="A19" s="3" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1526</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>1526</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>7</v>
+      <c r="A20" s="4" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>1528</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>1527</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>1528</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="A21" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>1530</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>5</v>
+      <c r="A22" s="4" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>1532</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>1531</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>1532</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>7</v>
+      <c r="A23" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1534</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>1534</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>5</v>
+      <c r="A24" s="4" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>1536</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>1535</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>1536</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>7</v>
+      <c r="A25" s="3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1538</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1537</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>1538</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
+      <c r="A26" s="4" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>1540</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>1540</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
+      <c r="A27" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>325</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>5</v>
+      <c r="A28" s="4" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>1542</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>1543</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>7</v>
+      <c r="A29" s="3" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1545</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1544</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>1545</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>5</v>
+      <c r="A30" s="4" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>1546</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>1547</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="A31" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1549</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>1548</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>1549</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="4" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>1551</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>1550</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>1551</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>7</v>
+      <c r="A33" s="3" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1553</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>1552</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>1553</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>10</v>
+      <c r="A34" s="4" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>1555</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1555</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="A35" s="3" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1557</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>1556</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>1557</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>7</v>
+      <c r="A36" s="4" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>1559</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>1558</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>1559</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>5</v>
+      <c r="A37" s="3" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1561</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>1560</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>1561</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>7</v>
+      <c r="A38" s="4" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>1563</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>1562</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>5</v>
+      <c r="A39" s="3" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>1565</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>1564</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>7</v>
+      <c r="A40" s="4" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>1567</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>1566</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="A41" s="3" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1569</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>1568</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>1569</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>5</v>
+      <c r="A42" s="4" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>1571</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>1570</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>1571</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>7</v>
+      <c r="A43" s="3" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1573</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>1572</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>1573</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>5</v>
+      <c r="A44" s="4" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>1575</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>1574</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>1575</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>7</v>
+      <c r="A45" s="3" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>1576</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>1577</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>5</v>
+      <c r="A46" s="4" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>1578</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>1579</v>
-      </c>
-      <c r="C47" s="4" t="s">
+      <c r="A47" s="3" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>1580</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>1581</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>7</v>
+      <c r="A48" s="4" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>1582</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>1583</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>5</v>
+      <c r="A49" s="3" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1585</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>1584</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>1585</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="A50" s="4" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>1586</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>1587</v>
-      </c>
-      <c r="C51" s="4" t="s">
+      <c r="A51" s="3" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>1588</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>1589</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>7</v>
+      <c r="A52" s="4" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>1591</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>1590</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>1591</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>5</v>
+      <c r="A53" s="3" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>1593</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>1592</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>1593</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>7</v>
+      <c r="A54" s="4" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>1595</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>1594</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>1595</v>
-      </c>
-      <c r="C55" s="4" t="s">
+      <c r="A55" s="3" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>1597</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>1596</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>1597</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>10</v>
+      <c r="A56" s="4" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>1599</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>1598</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>1599</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>7</v>
+      <c r="A57" s="3" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>1601</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>1600</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>1601</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>5</v>
+      <c r="A58" s="4" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>1603</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>1602</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C59" s="4" t="s">
+      <c r="A59" s="3" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>1605</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>1604</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>1605</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>7</v>
+      <c r="A60" s="4" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>1606</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>1607</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>5</v>
+      <c r="A61" s="3" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>1609</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>1608</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C62" s="3" t="s">
+      <c r="A62" s="4" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>1611</v>
+      </c>
+      <c r="C62" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>1610</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>1611</v>
-      </c>
-      <c r="C63" s="4" t="s">
+      <c r="A63" s="3" t="s">
+        <v>1612</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>1613</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>1612</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>1613</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="A64" s="4" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>1615</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>1614</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>1615</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="A65" s="3" t="s">
+        <v>1616</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>1617</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>1616</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>1617</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>7</v>
+      <c r="A66" s="4" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>1618</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>1619</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>10</v>
+      <c r="A67" s="3" t="s">
+        <v>1620</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>1621</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>1620</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>1621</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>7</v>
+      <c r="A68" s="4" t="s">
+        <v>1622</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>1623</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>1622</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>1623</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>5</v>
+      <c r="A69" s="3" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>1625</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>1624</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>1625</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>7</v>
+      <c r="A70" s="4" t="s">
+        <v>1626</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>1627</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>1626</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>1627</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>5</v>
+      <c r="A71" s="3" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>1629</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>1628</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>1629</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>10</v>
+      <c r="A72" s="4" t="s">
+        <v>1630</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>1631</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>1630</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>1631</v>
-      </c>
-      <c r="C73" s="4" t="s">
+      <c r="A73" s="3" t="s">
+        <v>1632</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>1633</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
-        <v>1632</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>1633</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>7</v>
+      <c r="A74" s="4" t="s">
+        <v>1634</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>1635</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>1635</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>5</v>
+      <c r="A75" s="3" t="s">
+        <v>1636</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>1636</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>1637</v>
-      </c>
-      <c r="C76" s="3" t="s">
+      <c r="A76" s="4" t="s">
+        <v>1638</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C76" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
-        <v>1638</v>
-      </c>
-      <c r="B77" s="10" t="s">
-        <v>1639</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>7</v>
+      <c r="A77" s="3" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>1641</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
-        <v>1640</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>1641</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>5</v>
+      <c r="A78" s="4" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>1643</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="4" t="s">
-        <v>1642</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>1643</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>7</v>
+      <c r="A79" s="3" t="s">
+        <v>1644</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>1645</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="3" t="s">
-        <v>1644</v>
-      </c>
-      <c r="B80" s="9" t="s">
-        <v>1645</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>5</v>
+      <c r="A80" s="4" t="s">
+        <v>1646</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>1647</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="4" t="s">
-        <v>1646</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>1647</v>
-      </c>
-      <c r="C81" s="4" t="s">
+      <c r="A81" s="3" t="s">
+        <v>1648</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>1649</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="3" t="s">
-        <v>1648</v>
-      </c>
-      <c r="B82" s="9" t="s">
-        <v>1649</v>
-      </c>
-      <c r="C82" s="3" t="s">
+      <c r="A82" s="4" t="s">
+        <v>1650</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>1651</v>
+      </c>
+      <c r="C82" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="4" t="s">
-        <v>1650</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>1651</v>
-      </c>
-      <c r="C83" s="4" t="s">
+      <c r="A83" s="3" t="s">
+        <v>1652</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>1653</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
-        <v>1652</v>
-      </c>
-      <c r="B84" s="9" t="s">
-        <v>1653</v>
-      </c>
-      <c r="C84" s="3" t="s">
+      <c r="A84" s="4" t="s">
+        <v>1654</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C84" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>1654</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>1655</v>
-      </c>
-      <c r="C85" s="4" t="s">
+      <c r="A85" s="3" t="s">
+        <v>1656</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>1657</v>
+      </c>
+      <c r="C85" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="3" t="s">
-        <v>1656</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>1657</v>
-      </c>
-      <c r="C86" s="3" t="s">
+      <c r="A86" s="4" t="s">
+        <v>1658</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>1659</v>
+      </c>
+      <c r="C86" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
-        <v>1658</v>
-      </c>
-      <c r="B87" s="10" t="s">
-        <v>1659</v>
-      </c>
-      <c r="C87" s="4" t="s">
+      <c r="A87" s="3" t="s">
+        <v>1660</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C87" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>1660</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>1661</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>7</v>
+      <c r="A88" s="4" t="s">
+        <v>1662</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>1663</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="4" t="s">
-        <v>1662</v>
-      </c>
-      <c r="B89" s="10" t="s">
-        <v>1663</v>
-      </c>
-      <c r="C89" s="4" t="s">
+      <c r="A89" s="3" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B89" s="9" t="s">
+        <v>1665</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
-        <v>1664</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>1665</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>5</v>
+      <c r="A90" s="4" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>1667</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
-        <v>1666</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>1667</v>
-      </c>
-      <c r="C91" s="4" t="s">
+      <c r="A91" s="3" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>1669</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="3" t="s">
-        <v>1668</v>
-      </c>
-      <c r="B92" s="9" t="s">
-        <v>1669</v>
-      </c>
-      <c r="C92" s="3" t="s">
+      <c r="A92" s="4" t="s">
+        <v>1670</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>1671</v>
+      </c>
+      <c r="C92" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
-        <v>1670</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>1671</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="A93" s="3" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="3" t="s">
-        <v>1672</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>1673</v>
-      </c>
-      <c r="C94" s="3" t="s">
+      <c r="A94" s="4" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>1675</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
-        <v>1674</v>
-      </c>
-      <c r="B95" s="10" t="s">
-        <v>1675</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>7</v>
+      <c r="A95" s="3" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="3" t="s">
-        <v>1676</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>1677</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>5</v>
+      <c r="A96" s="4" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B96" s="10" t="s">
+        <v>1679</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>1678</v>
-      </c>
-      <c r="B97" s="10" t="s">
-        <v>1679</v>
-      </c>
-      <c r="C97" s="4" t="s">
-        <v>7</v>
+      <c r="A97" s="3" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>1681</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>5</v>
+      <c r="A98" s="4" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B98" s="10" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
-        <v>1682</v>
-      </c>
-      <c r="B99" s="10" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C99" s="4" t="s">
+      <c r="A99" s="3" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>1685</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="3" t="s">
-        <v>1684</v>
-      </c>
-      <c r="B100" s="9" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C100" s="3" t="s">
+      <c r="A100" s="4" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>1687</v>
+      </c>
+      <c r="C100" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
-        <v>1686</v>
-      </c>
-      <c r="B101" s="10" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C101" s="4" t="s">
-        <v>7</v>
+      <c r="A101" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>1689</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
-        <v>1688</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>5</v>
+      <c r="A102" s="4" t="s">
+        <v>1690</v>
+      </c>
+      <c r="B102" s="10" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>1690</v>
-      </c>
-      <c r="B103" s="10" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C103" s="4" t="s">
+      <c r="A103" s="3" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>1693</v>
+      </c>
+      <c r="C103" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="3" t="s">
-        <v>1692</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>7</v>
+      <c r="A104" s="4" t="s">
+        <v>1694</v>
+      </c>
+      <c r="B104" s="10" t="s">
+        <v>1695</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="4" t="s">
-        <v>1694</v>
-      </c>
-      <c r="B105" s="10" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C105" s="4" t="s">
+      <c r="A105" s="3" t="s">
+        <v>1696</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>1697</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="3" t="s">
-        <v>1696</v>
-      </c>
-      <c r="B106" s="9" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C106" s="3" t="s">
+      <c r="A106" s="4" t="s">
+        <v>1698</v>
+      </c>
+      <c r="B106" s="10" t="s">
+        <v>1699</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="4" t="s">
-        <v>1698</v>
-      </c>
-      <c r="B107" s="10" t="s">
-        <v>1699</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>10</v>
+      <c r="A107" s="3" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>1701</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="3" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C108" s="3" t="s">
+      <c r="A108" s="4" t="s">
+        <v>1702</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>1703</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>1702</v>
-      </c>
-      <c r="B109" s="10" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>7</v>
+      <c r="A109" s="3" t="s">
+        <v>1704</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>1705</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="3" t="s">
-        <v>1704</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C110" s="3" t="s">
+      <c r="A110" s="4" t="s">
+        <v>1706</v>
+      </c>
+      <c r="B110" s="10" t="s">
+        <v>1707</v>
+      </c>
+      <c r="C110" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
-        <v>1706</v>
-      </c>
-      <c r="B111" s="10" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="3" t="s">
+      <c r="A111" s="3" t="s">
         <v>1708</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B111" s="9" t="s">
         <v>1709</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="C111" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="1"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="1"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="15"/>
       <c r="C113" s="1"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:D3" xr:uid="{80F38252-6BCC-4A33-87B6-D592758D0927}"/>
+  <autoFilter ref="A2:D111" xr:uid="{80F38252-6BCC-4A33-87B6-D592758D0927}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://leetcode-cn.com/problems/is-unique-lcci" xr:uid="{65988DF1-DDBD-46D8-BCC3-D068AE11422C}"/>
-    <hyperlink ref="B5" r:id="rId2" display="https://leetcode-cn.com/problems/check-permutation-lcci" xr:uid="{0F986469-D424-4433-A305-0707C512BE27}"/>
-    <hyperlink ref="B6" r:id="rId3" display="https://leetcode-cn.com/problems/string-to-url-lcci" xr:uid="{2F3400F8-7380-4798-9149-265A7BB1A510}"/>
-    <hyperlink ref="B7" r:id="rId4" display="https://leetcode-cn.com/problems/palindrome-permutation-lcci" xr:uid="{AF8B9FE0-CB83-43BA-BD8D-34539B7B3D3F}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://leetcode-cn.com/problems/one-away-lcci" xr:uid="{233DA28C-8530-4F86-BB02-147DF97D05FF}"/>
-    <hyperlink ref="B9" r:id="rId6" display="https://leetcode-cn.com/problems/compress-string-lcci" xr:uid="{CA2FBC9D-4720-468C-971C-6C8500655155}"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://leetcode-cn.com/problems/rotate-matrix-lcci" xr:uid="{DB282451-E4EE-4BC9-BB2E-3E4BA8A4F634}"/>
-    <hyperlink ref="B11" r:id="rId8" display="https://leetcode-cn.com/problems/zero-matrix-lcci" xr:uid="{FC91657D-C8C8-4B82-A3F5-00E874E63D20}"/>
-    <hyperlink ref="B12" r:id="rId9" display="https://leetcode-cn.com/problems/string-rotation-lcci" xr:uid="{75E626F9-C1B4-4ACC-8FC0-84C6CD3CF23D}"/>
-    <hyperlink ref="B13" r:id="rId10" display="https://leetcode-cn.com/problems/remove-duplicate-node-lcci" xr:uid="{B6DF184B-08EA-411E-91E0-83C90D97098B}"/>
-    <hyperlink ref="B14" r:id="rId11" display="https://leetcode-cn.com/problems/kth-node-from-end-of-list-lcci" xr:uid="{2D335B55-C4F4-4EC2-AA0E-84245FA91EA6}"/>
-    <hyperlink ref="B15" r:id="rId12" display="https://leetcode-cn.com/problems/delete-middle-node-lcci" xr:uid="{32932FCA-A4B6-4926-A277-2DBF968FB66F}"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://leetcode-cn.com/problems/partition-list-lcci" xr:uid="{B3BB5593-453D-4B9A-ACD7-796A5A68895F}"/>
-    <hyperlink ref="B17" r:id="rId14" display="https://leetcode-cn.com/problems/sum-lists-lcci" xr:uid="{FF9325D2-355A-4B6A-99C1-A1507D7AA8C6}"/>
-    <hyperlink ref="B18" r:id="rId15" display="https://leetcode-cn.com/problems/palindrome-linked-list-lcci" xr:uid="{9D69124C-8275-48C5-89C6-47C06A7A226B}"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://leetcode-cn.com/problems/intersection-of-two-linked-lists-lcci" xr:uid="{B2077538-5DC1-4718-ACD3-3CD39677C311}"/>
-    <hyperlink ref="B20" r:id="rId17" display="https://leetcode-cn.com/problems/linked-list-cycle-lcci" xr:uid="{8683A9A3-D47D-4ECD-A89C-30DB4235B322}"/>
-    <hyperlink ref="B21" r:id="rId18" display="https://leetcode-cn.com/problems/three-in-one-lcci" xr:uid="{16A71F7A-0E5E-4A2F-9519-F1DCF8AE0A9C}"/>
-    <hyperlink ref="B22" r:id="rId19" display="https://leetcode-cn.com/problems/min-stack-lcci" xr:uid="{41B71FE5-16D7-4D2F-B01B-46203567C258}"/>
-    <hyperlink ref="B23" r:id="rId20" display="https://leetcode-cn.com/problems/stack-of-plates-lcci" xr:uid="{EA85FEC0-0658-46E8-AA7B-3A73A42E9CD0}"/>
-    <hyperlink ref="B24" r:id="rId21" display="https://leetcode-cn.com/problems/implement-queue-using-stacks-lcci" xr:uid="{7C364CD7-B3C4-44D2-A286-BC975B86E112}"/>
-    <hyperlink ref="B25" r:id="rId22" display="https://leetcode-cn.com/problems/sort-of-stacks-lcci" xr:uid="{91BF0172-A7F3-42AC-9962-8401A3E37B5B}"/>
-    <hyperlink ref="B26" r:id="rId23" display="https://leetcode-cn.com/problems/animal-shelter-lcci" xr:uid="{BE33DA3D-66F5-4848-B175-AC6D044ACFE2}"/>
-    <hyperlink ref="B27" r:id="rId24" display="https://leetcode-cn.com/problems/route-between-nodes-lcci" xr:uid="{C28C6B2C-3E5F-4DA3-9E4E-DF9536475314}"/>
-    <hyperlink ref="B28" r:id="rId25" display="https://leetcode-cn.com/problems/minimum-height-tree-lcci" xr:uid="{67D13540-FF3C-4489-BAED-66DA7709317D}"/>
-    <hyperlink ref="B29" r:id="rId26" display="https://leetcode-cn.com/problems/list-of-depth-lcci" xr:uid="{7036EF6D-E728-4AEA-B879-F0C023C884B6}"/>
-    <hyperlink ref="B30" r:id="rId27" display="https://leetcode-cn.com/problems/check-balance-lcci" xr:uid="{7FEE5AC8-7FBD-4D6E-9E53-9E1B19BFC3D7}"/>
-    <hyperlink ref="B31" r:id="rId28" display="https://leetcode-cn.com/problems/legal-binary-search-tree-lcci" xr:uid="{FB83AADB-12BE-4B14-AA18-72EB3F224ECC}"/>
-    <hyperlink ref="B32" r:id="rId29" display="https://leetcode-cn.com/problems/successor-lcci" xr:uid="{3A79340E-7A7F-4104-A79C-2B88D339BE1D}"/>
-    <hyperlink ref="B33" r:id="rId30" display="https://leetcode-cn.com/problems/first-common-ancestor-lcci" xr:uid="{7B105FA3-0BDA-402D-A47E-84E208984D86}"/>
-    <hyperlink ref="B34" r:id="rId31" display="https://leetcode-cn.com/problems/bst-sequences-lcci" xr:uid="{1E6C4BFF-3E92-4CE1-B9DA-67CD7D5FA8DB}"/>
-    <hyperlink ref="B35" r:id="rId32" display="https://leetcode-cn.com/problems/check-subtree-lcci" xr:uid="{5654310E-07E7-40C0-92A2-C1D32D014928}"/>
-    <hyperlink ref="B36" r:id="rId33" display="https://leetcode-cn.com/problems/paths-with-sum-lcci" xr:uid="{38839549-B0D3-459B-A535-D5E776555AD9}"/>
-    <hyperlink ref="B37" r:id="rId34" display="https://leetcode-cn.com/problems/insert-into-bits-lcci" xr:uid="{BBD266AD-2B1F-44AC-90B5-4719FAD4FC0A}"/>
-    <hyperlink ref="B38" r:id="rId35" display="https://leetcode-cn.com/problems/bianry-number-to-string-lcci" xr:uid="{326A058F-888D-49BC-8047-C7E90975BF8F}"/>
-    <hyperlink ref="B39" r:id="rId36" display="https://leetcode-cn.com/problems/reverse-bits-lcci" xr:uid="{EF74E6F3-82B2-4E0F-9DAE-9AEE2C919B59}"/>
-    <hyperlink ref="B40" r:id="rId37" display="https://leetcode-cn.com/problems/closed-number-lcci" xr:uid="{25D60044-C22A-4B7F-8C47-BACC6E36E49E}"/>
-    <hyperlink ref="B41" r:id="rId38" display="https://leetcode-cn.com/problems/convert-integer-lcci" xr:uid="{93B8B2FA-5B00-44C7-9CE7-AF4AA3058F0E}"/>
-    <hyperlink ref="B42" r:id="rId39" display="https://leetcode-cn.com/problems/exchange-lcci" xr:uid="{B075CBBE-02CE-41A2-96E8-82EF927A6D97}"/>
-    <hyperlink ref="B43" r:id="rId40" display="https://leetcode-cn.com/problems/draw-line-lcci" xr:uid="{E357632D-8E06-4853-8F86-A00DDEDAA067}"/>
-    <hyperlink ref="B44" r:id="rId41" display="https://leetcode-cn.com/problems/three-steps-problem-lcci" xr:uid="{92C63BFC-5378-42E5-98DB-EFF6CD2765F0}"/>
-    <hyperlink ref="B45" r:id="rId42" display="https://leetcode-cn.com/problems/robot-in-a-grid-lcci" xr:uid="{F9245D50-E6E9-4F27-B456-3B6F5A2B9B6D}"/>
-    <hyperlink ref="B46" r:id="rId43" display="https://leetcode-cn.com/problems/magic-index-lcci" xr:uid="{9D174FE5-BE18-4D10-8ACA-68AF645CED25}"/>
-    <hyperlink ref="B47" r:id="rId44" display="https://leetcode-cn.com/problems/power-set-lcci" xr:uid="{B4C5B35A-A4D3-4148-89C7-5BB0134E1A2C}"/>
-    <hyperlink ref="B48" r:id="rId45" display="https://leetcode-cn.com/problems/recursive-mulitply-lcci" xr:uid="{B7954E82-1AE1-46F6-B6E8-4E87236B0FB9}"/>
-    <hyperlink ref="B49" r:id="rId46" display="https://leetcode-cn.com/problems/hanota-lcci" xr:uid="{02C845D3-C541-43C6-8126-53596B4FE97C}"/>
-    <hyperlink ref="B50" r:id="rId47" display="https://leetcode-cn.com/problems/permutation-i-lcci" xr:uid="{F6DFAD70-604A-42B0-97A3-97F30C83ABDE}"/>
-    <hyperlink ref="B51" r:id="rId48" display="https://leetcode-cn.com/problems/permutation-ii-lcci" xr:uid="{8B64FD2C-A5AD-4EA1-8357-A9ADF2CF7A0E}"/>
-    <hyperlink ref="B52" r:id="rId49" display="https://leetcode-cn.com/problems/bracket-lcci" xr:uid="{151C1933-2408-4E04-8A9D-2C60CA2AED5F}"/>
-    <hyperlink ref="B53" r:id="rId50" display="https://leetcode-cn.com/problems/color-fill-lcci" xr:uid="{3D4A0143-5B32-4F5E-A7FD-958F4D7F20BC}"/>
-    <hyperlink ref="B54" r:id="rId51" display="https://leetcode-cn.com/problems/coin-lcci" xr:uid="{60620454-AA8A-4C73-BB5E-4651D5B4BF5D}"/>
-    <hyperlink ref="B55" r:id="rId52" display="https://leetcode-cn.com/problems/eight-queens-lcci" xr:uid="{EC46D030-DA0B-4F43-BC9D-782183396DF1}"/>
-    <hyperlink ref="B56" r:id="rId53" display="https://leetcode-cn.com/problems/pile-box-lcci" xr:uid="{B31CE329-5304-466A-B6BD-23B3B1C76D5C}"/>
-    <hyperlink ref="B57" r:id="rId54" display="https://leetcode-cn.com/problems/boolean-evaluation-lcci" xr:uid="{D1FC6764-ADB1-4188-87D0-1FC32AF8FCFB}"/>
-    <hyperlink ref="B58" r:id="rId55" display="https://leetcode-cn.com/problems/sorted-merge-lcci" xr:uid="{A26EB65E-AE99-487C-B30F-9DF54CB454C7}"/>
-    <hyperlink ref="B59" r:id="rId56" display="https://leetcode-cn.com/problems/group-anagrams-lcci" xr:uid="{8E72392C-CFA7-4D83-A95F-DCF988B9370D}"/>
-    <hyperlink ref="B60" r:id="rId57" display="https://leetcode-cn.com/problems/search-rotate-array-lcci" xr:uid="{CF8FE950-2200-48BB-BDB1-8429544AC371}"/>
-    <hyperlink ref="B61" r:id="rId58" display="https://leetcode-cn.com/problems/sparse-array-search-lcci" xr:uid="{A3280143-773F-48A5-BCAF-31B3103289F5}"/>
-    <hyperlink ref="B62" r:id="rId59" display="https://leetcode-cn.com/problems/sorted-matrix-search-lcci" xr:uid="{4679EDB6-17C7-4ADF-BD73-A4943A974E74}"/>
-    <hyperlink ref="B63" r:id="rId60" display="https://leetcode-cn.com/problems/rank-from-stream-lcci" xr:uid="{D0BA52FE-FA62-4DC5-B9DD-AB05974C8483}"/>
-    <hyperlink ref="B64" r:id="rId61" display="https://leetcode-cn.com/problems/peaks-and-valleys-lcci" xr:uid="{469F2ADA-EB5A-4C69-BF09-521D8FCE7060}"/>
-    <hyperlink ref="B65" r:id="rId62" display="https://leetcode-cn.com/problems/swap-numbers-lcci" xr:uid="{43FC9D7D-A5D1-4E1F-B654-14AF3FD61F69}"/>
-    <hyperlink ref="B66" r:id="rId63" display="https://leetcode-cn.com/problems/words-frequency-lcci" xr:uid="{FB1F45E1-EB24-4064-BC6C-A04EC9D58D40}"/>
-    <hyperlink ref="B67" r:id="rId64" display="https://leetcode-cn.com/problems/intersection-lcci" xr:uid="{6DB0B8DB-8B20-478C-AA61-6B3CABB16787}"/>
-    <hyperlink ref="B68" r:id="rId65" display="https://leetcode-cn.com/problems/tic-tac-toe-lcci" xr:uid="{6631C6D9-697A-4FB9-8F67-6381ABC8BBC1}"/>
-    <hyperlink ref="B69" r:id="rId66" display="https://leetcode-cn.com/problems/factorial-zeros-lcci" xr:uid="{EB2E2991-D43C-4F21-B3A4-5C8C70A44D2A}"/>
-    <hyperlink ref="B70" r:id="rId67" display="https://leetcode-cn.com/problems/smallest-difference-lcci" xr:uid="{4189AD0E-F488-4C87-906F-F7E0678D9632}"/>
-    <hyperlink ref="B71" r:id="rId68" display="https://leetcode-cn.com/problems/maximum-lcci" xr:uid="{D37124E5-F65C-402D-860B-617C0C80B687}"/>
-    <hyperlink ref="B72" r:id="rId69" display="https://leetcode-cn.com/problems/english-int-lcci" xr:uid="{5AF82742-D0B5-4F04-B2E9-D79264BE2D96}"/>
-    <hyperlink ref="B73" r:id="rId70" display="https://leetcode-cn.com/problems/operations-lcci" xr:uid="{63E0AF68-9AA1-47F8-B2CC-6130D2EDDE29}"/>
-    <hyperlink ref="B74" r:id="rId71" display="https://leetcode-cn.com/problems/living-people-lcci" xr:uid="{D710BEEB-FB7C-4B55-A6E8-F574781430AA}"/>
-    <hyperlink ref="B75" r:id="rId72" display="https://leetcode-cn.com/problems/diving-board-lcci" xr:uid="{7CB20116-A843-4EC9-AAE4-B576B510ECA8}"/>
-    <hyperlink ref="B76" r:id="rId73" display="https://leetcode-cn.com/problems/bisect-squares-lcci" xr:uid="{4B5489CA-A20B-41A4-8CA1-BBDB8B5A28CB}"/>
-    <hyperlink ref="B77" r:id="rId74" display="https://leetcode-cn.com/problems/best-line-lcci" xr:uid="{9698873B-AD9B-417C-915F-C118B01B1159}"/>
-    <hyperlink ref="B78" r:id="rId75" display="https://leetcode-cn.com/problems/master-mind-lcci" xr:uid="{4BE4B5F6-73B6-4B5E-975F-161F89B54708}"/>
-    <hyperlink ref="B79" r:id="rId76" display="https://leetcode-cn.com/problems/sub-sort-lcci" xr:uid="{89A4E8B0-D02D-4557-858E-DD3CA9165580}"/>
-    <hyperlink ref="B80" r:id="rId77" display="https://leetcode-cn.com/problems/contiguous-sequence-lcci" xr:uid="{5CCF6FBA-7DE4-45AF-9231-D9313C972AEA}"/>
-    <hyperlink ref="B81" r:id="rId78" display="https://leetcode-cn.com/problems/pattern-matching-lcci" xr:uid="{395FB40F-7682-4B89-AEDA-C5880E81AD5E}"/>
-    <hyperlink ref="B82" r:id="rId79" display="https://leetcode-cn.com/problems/pond-sizes-lcci" xr:uid="{6E2D58F4-D254-4928-A168-3B6EEA3B6E4D}"/>
-    <hyperlink ref="B83" r:id="rId80" display="https://leetcode-cn.com/problems/t9-lcci" xr:uid="{DA07B267-F7DB-46F6-979B-C2F883DE0454}"/>
-    <hyperlink ref="B84" r:id="rId81" display="https://leetcode-cn.com/problems/sum-swap-lcci" xr:uid="{7EB17C26-38AE-418F-9D65-DF4B6619444A}"/>
-    <hyperlink ref="B85" r:id="rId82" display="https://leetcode-cn.com/problems/langtons-ant-lcci" xr:uid="{F78BCB39-1E5D-4C24-ADEC-56316998B9B2}"/>
-    <hyperlink ref="B86" r:id="rId83" display="https://leetcode-cn.com/problems/pairs-with-sum-lcci" xr:uid="{1B9D93C6-2EE2-41B0-8B1E-47FE60D5A298}"/>
-    <hyperlink ref="B87" r:id="rId84" display="https://leetcode-cn.com/problems/lru-cache-lcci" xr:uid="{9B414F26-99FC-4B25-B02B-CCC508647EDE}"/>
-    <hyperlink ref="B88" r:id="rId85" display="https://leetcode-cn.com/problems/calculator-lcci" xr:uid="{E4BDC078-247B-42FC-84C3-19F1FAD929F7}"/>
-    <hyperlink ref="B89" r:id="rId86" display="https://leetcode-cn.com/problems/add-without-plus-lcci" xr:uid="{02C8DD3E-CB7A-415C-9D06-2A9B165A4A07}"/>
-    <hyperlink ref="B90" r:id="rId87" display="https://leetcode-cn.com/problems/missing-number-lcci" xr:uid="{5871C071-93D4-4CAA-8E0F-BF1BCE8CCC0D}"/>
-    <hyperlink ref="B91" r:id="rId88" display="https://leetcode-cn.com/problems/find-longest-subarray-lcci" xr:uid="{EE75AA24-AD4E-4B33-A69C-4DB5E2E6D6C3}"/>
-    <hyperlink ref="B92" r:id="rId89" display="https://leetcode-cn.com/problems/number-of-2s-in-range-lcci" xr:uid="{41E555F7-15F0-4930-98AC-AF53E453C55D}"/>
-    <hyperlink ref="B93" r:id="rId90" display="https://leetcode-cn.com/problems/baby-names-lcci" xr:uid="{0BF45C72-3F8F-4641-B10F-191B26DB63FF}"/>
-    <hyperlink ref="B94" r:id="rId91" display="https://leetcode-cn.com/problems/circus-tower-lcci" xr:uid="{A9E4A819-2C01-4E8F-BFED-1E8795E508DA}"/>
-    <hyperlink ref="B95" r:id="rId92" display="https://leetcode-cn.com/problems/get-kth-magic-number-lcci" xr:uid="{2A0EFA7D-F744-49CF-9CAA-DD0E5BF0387E}"/>
-    <hyperlink ref="B96" r:id="rId93" display="https://leetcode-cn.com/problems/find-majority-element-lcci" xr:uid="{1B8336E6-8051-4819-83A3-2C3628559D40}"/>
-    <hyperlink ref="B97" r:id="rId94" display="https://leetcode-cn.com/problems/find-closest-lcci" xr:uid="{BC76320B-12C4-48C8-A009-EBB55EF1933D}"/>
-    <hyperlink ref="B98" r:id="rId95" display="https://leetcode-cn.com/problems/binode-lcci" xr:uid="{F1BCB2F9-33D4-4584-9892-902E43D9A644}"/>
-    <hyperlink ref="B99" r:id="rId96" display="https://leetcode-cn.com/problems/re-space-lcci" xr:uid="{980A4797-78D5-4516-B2C4-1E4A32C814A2}"/>
-    <hyperlink ref="B100" r:id="rId97" display="https://leetcode-cn.com/problems/smallest-k-lcci" xr:uid="{9420EDED-D3B9-43A2-A100-D989CBB1604B}"/>
-    <hyperlink ref="B101" r:id="rId98" display="https://leetcode-cn.com/problems/longest-word-lcci" xr:uid="{8F2B59A7-6ADC-47E4-BAD1-13AFC3C0D7E0}"/>
-    <hyperlink ref="B102" r:id="rId99" display="https://leetcode-cn.com/problems/the-masseuse-lcci" xr:uid="{86A5A113-96E1-48BF-84A9-50A7B0748F89}"/>
-    <hyperlink ref="B103" r:id="rId100" display="https://leetcode-cn.com/problems/multi-search-lcci" xr:uid="{8B72DECA-92B4-4DF8-8591-D4B93237730A}"/>
-    <hyperlink ref="B104" r:id="rId101" display="https://leetcode-cn.com/problems/shortest-supersequence-lcci" xr:uid="{ECF4C719-7A41-4BAA-AE6A-38AD845FED2A}"/>
-    <hyperlink ref="B105" r:id="rId102" display="https://leetcode-cn.com/problems/missing-two-lcci" xr:uid="{589EF060-DDBE-42F7-999A-718452DDB0A6}"/>
-    <hyperlink ref="B106" r:id="rId103" display="https://leetcode-cn.com/problems/continuous-median-lcci" xr:uid="{A1A67E99-E8D5-4A1C-8299-EEBA924AA77F}"/>
-    <hyperlink ref="B107" r:id="rId104" display="https://leetcode-cn.com/problems/volume-of-histogram-lcci" xr:uid="{877FD415-8962-4351-A26B-E79F40846A2A}"/>
-    <hyperlink ref="B108" r:id="rId105" display="https://leetcode-cn.com/problems/word-transformer-lcci" xr:uid="{93500134-4C38-487D-AF8B-A453EF6A5F41}"/>
-    <hyperlink ref="B109" r:id="rId106" display="https://leetcode-cn.com/problems/max-black-square-lcci" xr:uid="{4CB8B84B-0434-4289-864E-2B8F6EB05BE9}"/>
-    <hyperlink ref="B110" r:id="rId107" display="https://leetcode-cn.com/problems/max-submatrix-lcci" xr:uid="{6CB09E9D-2A22-486F-BBBD-30285F51277B}"/>
-    <hyperlink ref="B111" r:id="rId108" display="https://leetcode-cn.com/problems/word-rectangle-lcci" xr:uid="{FBBA00A7-D7D2-4365-AB95-5568A0451AB3}"/>
-    <hyperlink ref="B112" r:id="rId109" display="https://leetcode-cn.com/problems/sparse-similarity-lcci" xr:uid="{A3B1D418-E51B-47DF-8F1D-86BABB239D06}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://leetcode-cn.com/problems/is-unique-lcci" xr:uid="{65988DF1-DDBD-46D8-BCC3-D068AE11422C}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://leetcode-cn.com/problems/check-permutation-lcci" xr:uid="{0F986469-D424-4433-A305-0707C512BE27}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://leetcode-cn.com/problems/string-to-url-lcci" xr:uid="{2F3400F8-7380-4798-9149-265A7BB1A510}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://leetcode-cn.com/problems/palindrome-permutation-lcci" xr:uid="{AF8B9FE0-CB83-43BA-BD8D-34539B7B3D3F}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://leetcode-cn.com/problems/one-away-lcci" xr:uid="{233DA28C-8530-4F86-BB02-147DF97D05FF}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://leetcode-cn.com/problems/compress-string-lcci" xr:uid="{CA2FBC9D-4720-468C-971C-6C8500655155}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://leetcode-cn.com/problems/rotate-matrix-lcci" xr:uid="{DB282451-E4EE-4BC9-BB2E-3E4BA8A4F634}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://leetcode-cn.com/problems/zero-matrix-lcci" xr:uid="{FC91657D-C8C8-4B82-A3F5-00E874E63D20}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://leetcode-cn.com/problems/string-rotation-lcci" xr:uid="{75E626F9-C1B4-4ACC-8FC0-84C6CD3CF23D}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://leetcode-cn.com/problems/remove-duplicate-node-lcci" xr:uid="{B6DF184B-08EA-411E-91E0-83C90D97098B}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://leetcode-cn.com/problems/kth-node-from-end-of-list-lcci" xr:uid="{2D335B55-C4F4-4EC2-AA0E-84245FA91EA6}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://leetcode-cn.com/problems/delete-middle-node-lcci" xr:uid="{32932FCA-A4B6-4926-A277-2DBF968FB66F}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://leetcode-cn.com/problems/partition-list-lcci" xr:uid="{B3BB5593-453D-4B9A-ACD7-796A5A68895F}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://leetcode-cn.com/problems/sum-lists-lcci" xr:uid="{FF9325D2-355A-4B6A-99C1-A1507D7AA8C6}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://leetcode-cn.com/problems/palindrome-linked-list-lcci" xr:uid="{9D69124C-8275-48C5-89C6-47C06A7A226B}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://leetcode-cn.com/problems/intersection-of-two-linked-lists-lcci" xr:uid="{B2077538-5DC1-4718-ACD3-3CD39677C311}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://leetcode-cn.com/problems/linked-list-cycle-lcci" xr:uid="{8683A9A3-D47D-4ECD-A89C-30DB4235B322}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://leetcode-cn.com/problems/three-in-one-lcci" xr:uid="{16A71F7A-0E5E-4A2F-9519-F1DCF8AE0A9C}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://leetcode-cn.com/problems/min-stack-lcci" xr:uid="{41B71FE5-16D7-4D2F-B01B-46203567C258}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://leetcode-cn.com/problems/stack-of-plates-lcci" xr:uid="{EA85FEC0-0658-46E8-AA7B-3A73A42E9CD0}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://leetcode-cn.com/problems/implement-queue-using-stacks-lcci" xr:uid="{7C364CD7-B3C4-44D2-A286-BC975B86E112}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://leetcode-cn.com/problems/sort-of-stacks-lcci" xr:uid="{91BF0172-A7F3-42AC-9962-8401A3E37B5B}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://leetcode-cn.com/problems/animal-shelter-lcci" xr:uid="{BE33DA3D-66F5-4848-B175-AC6D044ACFE2}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://leetcode-cn.com/problems/route-between-nodes-lcci" xr:uid="{C28C6B2C-3E5F-4DA3-9E4E-DF9536475314}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://leetcode-cn.com/problems/minimum-height-tree-lcci" xr:uid="{67D13540-FF3C-4489-BAED-66DA7709317D}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://leetcode-cn.com/problems/list-of-depth-lcci" xr:uid="{7036EF6D-E728-4AEA-B879-F0C023C884B6}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://leetcode-cn.com/problems/check-balance-lcci" xr:uid="{7FEE5AC8-7FBD-4D6E-9E53-9E1B19BFC3D7}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://leetcode-cn.com/problems/legal-binary-search-tree-lcci" xr:uid="{FB83AADB-12BE-4B14-AA18-72EB3F224ECC}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://leetcode-cn.com/problems/successor-lcci" xr:uid="{3A79340E-7A7F-4104-A79C-2B88D339BE1D}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://leetcode-cn.com/problems/first-common-ancestor-lcci" xr:uid="{7B105FA3-0BDA-402D-A47E-84E208984D86}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://leetcode-cn.com/problems/bst-sequences-lcci" xr:uid="{1E6C4BFF-3E92-4CE1-B9DA-67CD7D5FA8DB}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://leetcode-cn.com/problems/check-subtree-lcci" xr:uid="{5654310E-07E7-40C0-92A2-C1D32D014928}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://leetcode-cn.com/problems/paths-with-sum-lcci" xr:uid="{38839549-B0D3-459B-A535-D5E776555AD9}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://leetcode-cn.com/problems/insert-into-bits-lcci" xr:uid="{BBD266AD-2B1F-44AC-90B5-4719FAD4FC0A}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://leetcode-cn.com/problems/bianry-number-to-string-lcci" xr:uid="{326A058F-888D-49BC-8047-C7E90975BF8F}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://leetcode-cn.com/problems/reverse-bits-lcci" xr:uid="{EF74E6F3-82B2-4E0F-9DAE-9AEE2C919B59}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://leetcode-cn.com/problems/closed-number-lcci" xr:uid="{25D60044-C22A-4B7F-8C47-BACC6E36E49E}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://leetcode-cn.com/problems/convert-integer-lcci" xr:uid="{93B8B2FA-5B00-44C7-9CE7-AF4AA3058F0E}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://leetcode-cn.com/problems/exchange-lcci" xr:uid="{B075CBBE-02CE-41A2-96E8-82EF927A6D97}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://leetcode-cn.com/problems/draw-line-lcci" xr:uid="{E357632D-8E06-4853-8F86-A00DDEDAA067}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://leetcode-cn.com/problems/three-steps-problem-lcci" xr:uid="{92C63BFC-5378-42E5-98DB-EFF6CD2765F0}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://leetcode-cn.com/problems/robot-in-a-grid-lcci" xr:uid="{F9245D50-E6E9-4F27-B456-3B6F5A2B9B6D}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://leetcode-cn.com/problems/magic-index-lcci" xr:uid="{9D174FE5-BE18-4D10-8ACA-68AF645CED25}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://leetcode-cn.com/problems/power-set-lcci" xr:uid="{B4C5B35A-A4D3-4148-89C7-5BB0134E1A2C}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://leetcode-cn.com/problems/recursive-mulitply-lcci" xr:uid="{B7954E82-1AE1-46F6-B6E8-4E87236B0FB9}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://leetcode-cn.com/problems/hanota-lcci" xr:uid="{02C845D3-C541-43C6-8126-53596B4FE97C}"/>
+    <hyperlink ref="B49" r:id="rId47" display="https://leetcode-cn.com/problems/permutation-i-lcci" xr:uid="{F6DFAD70-604A-42B0-97A3-97F30C83ABDE}"/>
+    <hyperlink ref="B50" r:id="rId48" display="https://leetcode-cn.com/problems/permutation-ii-lcci" xr:uid="{8B64FD2C-A5AD-4EA1-8357-A9ADF2CF7A0E}"/>
+    <hyperlink ref="B51" r:id="rId49" display="https://leetcode-cn.com/problems/bracket-lcci" xr:uid="{151C1933-2408-4E04-8A9D-2C60CA2AED5F}"/>
+    <hyperlink ref="B52" r:id="rId50" display="https://leetcode-cn.com/problems/color-fill-lcci" xr:uid="{3D4A0143-5B32-4F5E-A7FD-958F4D7F20BC}"/>
+    <hyperlink ref="B53" r:id="rId51" display="https://leetcode-cn.com/problems/coin-lcci" xr:uid="{60620454-AA8A-4C73-BB5E-4651D5B4BF5D}"/>
+    <hyperlink ref="B54" r:id="rId52" display="https://leetcode-cn.com/problems/eight-queens-lcci" xr:uid="{EC46D030-DA0B-4F43-BC9D-782183396DF1}"/>
+    <hyperlink ref="B55" r:id="rId53" display="https://leetcode-cn.com/problems/pile-box-lcci" xr:uid="{B31CE329-5304-466A-B6BD-23B3B1C76D5C}"/>
+    <hyperlink ref="B56" r:id="rId54" display="https://leetcode-cn.com/problems/boolean-evaluation-lcci" xr:uid="{D1FC6764-ADB1-4188-87D0-1FC32AF8FCFB}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://leetcode-cn.com/problems/sorted-merge-lcci" xr:uid="{A26EB65E-AE99-487C-B30F-9DF54CB454C7}"/>
+    <hyperlink ref="B58" r:id="rId56" display="https://leetcode-cn.com/problems/group-anagrams-lcci" xr:uid="{8E72392C-CFA7-4D83-A95F-DCF988B9370D}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://leetcode-cn.com/problems/search-rotate-array-lcci" xr:uid="{CF8FE950-2200-48BB-BDB1-8429544AC371}"/>
+    <hyperlink ref="B60" r:id="rId58" display="https://leetcode-cn.com/problems/sparse-array-search-lcci" xr:uid="{A3280143-773F-48A5-BCAF-31B3103289F5}"/>
+    <hyperlink ref="B61" r:id="rId59" display="https://leetcode-cn.com/problems/sorted-matrix-search-lcci" xr:uid="{4679EDB6-17C7-4ADF-BD73-A4943A974E74}"/>
+    <hyperlink ref="B62" r:id="rId60" display="https://leetcode-cn.com/problems/rank-from-stream-lcci" xr:uid="{D0BA52FE-FA62-4DC5-B9DD-AB05974C8483}"/>
+    <hyperlink ref="B63" r:id="rId61" display="https://leetcode-cn.com/problems/peaks-and-valleys-lcci" xr:uid="{469F2ADA-EB5A-4C69-BF09-521D8FCE7060}"/>
+    <hyperlink ref="B64" r:id="rId62" display="https://leetcode-cn.com/problems/swap-numbers-lcci" xr:uid="{43FC9D7D-A5D1-4E1F-B654-14AF3FD61F69}"/>
+    <hyperlink ref="B65" r:id="rId63" display="https://leetcode-cn.com/problems/words-frequency-lcci" xr:uid="{FB1F45E1-EB24-4064-BC6C-A04EC9D58D40}"/>
+    <hyperlink ref="B66" r:id="rId64" display="https://leetcode-cn.com/problems/intersection-lcci" xr:uid="{6DB0B8DB-8B20-478C-AA61-6B3CABB16787}"/>
+    <hyperlink ref="B67" r:id="rId65" display="https://leetcode-cn.com/problems/tic-tac-toe-lcci" xr:uid="{6631C6D9-697A-4FB9-8F67-6381ABC8BBC1}"/>
+    <hyperlink ref="B68" r:id="rId66" display="https://leetcode-cn.com/problems/factorial-zeros-lcci" xr:uid="{EB2E2991-D43C-4F21-B3A4-5C8C70A44D2A}"/>
+    <hyperlink ref="B69" r:id="rId67" display="https://leetcode-cn.com/problems/smallest-difference-lcci" xr:uid="{4189AD0E-F488-4C87-906F-F7E0678D9632}"/>
+    <hyperlink ref="B70" r:id="rId68" display="https://leetcode-cn.com/problems/maximum-lcci" xr:uid="{D37124E5-F65C-402D-860B-617C0C80B687}"/>
+    <hyperlink ref="B71" r:id="rId69" display="https://leetcode-cn.com/problems/english-int-lcci" xr:uid="{5AF82742-D0B5-4F04-B2E9-D79264BE2D96}"/>
+    <hyperlink ref="B72" r:id="rId70" display="https://leetcode-cn.com/problems/operations-lcci" xr:uid="{63E0AF68-9AA1-47F8-B2CC-6130D2EDDE29}"/>
+    <hyperlink ref="B73" r:id="rId71" display="https://leetcode-cn.com/problems/living-people-lcci" xr:uid="{D710BEEB-FB7C-4B55-A6E8-F574781430AA}"/>
+    <hyperlink ref="B74" r:id="rId72" display="https://leetcode-cn.com/problems/diving-board-lcci" xr:uid="{7CB20116-A843-4EC9-AAE4-B576B510ECA8}"/>
+    <hyperlink ref="B75" r:id="rId73" display="https://leetcode-cn.com/problems/bisect-squares-lcci" xr:uid="{4B5489CA-A20B-41A4-8CA1-BBDB8B5A28CB}"/>
+    <hyperlink ref="B76" r:id="rId74" display="https://leetcode-cn.com/problems/best-line-lcci" xr:uid="{9698873B-AD9B-417C-915F-C118B01B1159}"/>
+    <hyperlink ref="B77" r:id="rId75" display="https://leetcode-cn.com/problems/master-mind-lcci" xr:uid="{4BE4B5F6-73B6-4B5E-975F-161F89B54708}"/>
+    <hyperlink ref="B78" r:id="rId76" display="https://leetcode-cn.com/problems/sub-sort-lcci" xr:uid="{89A4E8B0-D02D-4557-858E-DD3CA9165580}"/>
+    <hyperlink ref="B79" r:id="rId77" display="https://leetcode-cn.com/problems/contiguous-sequence-lcci" xr:uid="{5CCF6FBA-7DE4-45AF-9231-D9313C972AEA}"/>
+    <hyperlink ref="B80" r:id="rId78" display="https://leetcode-cn.com/problems/pattern-matching-lcci" xr:uid="{395FB40F-7682-4B89-AEDA-C5880E81AD5E}"/>
+    <hyperlink ref="B81" r:id="rId79" display="https://leetcode-cn.com/problems/pond-sizes-lcci" xr:uid="{6E2D58F4-D254-4928-A168-3B6EEA3B6E4D}"/>
+    <hyperlink ref="B82" r:id="rId80" display="https://leetcode-cn.com/problems/t9-lcci" xr:uid="{DA07B267-F7DB-46F6-979B-C2F883DE0454}"/>
+    <hyperlink ref="B83" r:id="rId81" display="https://leetcode-cn.com/problems/sum-swap-lcci" xr:uid="{7EB17C26-38AE-418F-9D65-DF4B6619444A}"/>
+    <hyperlink ref="B84" r:id="rId82" display="https://leetcode-cn.com/problems/langtons-ant-lcci" xr:uid="{F78BCB39-1E5D-4C24-ADEC-56316998B9B2}"/>
+    <hyperlink ref="B85" r:id="rId83" display="https://leetcode-cn.com/problems/pairs-with-sum-lcci" xr:uid="{1B9D93C6-2EE2-41B0-8B1E-47FE60D5A298}"/>
+    <hyperlink ref="B86" r:id="rId84" display="https://leetcode-cn.com/problems/lru-cache-lcci" xr:uid="{9B414F26-99FC-4B25-B02B-CCC508647EDE}"/>
+    <hyperlink ref="B87" r:id="rId85" display="https://leetcode-cn.com/problems/calculator-lcci" xr:uid="{E4BDC078-247B-42FC-84C3-19F1FAD929F7}"/>
+    <hyperlink ref="B88" r:id="rId86" display="https://leetcode-cn.com/problems/add-without-plus-lcci" xr:uid="{02C8DD3E-CB7A-415C-9D06-2A9B165A4A07}"/>
+    <hyperlink ref="B89" r:id="rId87" display="https://leetcode-cn.com/problems/missing-number-lcci" xr:uid="{5871C071-93D4-4CAA-8E0F-BF1BCE8CCC0D}"/>
+    <hyperlink ref="B90" r:id="rId88" display="https://leetcode-cn.com/problems/find-longest-subarray-lcci" xr:uid="{EE75AA24-AD4E-4B33-A69C-4DB5E2E6D6C3}"/>
+    <hyperlink ref="B91" r:id="rId89" display="https://leetcode-cn.com/problems/number-of-2s-in-range-lcci" xr:uid="{41E555F7-15F0-4930-98AC-AF53E453C55D}"/>
+    <hyperlink ref="B92" r:id="rId90" display="https://leetcode-cn.com/problems/baby-names-lcci" xr:uid="{0BF45C72-3F8F-4641-B10F-191B26DB63FF}"/>
+    <hyperlink ref="B93" r:id="rId91" display="https://leetcode-cn.com/problems/circus-tower-lcci" xr:uid="{A9E4A819-2C01-4E8F-BFED-1E8795E508DA}"/>
+    <hyperlink ref="B94" r:id="rId92" display="https://leetcode-cn.com/problems/get-kth-magic-number-lcci" xr:uid="{2A0EFA7D-F744-49CF-9CAA-DD0E5BF0387E}"/>
+    <hyperlink ref="B95" r:id="rId93" display="https://leetcode-cn.com/problems/find-majority-element-lcci" xr:uid="{1B8336E6-8051-4819-83A3-2C3628559D40}"/>
+    <hyperlink ref="B96" r:id="rId94" display="https://leetcode-cn.com/problems/find-closest-lcci" xr:uid="{BC76320B-12C4-48C8-A009-EBB55EF1933D}"/>
+    <hyperlink ref="B97" r:id="rId95" display="https://leetcode-cn.com/problems/binode-lcci" xr:uid="{F1BCB2F9-33D4-4584-9892-902E43D9A644}"/>
+    <hyperlink ref="B98" r:id="rId96" display="https://leetcode-cn.com/problems/re-space-lcci" xr:uid="{980A4797-78D5-4516-B2C4-1E4A32C814A2}"/>
+    <hyperlink ref="B99" r:id="rId97" display="https://leetcode-cn.com/problems/smallest-k-lcci" xr:uid="{9420EDED-D3B9-43A2-A100-D989CBB1604B}"/>
+    <hyperlink ref="B100" r:id="rId98" display="https://leetcode-cn.com/problems/longest-word-lcci" xr:uid="{8F2B59A7-6ADC-47E4-BAD1-13AFC3C0D7E0}"/>
+    <hyperlink ref="B101" r:id="rId99" display="https://leetcode-cn.com/problems/the-masseuse-lcci" xr:uid="{86A5A113-96E1-48BF-84A9-50A7B0748F89}"/>
+    <hyperlink ref="B102" r:id="rId100" display="https://leetcode-cn.com/problems/multi-search-lcci" xr:uid="{8B72DECA-92B4-4DF8-8591-D4B93237730A}"/>
+    <hyperlink ref="B103" r:id="rId101" display="https://leetcode-cn.com/problems/shortest-supersequence-lcci" xr:uid="{ECF4C719-7A41-4BAA-AE6A-38AD845FED2A}"/>
+    <hyperlink ref="B104" r:id="rId102" display="https://leetcode-cn.com/problems/missing-two-lcci" xr:uid="{589EF060-DDBE-42F7-999A-718452DDB0A6}"/>
+    <hyperlink ref="B105" r:id="rId103" display="https://leetcode-cn.com/problems/continuous-median-lcci" xr:uid="{A1A67E99-E8D5-4A1C-8299-EEBA924AA77F}"/>
+    <hyperlink ref="B106" r:id="rId104" display="https://leetcode-cn.com/problems/volume-of-histogram-lcci" xr:uid="{877FD415-8962-4351-A26B-E79F40846A2A}"/>
+    <hyperlink ref="B107" r:id="rId105" display="https://leetcode-cn.com/problems/word-transformer-lcci" xr:uid="{93500134-4C38-487D-AF8B-A453EF6A5F41}"/>
+    <hyperlink ref="B108" r:id="rId106" display="https://leetcode-cn.com/problems/max-black-square-lcci" xr:uid="{4CB8B84B-0434-4289-864E-2B8F6EB05BE9}"/>
+    <hyperlink ref="B109" r:id="rId107" display="https://leetcode-cn.com/problems/max-submatrix-lcci" xr:uid="{6CB09E9D-2A22-486F-BBBD-30285F51277B}"/>
+    <hyperlink ref="B110" r:id="rId108" display="https://leetcode-cn.com/problems/word-rectangle-lcci" xr:uid="{FBBA00A7-D7D2-4365-AB95-5568A0451AB3}"/>
+    <hyperlink ref="B111" r:id="rId109" display="https://leetcode-cn.com/problems/sparse-similarity-lcci" xr:uid="{A3B1D418-E51B-47DF-8F1D-86BABB239D06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId110"/>
@@ -31383,10 +31394,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3974A999-81B9-4707-8EBA-5693F79999D0}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31397,7 +31408,7 @@
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="39" t="s">
         <v>1710</v>
       </c>
@@ -31405,933 +31416,928 @@
       <c r="C1" s="39"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>3</v>
+      <c r="A3" s="3" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1712</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2497</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1711</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2497</v>
+      <c r="A4" s="4" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>1714</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1713</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>1715</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>1715</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>1716</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>1717</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>1717</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>1718</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
+      <c r="A7" s="3" t="s">
+        <v>1719</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>1719</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>1720</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>1722</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>1721</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>1722</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1724</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>1724</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="A10" s="4" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>1726</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>1725</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>1726</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1728</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>1727</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>1728</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>5</v>
+      <c r="A12" s="4" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1730</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>1729</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1730</v>
-      </c>
-      <c r="C13" s="4" t="s">
+      <c r="A13" s="3" t="s">
+        <v>1731</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1732</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>1731</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="A14" s="4" t="s">
+        <v>1733</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>1734</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>1733</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1734</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="A15" s="3" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1736</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>1735</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>1736</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
+      <c r="A16" s="4" t="s">
+        <v>1737</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>1738</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>1737</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>1738</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
+      <c r="A17" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1740</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>1739</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>1740</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>7</v>
+      <c r="A18" s="4" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>1742</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>1741</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="A19" s="3" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1744</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>1743</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>5</v>
+      <c r="A20" s="4" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>1745</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>10</v>
+      <c r="A21" s="3" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>1746</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
+      <c r="A22" s="4" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>1748</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>1749</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="A23" s="3" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>1750</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>1751</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="A24" s="4" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>1752</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="A25" s="3" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>1753</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>1754</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>5</v>
+      <c r="A26" s="4" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>7</v>
+      <c r="A27" s="3" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>1758</v>
-      </c>
-      <c r="C28" s="3" t="s">
+      <c r="A28" s="4" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>1760</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>1760</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="A29" s="3" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>1761</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>1762</v>
-      </c>
-      <c r="C30" s="3" t="s">
+      <c r="A30" s="4" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>1764</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>1763</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>1764</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>5</v>
+      <c r="A31" s="3" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1766</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>1765</v>
-      </c>
-      <c r="B32" s="9" t="s">
-        <v>1766</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="4" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>1767</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>1768</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>7</v>
+      <c r="A33" s="3" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>1769</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>1770</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>5</v>
+      <c r="A34" s="4" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1772</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="A35" s="3" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1774</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>1773</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>1774</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="A36" s="4" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>1776</v>
+      </c>
+      <c r="C36" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>1775</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>1776</v>
-      </c>
-      <c r="C37" s="4" t="s">
+      <c r="A37" s="3" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1778</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>1778</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="A38" s="4" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>1780</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>1780</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>7</v>
+      <c r="A39" s="3" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>1782</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>1781</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>1782</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>10</v>
+      <c r="A40" s="4" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>585</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>1783</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>585</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>7</v>
+      <c r="A41" s="3" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>1784</v>
-      </c>
-      <c r="B42" s="9" t="s">
-        <v>1785</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="A42" s="4" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>1787</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
-        <v>1786</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>1787</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>5</v>
+      <c r="A43" s="3" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1789</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>1788</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>1789</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>10</v>
+      <c r="A44" s="4" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
-        <v>1790</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>5</v>
+      <c r="A45" s="3" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1793</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>1792</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>1793</v>
-      </c>
-      <c r="C46" s="3" t="s">
+      <c r="A46" s="4" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>1795</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>1794</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>1795</v>
-      </c>
-      <c r="C47" s="4" t="s">
+      <c r="A47" s="3" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1797</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>1796</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>1797</v>
-      </c>
-      <c r="C48" s="3" t="s">
+      <c r="A48" s="4" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>1799</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>1798</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>1799</v>
-      </c>
-      <c r="C49" s="4" t="s">
+      <c r="A49" s="3" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1801</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>1800</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>1801</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="A50" s="4" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>1803</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
-        <v>1802</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>1803</v>
-      </c>
-      <c r="C51" s="4" t="s">
+      <c r="A51" s="3" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>1804</v>
-      </c>
-      <c r="B52" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>7</v>
+      <c r="A52" s="4" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>1805</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>1806</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>5</v>
+      <c r="A53" s="3" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>1807</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>1808</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>10</v>
+      <c r="A54" s="4" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>1810</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>1809</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>1810</v>
-      </c>
-      <c r="C55" s="4" t="s">
+      <c r="A55" s="3" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>1812</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>1811</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>1812</v>
-      </c>
-      <c r="C56" s="3" t="s">
+      <c r="A56" s="4" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>1814</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>1813</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>1814</v>
-      </c>
-      <c r="C57" s="4" t="s">
+      <c r="A57" s="3" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>1816</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>1815</v>
-      </c>
-      <c r="B58" s="9" t="s">
-        <v>1816</v>
-      </c>
-      <c r="C58" s="3" t="s">
+      <c r="A58" s="4" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>1818</v>
+      </c>
+      <c r="C58" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>1817</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>1818</v>
-      </c>
-      <c r="C59" s="4" t="s">
+      <c r="A59" s="3" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>1819</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>5</v>
+      <c r="A60" s="4" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>1821</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
-        <v>1820</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C61" s="4" t="s">
+      <c r="A61" s="3" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>1823</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>1822</v>
-      </c>
-      <c r="B62" s="9" t="s">
-        <v>1823</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>7</v>
+      <c r="A62" s="4" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>1825</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
-        <v>1824</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>1825</v>
-      </c>
-      <c r="C63" s="4" t="s">
+      <c r="A63" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>1827</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>1826</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>1827</v>
-      </c>
-      <c r="C64" s="3" t="s">
+      <c r="A64" s="4" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>1829</v>
+      </c>
+      <c r="C64" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>1828</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>1829</v>
-      </c>
-      <c r="C65" s="4" t="s">
+      <c r="A65" s="3" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>1831</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>1830</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>1831</v>
-      </c>
-      <c r="C66" s="3" t="s">
+      <c r="A66" s="4" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>1833</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>1832</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>1833</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>5</v>
+      <c r="A67" s="3" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>1834</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>1835</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>7</v>
+      <c r="A68" s="4" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>1837</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>1836</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>1837</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="A69" s="3" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>1839</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="3" t="s">
-        <v>1838</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>1839</v>
-      </c>
-      <c r="C70" s="3" t="s">
+      <c r="A70" s="4" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>1841</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>1840</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>1841</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>5</v>
+      <c r="A71" s="3" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>1843</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
-        <v>1842</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>1843</v>
-      </c>
-      <c r="C72" s="3" t="s">
+      <c r="A72" s="4" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>1845</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>1844</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>1845</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>7</v>
+      <c r="A73" s="3" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>1847</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="3" t="s">
-        <v>1846</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>1847</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="A74" s="4" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C74" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>1848</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>1849</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>5</v>
+      <c r="A75" s="3" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>1851</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="3" t="s">
-        <v>1850</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>1851</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="4" t="s">
+      <c r="A76" s="4" t="s">
         <v>1852</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="7" t="s">
+      <c r="C76" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
         <v>1853</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B77" s="11" t="s">
         <v>251</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:D3" xr:uid="{EC5A4BF5-830B-4D96-9F63-CD23D514A0FC}"/>
+  <autoFilter ref="A2:D77" xr:uid="{EC5A4BF5-830B-4D96-9F63-CD23D514A0FC}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="https://leetcode-cn.com/problems/shu-zu-zhong-zhong-fu-de-shu-zi-lcof" xr:uid="{72D31594-4607-407E-9D7A-8FCEFD3AF5D0}"/>
-    <hyperlink ref="B5" r:id="rId2" display="https://leetcode-cn.com/problems/er-wei-shu-zu-zhong-de-cha-zhao-lcof" xr:uid="{FEF58301-241B-4A62-B190-DDB7942731FE}"/>
-    <hyperlink ref="B6" r:id="rId3" display="https://leetcode-cn.com/problems/ti-huan-kong-ge-lcof" xr:uid="{5CF4076E-720A-4EEF-A405-97626B91CEE4}"/>
-    <hyperlink ref="B7" r:id="rId4" display="https://leetcode-cn.com/problems/cong-wei-dao-tou-da-yin-lian-biao-lcof" xr:uid="{4E1999BD-EC6A-40A5-A38B-93A63D1C7DF2}"/>
-    <hyperlink ref="B8" r:id="rId5" display="https://leetcode-cn.com/problems/zhong-jian-er-cha-shu-lcof" xr:uid="{D661990F-C1B4-4B88-8704-75A2C6313DA9}"/>
-    <hyperlink ref="B9" r:id="rId6" display="https://leetcode-cn.com/problems/yong-liang-ge-zhan-shi-xian-dui-lie-lcof" xr:uid="{0802D550-03EB-4920-8A59-2C4A91C6C43A}"/>
-    <hyperlink ref="B10" r:id="rId7" display="https://leetcode-cn.com/problems/fei-bo-na-qi-shu-lie-lcof" xr:uid="{FF2BA3C6-18C5-4C18-9EE4-0EC0DFAC97E2}"/>
-    <hyperlink ref="B11" r:id="rId8" display="https://leetcode-cn.com/problems/qing-wa-tiao-tai-jie-wen-ti-lcof" xr:uid="{B25E8A91-981A-461F-82F2-94AE68E9BA5A}"/>
-    <hyperlink ref="B12" r:id="rId9" display="https://leetcode-cn.com/problems/xuan-zhuan-shu-zu-de-zui-xiao-shu-zi-lcof" xr:uid="{F8CBFE42-4D9E-43E6-9ACF-3176EE8A1B9E}"/>
-    <hyperlink ref="B13" r:id="rId10" display="https://leetcode-cn.com/problems/ju-zhen-zhong-de-lu-jing-lcof" xr:uid="{6BD212E3-F970-4F77-9DBD-CB1473B26574}"/>
-    <hyperlink ref="B14" r:id="rId11" display="https://leetcode-cn.com/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof" xr:uid="{E14969FE-545A-466F-A3DD-A71785F35CBC}"/>
-    <hyperlink ref="B15" r:id="rId12" display="https://leetcode-cn.com/problems/jian-sheng-zi-lcof" xr:uid="{F89CBD3C-3D82-4199-ACBB-6859B8C9AF44}"/>
-    <hyperlink ref="B16" r:id="rId13" display="https://leetcode-cn.com/problems/jian-sheng-zi-ii-lcof" xr:uid="{2FEC314D-469D-4552-9B1E-C9A4E57409D1}"/>
-    <hyperlink ref="B17" r:id="rId14" display="https://leetcode-cn.com/problems/er-jin-zhi-zhong-1de-ge-shu-lcof" xr:uid="{B8E21C0A-E74A-4B6C-BDCF-8395FA3DC6E2}"/>
-    <hyperlink ref="B18" r:id="rId15" display="https://leetcode-cn.com/problems/shu-zhi-de-zheng-shu-ci-fang-lcof" xr:uid="{8A8781F1-9368-40E7-BBE3-82A283154FA7}"/>
-    <hyperlink ref="B19" r:id="rId16" display="https://leetcode-cn.com/problems/da-yin-cong-1dao-zui-da-de-nwei-shu-lcof" xr:uid="{60831753-1E8D-43C0-9434-AA317BDE53F1}"/>
-    <hyperlink ref="B20" r:id="rId17" display="https://leetcode-cn.com/problems/shan-chu-lian-biao-de-jie-dian-lcof" xr:uid="{DAF41D0C-ED86-43D4-8EE4-868508FF7962}"/>
-    <hyperlink ref="B21" r:id="rId18" display="https://leetcode-cn.com/problems/zheng-ze-biao-da-shi-pi-pei-lcof" xr:uid="{6D0901B2-76F3-4FEF-8D66-FA02C43F0FF5}"/>
-    <hyperlink ref="B22" r:id="rId19" display="https://leetcode-cn.com/problems/biao-shi-shu-zhi-de-zi-fu-chuan-lcof" xr:uid="{742BE26B-4F22-4951-A68F-726DD427185D}"/>
-    <hyperlink ref="B23" r:id="rId20" display="https://leetcode-cn.com/problems/diao-zheng-shu-zu-shun-xu-shi-qi-shu-wei-yu-ou-shu-qian-mian-lcof" xr:uid="{50F7C033-54C8-4AC1-ADAD-10C8111C8DBF}"/>
-    <hyperlink ref="B24" r:id="rId21" display="https://leetcode-cn.com/problems/lian-biao-zhong-dao-shu-di-kge-jie-dian-lcof" xr:uid="{BEFF6510-D937-4321-AFC4-75ED7A96C623}"/>
-    <hyperlink ref="B25" r:id="rId22" display="https://leetcode-cn.com/problems/fan-zhuan-lian-biao-lcof" xr:uid="{CC0EFFFC-DE4D-4C21-AF35-C5439A079C1B}"/>
-    <hyperlink ref="B26" r:id="rId23" display="https://leetcode-cn.com/problems/he-bing-liang-ge-pai-xu-de-lian-biao-lcof" xr:uid="{465986D0-E756-48BA-A12A-87FB66BF60BD}"/>
-    <hyperlink ref="B27" r:id="rId24" display="https://leetcode-cn.com/problems/shu-de-zi-jie-gou-lcof" xr:uid="{AA3DC36F-39AB-4A44-BEDF-DAA8CDB41FF8}"/>
-    <hyperlink ref="B28" r:id="rId25" display="https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof" xr:uid="{D825747A-3DC7-4290-967D-8472B710C899}"/>
-    <hyperlink ref="B29" r:id="rId26" display="https://leetcode-cn.com/problems/dui-cheng-de-er-cha-shu-lcof" xr:uid="{2745C15A-56BD-46D0-AF19-8B26DAA0B4DF}"/>
-    <hyperlink ref="B30" r:id="rId27" display="https://leetcode-cn.com/problems/shun-shi-zhen-da-yin-ju-zhen-lcof" xr:uid="{6C5D5BEE-BA35-49F2-9636-AD4AEC903B17}"/>
-    <hyperlink ref="B31" r:id="rId28" display="https://leetcode-cn.com/problems/bao-han-minhan-shu-de-zhan-lcof" xr:uid="{DBD30F17-C2E8-4701-B465-5A2DEEF24956}"/>
-    <hyperlink ref="B32" r:id="rId29" display="https://leetcode-cn.com/problems/zhan-de-ya-ru-dan-chu-xu-lie-lcof" xr:uid="{27531A6F-5866-48DF-8139-013DC23CEC4F}"/>
-    <hyperlink ref="B33" r:id="rId30" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-lcof" xr:uid="{3FBC6143-46A6-4875-A26C-D7774B935CEB}"/>
-    <hyperlink ref="B34" r:id="rId31" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-ii-lcof" xr:uid="{456E6F4B-2CFE-4FE0-9278-78EB353CBC59}"/>
-    <hyperlink ref="B35" r:id="rId32" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-iii-lcof" xr:uid="{F0D404ED-91F9-4CE5-BA10-E3AF6C8656AC}"/>
-    <hyperlink ref="B36" r:id="rId33" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-hou-xu-bian-li-xu-lie-lcof" xr:uid="{9056E135-065B-479E-864B-3A3340415442}"/>
-    <hyperlink ref="B37" r:id="rId34" display="https://leetcode-cn.com/problems/er-cha-shu-zhong-he-wei-mou-yi-zhi-de-lu-jing-lcof" xr:uid="{08E9089C-EE30-4D81-9F92-5C475B27094C}"/>
-    <hyperlink ref="B38" r:id="rId35" display="https://leetcode-cn.com/problems/fu-za-lian-biao-de-fu-zhi-lcof" xr:uid="{14FDD468-B9C2-496E-AD6A-A3ACB538D3D4}"/>
-    <hyperlink ref="B39" r:id="rId36" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-yu-shuang-xiang-lian-biao-lcof" xr:uid="{AF63E0B3-5D94-4E6F-9B09-D00637A83A45}"/>
-    <hyperlink ref="B40" r:id="rId37" display="https://leetcode-cn.com/problems/xu-lie-hua-er-cha-shu-lcof" xr:uid="{B3B9C22B-84E3-4580-A684-E871F3284EAD}"/>
-    <hyperlink ref="B41" r:id="rId38" display="https://leetcode-cn.com/problems/zi-fu-chuan-de-pai-lie-lcof" xr:uid="{AEA41E3D-AE80-418C-B46E-F41A50890E30}"/>
-    <hyperlink ref="B42" r:id="rId39" display="https://leetcode-cn.com/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof" xr:uid="{359D1099-8C8A-40C6-A25B-23450F07CD15}"/>
-    <hyperlink ref="B43" r:id="rId40" display="https://leetcode-cn.com/problems/zui-xiao-de-kge-shu-lcof" xr:uid="{E7C7A5AD-B859-4E5E-86B1-359F00FEDDAD}"/>
-    <hyperlink ref="B44" r:id="rId41" display="https://leetcode-cn.com/problems/shu-ju-liu-zhong-de-zhong-wei-shu-lcof" xr:uid="{54A861A7-11B0-42E9-BA02-722EF6C3E8D7}"/>
-    <hyperlink ref="B45" r:id="rId42" display="https://leetcode-cn.com/problems/lian-xu-zi-shu-zu-de-zui-da-he-lcof" xr:uid="{8ECEA71D-F430-4E18-8C69-093B138157A1}"/>
-    <hyperlink ref="B46" r:id="rId43" display="https://leetcode-cn.com/problems/1nzheng-shu-zhong-1chu-xian-de-ci-shu-lcof" xr:uid="{6291261D-51DC-4CB0-B1F5-A2F918901A54}"/>
-    <hyperlink ref="B47" r:id="rId44" display="https://leetcode-cn.com/problems/shu-zi-xu-lie-zhong-mou-yi-wei-de-shu-zi-lcof" xr:uid="{D5F4EC7E-9AA3-4067-81A0-89D9ADDA376D}"/>
-    <hyperlink ref="B48" r:id="rId45" display="https://leetcode-cn.com/problems/ba-shu-zu-pai-cheng-zui-xiao-de-shu-lcof" xr:uid="{E2E38022-6009-4E33-A8D4-8848F5FD81C1}"/>
-    <hyperlink ref="B49" r:id="rId46" display="https://leetcode-cn.com/problems/ba-shu-zi-fan-yi-cheng-zi-fu-chuan-lcof" xr:uid="{46F8BEEF-FB20-4612-8D81-4292365F93A1}"/>
-    <hyperlink ref="B50" r:id="rId47" display="https://leetcode-cn.com/problems/li-wu-de-zui-da-jie-zhi-lcof" xr:uid="{0715D293-5E59-4C33-BB53-97995774BAC5}"/>
-    <hyperlink ref="B51" r:id="rId48" display="https://leetcode-cn.com/problems/zui-chang-bu-han-zhong-fu-zi-fu-de-zi-zi-fu-chuan-lcof" xr:uid="{D538A808-29AB-4805-8914-0CE89A5539F9}"/>
-    <hyperlink ref="B52" r:id="rId49" display="https://leetcode-cn.com/problems/chou-shu-lcof" xr:uid="{8D401D28-FDA4-4247-B064-127A605F4647}"/>
-    <hyperlink ref="B53" r:id="rId50" display="https://leetcode-cn.com/problems/di-yi-ge-zhi-chu-xian-yi-ci-de-zi-fu-lcof" xr:uid="{22F879CD-9FB8-4A5B-BCAE-890A1D84C614}"/>
-    <hyperlink ref="B54" r:id="rId51" display="https://leetcode-cn.com/problems/shu-zu-zhong-de-ni-xu-dui-lcof" xr:uid="{D942AB72-33C5-4DD0-9B55-809609CBA4A3}"/>
-    <hyperlink ref="B55" r:id="rId52" display="https://leetcode-cn.com/problems/liang-ge-lian-biao-de-di-yi-ge-gong-gong-jie-dian-lcof" xr:uid="{AA841958-C6AE-4439-9DF5-C4E53EE53185}"/>
-    <hyperlink ref="B56" r:id="rId53" display="https://leetcode-cn.com/problems/zai-pai-xu-shu-zu-zhong-cha-zhao-shu-zi-lcof" xr:uid="{8A7B0C49-A4C2-4B08-9CB0-406638957798}"/>
-    <hyperlink ref="B57" r:id="rId54" display="https://leetcode-cn.com/problems/que-shi-de-shu-zi-lcof" xr:uid="{A3C968F8-61B3-4B11-94C1-3C6D9FB4F076}"/>
-    <hyperlink ref="B58" r:id="rId55" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-di-kda-jie-dian-lcof" xr:uid="{127771CE-A1B1-4D07-A0AC-69CEB5A5DC43}"/>
-    <hyperlink ref="B59" r:id="rId56" display="https://leetcode-cn.com/problems/er-cha-shu-de-shen-du-lcof" xr:uid="{8B2DFFB3-ACAD-4D95-A5FE-559ADAA9F2C7}"/>
-    <hyperlink ref="B60" r:id="rId57" display="https://leetcode-cn.com/problems/ping-heng-er-cha-shu-lcof" xr:uid="{4A846F3B-1DAD-4069-9FC8-93548969D7BC}"/>
-    <hyperlink ref="B61" r:id="rId58" display="https://leetcode-cn.com/problems/shu-zu-zhong-shu-zi-chu-xian-de-ci-shu-lcof" xr:uid="{3086BEA4-94EA-49D1-97EF-90C6DE5A7241}"/>
-    <hyperlink ref="B62" r:id="rId59" display="https://leetcode-cn.com/problems/shu-zu-zhong-shu-zi-chu-xian-de-ci-shu-ii-lcof" xr:uid="{102EB7B3-0D9A-4CA8-91FE-8F201D225D14}"/>
-    <hyperlink ref="B63" r:id="rId60" display="https://leetcode-cn.com/problems/he-wei-sde-liang-ge-shu-zi-lcof" xr:uid="{FBB52087-47FE-4DF7-8D20-FE8818CB989A}"/>
-    <hyperlink ref="B64" r:id="rId61" display="https://leetcode-cn.com/problems/he-wei-sde-lian-xu-zheng-shu-xu-lie-lcof" xr:uid="{410772D6-40B7-4D4D-98C3-6C0540682497}"/>
-    <hyperlink ref="B65" r:id="rId62" display="https://leetcode-cn.com/problems/fan-zhuan-dan-ci-shun-xu-lcof" xr:uid="{AB0A3147-6B7A-4899-BF91-A348D6E32A05}"/>
-    <hyperlink ref="B66" r:id="rId63" display="https://leetcode-cn.com/problems/zuo-xuan-zhuan-zi-fu-chuan-lcof" xr:uid="{BF20F806-3587-4F64-BB27-5AB3CC250706}"/>
-    <hyperlink ref="B67" r:id="rId64" display="https://leetcode-cn.com/problems/hua-dong-chuang-kou-de-zui-da-zhi-lcof" xr:uid="{6B9961D5-54F2-49DF-A8EC-BE3A5685C50C}"/>
-    <hyperlink ref="B68" r:id="rId65" display="https://leetcode-cn.com/problems/dui-lie-de-zui-da-zhi-lcof" xr:uid="{CE7D320D-7BC6-4A76-A2B9-583E218A18FA}"/>
-    <hyperlink ref="B69" r:id="rId66" display="https://leetcode-cn.com/problems/nge-tou-zi-de-dian-shu-lcof" xr:uid="{D94C929E-2157-47CC-A48E-A4C23FCDC2FE}"/>
-    <hyperlink ref="B70" r:id="rId67" display="https://leetcode-cn.com/problems/bu-ke-pai-zhong-de-shun-zi-lcof" xr:uid="{FE7D2019-A779-4473-AB88-9B4B39641957}"/>
-    <hyperlink ref="B71" r:id="rId68" display="https://leetcode-cn.com/problems/yuan-quan-zhong-zui-hou-sheng-xia-de-shu-zi-lcof" xr:uid="{F319127C-F0E2-43D7-A9BD-0730BBF25976}"/>
-    <hyperlink ref="B72" r:id="rId69" display="https://leetcode-cn.com/problems/gu-piao-de-zui-da-li-run-lcof" xr:uid="{A8CBF796-20AA-4D4A-B1EC-7C40DE03AD8B}"/>
-    <hyperlink ref="B73" r:id="rId70" display="https://leetcode-cn.com/problems/qiu-12n-lcof" xr:uid="{C1E0137A-BA46-45E7-B6B1-6B719AB179D0}"/>
-    <hyperlink ref="B74" r:id="rId71" display="https://leetcode-cn.com/problems/bu-yong-jia-jian-cheng-chu-zuo-jia-fa-lcof" xr:uid="{70868E24-A8A9-4E58-8FC7-F673AFD16A77}"/>
-    <hyperlink ref="B75" r:id="rId72" display="https://leetcode-cn.com/problems/gou-jian-cheng-ji-shu-zu-lcof" xr:uid="{528E1A99-21AB-4BC2-ACDE-F38962C08BD3}"/>
-    <hyperlink ref="B76" r:id="rId73" display="https://leetcode-cn.com/problems/ba-zi-fu-chuan-zhuan-huan-cheng-zheng-shu-lcof" xr:uid="{C28D6499-074A-4298-B56B-4B1A8AA4916B}"/>
-    <hyperlink ref="B77" r:id="rId74" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-zui-jin-gong-gong-zu-xian-lcof" xr:uid="{24DE338F-690B-420B-913B-C6D99FBE592E}"/>
-    <hyperlink ref="B78" r:id="rId75" display="https://leetcode-cn.com/problems/er-cha-shu-de-zui-jin-gong-gong-zu-xian-lcof" xr:uid="{35FF0319-BBA2-492F-8458-45AAEEA67F96}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://leetcode-cn.com/problems/shu-zu-zhong-zhong-fu-de-shu-zi-lcof" xr:uid="{72D31594-4607-407E-9D7A-8FCEFD3AF5D0}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://leetcode-cn.com/problems/er-wei-shu-zu-zhong-de-cha-zhao-lcof" xr:uid="{FEF58301-241B-4A62-B190-DDB7942731FE}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://leetcode-cn.com/problems/ti-huan-kong-ge-lcof" xr:uid="{5CF4076E-720A-4EEF-A405-97626B91CEE4}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://leetcode-cn.com/problems/cong-wei-dao-tou-da-yin-lian-biao-lcof" xr:uid="{4E1999BD-EC6A-40A5-A38B-93A63D1C7DF2}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://leetcode-cn.com/problems/zhong-jian-er-cha-shu-lcof" xr:uid="{D661990F-C1B4-4B88-8704-75A2C6313DA9}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://leetcode-cn.com/problems/yong-liang-ge-zhan-shi-xian-dui-lie-lcof" xr:uid="{0802D550-03EB-4920-8A59-2C4A91C6C43A}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://leetcode-cn.com/problems/fei-bo-na-qi-shu-lie-lcof" xr:uid="{FF2BA3C6-18C5-4C18-9EE4-0EC0DFAC97E2}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://leetcode-cn.com/problems/qing-wa-tiao-tai-jie-wen-ti-lcof" xr:uid="{B25E8A91-981A-461F-82F2-94AE68E9BA5A}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://leetcode-cn.com/problems/xuan-zhuan-shu-zu-de-zui-xiao-shu-zi-lcof" xr:uid="{F8CBFE42-4D9E-43E6-9ACF-3176EE8A1B9E}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://leetcode-cn.com/problems/ju-zhen-zhong-de-lu-jing-lcof" xr:uid="{6BD212E3-F970-4F77-9DBD-CB1473B26574}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://leetcode-cn.com/problems/ji-qi-ren-de-yun-dong-fan-wei-lcof" xr:uid="{E14969FE-545A-466F-A3DD-A71785F35CBC}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://leetcode-cn.com/problems/jian-sheng-zi-lcof" xr:uid="{F89CBD3C-3D82-4199-ACBB-6859B8C9AF44}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://leetcode-cn.com/problems/jian-sheng-zi-ii-lcof" xr:uid="{2FEC314D-469D-4552-9B1E-C9A4E57409D1}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://leetcode-cn.com/problems/er-jin-zhi-zhong-1de-ge-shu-lcof" xr:uid="{B8E21C0A-E74A-4B6C-BDCF-8395FA3DC6E2}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://leetcode-cn.com/problems/shu-zhi-de-zheng-shu-ci-fang-lcof" xr:uid="{8A8781F1-9368-40E7-BBE3-82A283154FA7}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://leetcode-cn.com/problems/da-yin-cong-1dao-zui-da-de-nwei-shu-lcof" xr:uid="{60831753-1E8D-43C0-9434-AA317BDE53F1}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://leetcode-cn.com/problems/shan-chu-lian-biao-de-jie-dian-lcof" xr:uid="{DAF41D0C-ED86-43D4-8EE4-868508FF7962}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://leetcode-cn.com/problems/zheng-ze-biao-da-shi-pi-pei-lcof" xr:uid="{6D0901B2-76F3-4FEF-8D66-FA02C43F0FF5}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://leetcode-cn.com/problems/biao-shi-shu-zhi-de-zi-fu-chuan-lcof" xr:uid="{742BE26B-4F22-4951-A68F-726DD427185D}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://leetcode-cn.com/problems/diao-zheng-shu-zu-shun-xu-shi-qi-shu-wei-yu-ou-shu-qian-mian-lcof" xr:uid="{50F7C033-54C8-4AC1-ADAD-10C8111C8DBF}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://leetcode-cn.com/problems/lian-biao-zhong-dao-shu-di-kge-jie-dian-lcof" xr:uid="{BEFF6510-D937-4321-AFC4-75ED7A96C623}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://leetcode-cn.com/problems/fan-zhuan-lian-biao-lcof" xr:uid="{CC0EFFFC-DE4D-4C21-AF35-C5439A079C1B}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://leetcode-cn.com/problems/he-bing-liang-ge-pai-xu-de-lian-biao-lcof" xr:uid="{465986D0-E756-48BA-A12A-87FB66BF60BD}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://leetcode-cn.com/problems/shu-de-zi-jie-gou-lcof" xr:uid="{AA3DC36F-39AB-4A44-BEDF-DAA8CDB41FF8}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://leetcode-cn.com/problems/er-cha-shu-de-jing-xiang-lcof" xr:uid="{D825747A-3DC7-4290-967D-8472B710C899}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://leetcode-cn.com/problems/dui-cheng-de-er-cha-shu-lcof" xr:uid="{2745C15A-56BD-46D0-AF19-8B26DAA0B4DF}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://leetcode-cn.com/problems/shun-shi-zhen-da-yin-ju-zhen-lcof" xr:uid="{6C5D5BEE-BA35-49F2-9636-AD4AEC903B17}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://leetcode-cn.com/problems/bao-han-minhan-shu-de-zhan-lcof" xr:uid="{DBD30F17-C2E8-4701-B465-5A2DEEF24956}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://leetcode-cn.com/problems/zhan-de-ya-ru-dan-chu-xu-lie-lcof" xr:uid="{27531A6F-5866-48DF-8139-013DC23CEC4F}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-lcof" xr:uid="{3FBC6143-46A6-4875-A26C-D7774B935CEB}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-ii-lcof" xr:uid="{456E6F4B-2CFE-4FE0-9278-78EB353CBC59}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://leetcode-cn.com/problems/cong-shang-dao-xia-da-yin-er-cha-shu-iii-lcof" xr:uid="{F0D404ED-91F9-4CE5-BA10-E3AF6C8656AC}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-hou-xu-bian-li-xu-lie-lcof" xr:uid="{9056E135-065B-479E-864B-3A3340415442}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://leetcode-cn.com/problems/er-cha-shu-zhong-he-wei-mou-yi-zhi-de-lu-jing-lcof" xr:uid="{08E9089C-EE30-4D81-9F92-5C475B27094C}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://leetcode-cn.com/problems/fu-za-lian-biao-de-fu-zhi-lcof" xr:uid="{14FDD468-B9C2-496E-AD6A-A3ACB538D3D4}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-yu-shuang-xiang-lian-biao-lcof" xr:uid="{AF63E0B3-5D94-4E6F-9B09-D00637A83A45}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://leetcode-cn.com/problems/xu-lie-hua-er-cha-shu-lcof" xr:uid="{B3B9C22B-84E3-4580-A684-E871F3284EAD}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://leetcode-cn.com/problems/zi-fu-chuan-de-pai-lie-lcof" xr:uid="{AEA41E3D-AE80-418C-B46E-F41A50890E30}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://leetcode-cn.com/problems/shu-zu-zhong-chu-xian-ci-shu-chao-guo-yi-ban-de-shu-zi-lcof" xr:uid="{359D1099-8C8A-40C6-A25B-23450F07CD15}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://leetcode-cn.com/problems/zui-xiao-de-kge-shu-lcof" xr:uid="{E7C7A5AD-B859-4E5E-86B1-359F00FEDDAD}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://leetcode-cn.com/problems/shu-ju-liu-zhong-de-zhong-wei-shu-lcof" xr:uid="{54A861A7-11B0-42E9-BA02-722EF6C3E8D7}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://leetcode-cn.com/problems/lian-xu-zi-shu-zu-de-zui-da-he-lcof" xr:uid="{8ECEA71D-F430-4E18-8C69-093B138157A1}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://leetcode-cn.com/problems/1nzheng-shu-zhong-1chu-xian-de-ci-shu-lcof" xr:uid="{6291261D-51DC-4CB0-B1F5-A2F918901A54}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://leetcode-cn.com/problems/shu-zi-xu-lie-zhong-mou-yi-wei-de-shu-zi-lcof" xr:uid="{D5F4EC7E-9AA3-4067-81A0-89D9ADDA376D}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://leetcode-cn.com/problems/ba-shu-zu-pai-cheng-zui-xiao-de-shu-lcof" xr:uid="{E2E38022-6009-4E33-A8D4-8848F5FD81C1}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://leetcode-cn.com/problems/ba-shu-zi-fan-yi-cheng-zi-fu-chuan-lcof" xr:uid="{46F8BEEF-FB20-4612-8D81-4292365F93A1}"/>
+    <hyperlink ref="B49" r:id="rId47" display="https://leetcode-cn.com/problems/li-wu-de-zui-da-jie-zhi-lcof" xr:uid="{0715D293-5E59-4C33-BB53-97995774BAC5}"/>
+    <hyperlink ref="B50" r:id="rId48" display="https://leetcode-cn.com/problems/zui-chang-bu-han-zhong-fu-zi-fu-de-zi-zi-fu-chuan-lcof" xr:uid="{D538A808-29AB-4805-8914-0CE89A5539F9}"/>
+    <hyperlink ref="B51" r:id="rId49" display="https://leetcode-cn.com/problems/chou-shu-lcof" xr:uid="{8D401D28-FDA4-4247-B064-127A605F4647}"/>
+    <hyperlink ref="B52" r:id="rId50" display="https://leetcode-cn.com/problems/di-yi-ge-zhi-chu-xian-yi-ci-de-zi-fu-lcof" xr:uid="{22F879CD-9FB8-4A5B-BCAE-890A1D84C614}"/>
+    <hyperlink ref="B53" r:id="rId51" display="https://leetcode-cn.com/problems/shu-zu-zhong-de-ni-xu-dui-lcof" xr:uid="{D942AB72-33C5-4DD0-9B55-809609CBA4A3}"/>
+    <hyperlink ref="B54" r:id="rId52" display="https://leetcode-cn.com/problems/liang-ge-lian-biao-de-di-yi-ge-gong-gong-jie-dian-lcof" xr:uid="{AA841958-C6AE-4439-9DF5-C4E53EE53185}"/>
+    <hyperlink ref="B55" r:id="rId53" display="https://leetcode-cn.com/problems/zai-pai-xu-shu-zu-zhong-cha-zhao-shu-zi-lcof" xr:uid="{8A7B0C49-A4C2-4B08-9CB0-406638957798}"/>
+    <hyperlink ref="B56" r:id="rId54" display="https://leetcode-cn.com/problems/que-shi-de-shu-zi-lcof" xr:uid="{A3C968F8-61B3-4B11-94C1-3C6D9FB4F076}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-di-kda-jie-dian-lcof" xr:uid="{127771CE-A1B1-4D07-A0AC-69CEB5A5DC43}"/>
+    <hyperlink ref="B58" r:id="rId56" display="https://leetcode-cn.com/problems/er-cha-shu-de-shen-du-lcof" xr:uid="{8B2DFFB3-ACAD-4D95-A5FE-559ADAA9F2C7}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://leetcode-cn.com/problems/ping-heng-er-cha-shu-lcof" xr:uid="{4A846F3B-1DAD-4069-9FC8-93548969D7BC}"/>
+    <hyperlink ref="B60" r:id="rId58" display="https://leetcode-cn.com/problems/shu-zu-zhong-shu-zi-chu-xian-de-ci-shu-lcof" xr:uid="{3086BEA4-94EA-49D1-97EF-90C6DE5A7241}"/>
+    <hyperlink ref="B61" r:id="rId59" display="https://leetcode-cn.com/problems/shu-zu-zhong-shu-zi-chu-xian-de-ci-shu-ii-lcof" xr:uid="{102EB7B3-0D9A-4CA8-91FE-8F201D225D14}"/>
+    <hyperlink ref="B62" r:id="rId60" display="https://leetcode-cn.com/problems/he-wei-sde-liang-ge-shu-zi-lcof" xr:uid="{FBB52087-47FE-4DF7-8D20-FE8818CB989A}"/>
+    <hyperlink ref="B63" r:id="rId61" display="https://leetcode-cn.com/problems/he-wei-sde-lian-xu-zheng-shu-xu-lie-lcof" xr:uid="{410772D6-40B7-4D4D-98C3-6C0540682497}"/>
+    <hyperlink ref="B64" r:id="rId62" display="https://leetcode-cn.com/problems/fan-zhuan-dan-ci-shun-xu-lcof" xr:uid="{AB0A3147-6B7A-4899-BF91-A348D6E32A05}"/>
+    <hyperlink ref="B65" r:id="rId63" display="https://leetcode-cn.com/problems/zuo-xuan-zhuan-zi-fu-chuan-lcof" xr:uid="{BF20F806-3587-4F64-BB27-5AB3CC250706}"/>
+    <hyperlink ref="B66" r:id="rId64" display="https://leetcode-cn.com/problems/hua-dong-chuang-kou-de-zui-da-zhi-lcof" xr:uid="{6B9961D5-54F2-49DF-A8EC-BE3A5685C50C}"/>
+    <hyperlink ref="B67" r:id="rId65" display="https://leetcode-cn.com/problems/dui-lie-de-zui-da-zhi-lcof" xr:uid="{CE7D320D-7BC6-4A76-A2B9-583E218A18FA}"/>
+    <hyperlink ref="B68" r:id="rId66" display="https://leetcode-cn.com/problems/nge-tou-zi-de-dian-shu-lcof" xr:uid="{D94C929E-2157-47CC-A48E-A4C23FCDC2FE}"/>
+    <hyperlink ref="B69" r:id="rId67" display="https://leetcode-cn.com/problems/bu-ke-pai-zhong-de-shun-zi-lcof" xr:uid="{FE7D2019-A779-4473-AB88-9B4B39641957}"/>
+    <hyperlink ref="B70" r:id="rId68" display="https://leetcode-cn.com/problems/yuan-quan-zhong-zui-hou-sheng-xia-de-shu-zi-lcof" xr:uid="{F319127C-F0E2-43D7-A9BD-0730BBF25976}"/>
+    <hyperlink ref="B71" r:id="rId69" display="https://leetcode-cn.com/problems/gu-piao-de-zui-da-li-run-lcof" xr:uid="{A8CBF796-20AA-4D4A-B1EC-7C40DE03AD8B}"/>
+    <hyperlink ref="B72" r:id="rId70" display="https://leetcode-cn.com/problems/qiu-12n-lcof" xr:uid="{C1E0137A-BA46-45E7-B6B1-6B719AB179D0}"/>
+    <hyperlink ref="B73" r:id="rId71" display="https://leetcode-cn.com/problems/bu-yong-jia-jian-cheng-chu-zuo-jia-fa-lcof" xr:uid="{70868E24-A8A9-4E58-8FC7-F673AFD16A77}"/>
+    <hyperlink ref="B74" r:id="rId72" display="https://leetcode-cn.com/problems/gou-jian-cheng-ji-shu-zu-lcof" xr:uid="{528E1A99-21AB-4BC2-ACDE-F38962C08BD3}"/>
+    <hyperlink ref="B75" r:id="rId73" display="https://leetcode-cn.com/problems/ba-zi-fu-chuan-zhuan-huan-cheng-zheng-shu-lcof" xr:uid="{C28D6499-074A-4298-B56B-4B1A8AA4916B}"/>
+    <hyperlink ref="B76" r:id="rId74" display="https://leetcode-cn.com/problems/er-cha-sou-suo-shu-de-zui-jin-gong-gong-zu-xian-lcof" xr:uid="{24DE338F-690B-420B-913B-C6D99FBE592E}"/>
+    <hyperlink ref="B77" r:id="rId75" display="https://leetcode-cn.com/problems/er-cha-shu-de-zui-jin-gong-gong-zu-xian-lcof" xr:uid="{35FF0319-BBA2-492F-8458-45AAEEA67F96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="300" r:id="rId76"/>

</xml_diff>

<commit_message>
add problem162& 278 and update 152&33
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BF648F-3D8E-4F62-AB2A-7C5B22B0716D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1A17E5-3DBC-4542-AD8F-024FCB9F3754}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5325" yWindow="915" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4349" uniqueCount="2508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4351" uniqueCount="2510">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -7559,6 +7559,12 @@
   </si>
   <si>
     <t>2020.6.17</t>
+  </si>
+  <si>
+    <t>2020.6.18(self)</t>
+  </si>
+  <si>
+    <t>2020.6.18</t>
   </si>
 </sst>
 </file>
@@ -8160,8 +8166,8 @@
   <dimension ref="A1:E1653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J63" sqref="J63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D163" sqref="D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10195,7 +10201,9 @@
       <c r="C163" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D163" s="4"/>
+      <c r="D163" s="4" t="s">
+        <v>2509</v>
+      </c>
     </row>
     <row r="164" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="20" t="s">
@@ -11605,7 +11613,9 @@
       <c r="C279" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D279" s="4"/>
+      <c r="D279" s="4" t="s">
+        <v>2508</v>
+      </c>
     </row>
     <row r="280" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A280" s="18">

</xml_diff>

<commit_message>
add 4 & 287
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650A0F2D-60C8-4A75-AC9D-B87EE95BCB3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678177D3-C8E4-4D70-95BF-0D6A18286869}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11325" yWindow="1410" windowWidth="28800" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4359" uniqueCount="2514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4363" uniqueCount="2515">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -7577,6 +7577,9 @@
   </si>
   <si>
     <t>2020,.6.20</t>
+  </si>
+  <si>
+    <t>2020.6.22</t>
   </si>
 </sst>
 </file>
@@ -8177,9 +8180,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36439EE-948F-4B95-AA31-6B4987F28A76}">
   <dimension ref="A1:E1653"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D351" sqref="D351"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8263,7 +8266,9 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>2514</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18">
@@ -11745,7 +11750,9 @@
       <c r="C288" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D288" s="3"/>
+      <c r="D288" s="3" t="s">
+        <v>2514</v>
+      </c>
     </row>
     <row r="289" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A289" s="20" t="s">
@@ -13235,7 +13242,9 @@
       <c r="C411" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D411" s="4"/>
+      <c r="D411" s="4" t="s">
+        <v>2514</v>
+      </c>
     </row>
     <row r="412" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A412" s="20" t="s">
@@ -16965,7 +16974,9 @@
       <c r="C720" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D720" s="3"/>
+      <c r="D720" s="3" t="s">
+        <v>2514</v>
+      </c>
     </row>
     <row r="721" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A721" s="19">
@@ -31454,7 +31465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3974A999-81B9-4707-8EBA-5693F79999D0}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20:C53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add 111&107&637 and update 102
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\N-5CG82730HK-Data\fuyao\Desktop\cpp\FLY\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA4C59A-4767-4995-97B0-E06DC5ABB151}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B14C929-0BD5-4FED-ADE8-5488FACB0390}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3345" windowWidth="27375" windowHeight="11385" firstSheet="8" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11835" yWindow="420" windowWidth="27375" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7125" uniqueCount="3655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7128" uniqueCount="3656">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -10505,9 +10505,6 @@
     <t>Balanced Binary Tree</t>
   </si>
   <si>
-    <t>#776</t>
-  </si>
-  <si>
     <t>Split BST</t>
   </si>
   <si>
@@ -11043,6 +11040,12 @@
   </si>
   <si>
     <t>2020.8.10</t>
+  </si>
+  <si>
+    <t>#$776</t>
+  </si>
+  <si>
+    <t>2020.8.11(self)</t>
   </si>
 </sst>
 </file>
@@ -12357,8 +12360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1701"/>
   <sheetViews>
-    <sheetView topLeftCell="A613" workbookViewId="0">
-      <selection activeCell="D618" sqref="D618"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13640,7 +13643,7 @@
         <v>7</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13678,7 +13681,7 @@
         <v>5</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13692,7 +13695,7 @@
         <v>7</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13718,7 +13721,7 @@
         <v>5</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13732,7 +13735,7 @@
         <v>7</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13746,7 +13749,7 @@
         <v>7</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13759,7 +13762,9 @@
       <c r="C108" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>3655</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="10">
@@ -13772,7 +13777,7 @@
         <v>5</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13798,7 +13803,7 @@
         <v>5</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13811,7 +13816,9 @@
       <c r="C112" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D112" s="3"/>
+      <c r="D112" s="3" t="s">
+        <v>3655</v>
+      </c>
     </row>
     <row r="113" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="10">
@@ -13824,7 +13831,7 @@
         <v>5</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13874,7 +13881,7 @@
         <v>7</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -13888,7 +13895,7 @@
         <v>7</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14604,7 +14611,7 @@
         <v>7</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="175" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14826,7 +14833,7 @@
         <v>5</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="192" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14840,7 +14847,7 @@
         <v>5</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="193" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -14926,7 +14933,7 @@
         <v>5</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15006,7 +15013,7 @@
         <v>5</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="206" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15060,7 +15067,7 @@
         <v>7</v>
       </c>
       <c r="D209" s="4" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15100,7 +15107,7 @@
         <v>7</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="213" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15114,7 +15121,7 @@
         <v>10</v>
       </c>
       <c r="D213" s="4" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15216,7 +15223,7 @@
         <v>7</v>
       </c>
       <c r="D221" s="4" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
     </row>
     <row r="222" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15292,7 +15299,7 @@
         <v>5</v>
       </c>
       <c r="D227" s="4" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="228" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15354,7 +15361,7 @@
         <v>5</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="233" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15408,7 +15415,7 @@
         <v>5</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="237" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -15422,7 +15429,7 @@
         <v>7</v>
       </c>
       <c r="D237" s="4" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="238" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16088,7 +16095,7 @@
         <v>5</v>
       </c>
       <c r="D291" s="4" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
     </row>
     <row r="292" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16174,7 +16181,7 @@
         <v>10</v>
       </c>
       <c r="D298" s="3" t="s">
-        <v>3644</v>
+        <v>3643</v>
       </c>
     </row>
     <row r="299" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16200,7 +16207,7 @@
         <v>5</v>
       </c>
       <c r="D300" s="3" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="301" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16250,7 +16257,7 @@
         <v>5</v>
       </c>
       <c r="D304" s="3" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="305" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16650,7 +16657,7 @@
         <v>10</v>
       </c>
       <c r="D337" s="4" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="338" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16724,7 +16731,7 @@
         <v>5</v>
       </c>
       <c r="D343" s="4" t="s">
-        <v>3630</v>
+        <v>3629</v>
       </c>
     </row>
     <row r="344" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17086,7 +17093,7 @@
         <v>5</v>
       </c>
       <c r="D372" s="3" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="373" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17312,7 +17319,7 @@
         <v>5</v>
       </c>
       <c r="D390" s="3" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="391" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17350,7 +17357,7 @@
         <v>5</v>
       </c>
       <c r="D393" s="4" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="394" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17462,7 +17469,7 @@
         <v>5</v>
       </c>
       <c r="D402" s="3" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="403" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17512,7 +17519,7 @@
         <v>5</v>
       </c>
       <c r="D406" s="3" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="407" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17562,7 +17569,7 @@
         <v>5</v>
       </c>
       <c r="D410" s="3" t="s">
-        <v>3637</v>
+        <v>3636</v>
       </c>
     </row>
     <row r="411" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17714,7 +17721,7 @@
         <v>7</v>
       </c>
       <c r="D422" s="3" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
     </row>
     <row r="423" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17812,7 +17819,7 @@
         <v>7</v>
       </c>
       <c r="D430" s="3" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="431" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -17962,7 +17969,7 @@
         <v>5</v>
       </c>
       <c r="D442" s="3" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="443" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18038,7 +18045,7 @@
         <v>5</v>
       </c>
       <c r="D448" s="3" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="449" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18078,7 +18085,7 @@
         <v>7</v>
       </c>
       <c r="D451" s="4" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="452" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18142,7 +18149,7 @@
         <v>5</v>
       </c>
       <c r="D456" s="3" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
     </row>
     <row r="457" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18218,7 +18225,7 @@
         <v>5</v>
       </c>
       <c r="D462" s="3" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="463" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18244,7 +18251,7 @@
         <v>5</v>
       </c>
       <c r="D464" s="3" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="465" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18390,7 +18397,7 @@
         <v>5</v>
       </c>
       <c r="D476" s="3" t="s">
-        <v>3627</v>
+        <v>3626</v>
       </c>
     </row>
     <row r="477" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18404,7 +18411,7 @@
         <v>5</v>
       </c>
       <c r="D477" s="4" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="478" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -18702,7 +18709,7 @@
         <v>5</v>
       </c>
       <c r="D501" s="4" t="s">
-        <v>3635</v>
+        <v>3634</v>
       </c>
     </row>
     <row r="502" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19428,7 +19435,7 @@
         <v>5</v>
       </c>
       <c r="D560" s="3" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
     </row>
     <row r="561" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19626,7 +19633,7 @@
         <v>5</v>
       </c>
       <c r="D576" s="3" t="s">
-        <v>3633</v>
+        <v>3632</v>
       </c>
     </row>
     <row r="577" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19798,7 +19805,7 @@
         <v>5</v>
       </c>
       <c r="D590" s="3" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="591" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19812,7 +19819,7 @@
         <v>5</v>
       </c>
       <c r="D591" s="4" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
     </row>
     <row r="592" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19862,7 +19869,7 @@
         <v>5</v>
       </c>
       <c r="D595" s="4" t="s">
-        <v>3634</v>
+        <v>3633</v>
       </c>
     </row>
     <row r="596" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20146,7 +20153,7 @@
         <v>5</v>
       </c>
       <c r="D618" s="3" t="s">
-        <v>3654</v>
+        <v>3653</v>
       </c>
     </row>
     <row r="619" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20391,7 +20398,9 @@
       <c r="C638" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D638" s="3"/>
+      <c r="D638" s="3" t="s">
+        <v>3655</v>
+      </c>
     </row>
     <row r="639" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A639" s="10">
@@ -20490,7 +20499,7 @@
         <v>5</v>
       </c>
       <c r="D646" s="3" t="s">
-        <v>3631</v>
+        <v>3630</v>
       </c>
     </row>
     <row r="647" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20528,7 +20537,7 @@
         <v>7</v>
       </c>
       <c r="D649" s="4" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="650" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -20890,7 +20899,7 @@
         <v>7</v>
       </c>
       <c r="D678" s="3" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
     </row>
     <row r="679" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21054,7 +21063,7 @@
         <v>5</v>
       </c>
       <c r="D691" s="4" t="s">
-        <v>3636</v>
+        <v>3635</v>
       </c>
     </row>
     <row r="692" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21092,7 +21101,7 @@
         <v>5</v>
       </c>
       <c r="D694" s="3" t="s">
-        <v>3629</v>
+        <v>3628</v>
       </c>
     </row>
     <row r="695" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21182,7 +21191,7 @@
         <v>5</v>
       </c>
       <c r="D701" s="4" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="702" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21196,7 +21205,7 @@
         <v>7</v>
       </c>
       <c r="D702" s="3" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="703" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21222,7 +21231,7 @@
         <v>5</v>
       </c>
       <c r="D704" s="3" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
     </row>
     <row r="705" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21440,7 +21449,7 @@
         <v>5</v>
       </c>
       <c r="D721" s="4" t="s">
-        <v>3632</v>
+        <v>3631</v>
       </c>
     </row>
     <row r="722" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -22778,7 +22787,7 @@
         <v>5</v>
       </c>
       <c r="D831" s="4" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
     </row>
     <row r="832" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -23490,7 +23499,7 @@
         <v>7</v>
       </c>
       <c r="D890" s="3" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
     </row>
     <row r="891" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -24940,7 +24949,7 @@
         <v>5</v>
       </c>
       <c r="D1010" s="3" t="s">
-        <v>3628</v>
+        <v>3627</v>
       </c>
     </row>
     <row r="1011" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25136,7 +25145,7 @@
         <v>5</v>
       </c>
       <c r="D1026" s="3" t="s">
-        <v>3638</v>
+        <v>3637</v>
       </c>
     </row>
     <row r="1027" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -37924,7 +37933,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>3626</v>
+        <v>3625</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -39748,8 +39757,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39794,13 +39803,13 @@
       </c>
     </row>
     <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="22">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="22" t="s">
         <v>2860</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="22" t="s">
         <v>2859</v>
       </c>
       <c r="D4" s="32" t="s">
@@ -39878,13 +39887,13 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="22">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="22" t="s">
         <v>3427</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="22" t="s">
         <v>3428</v>
       </c>
       <c r="D10" s="22" t="s">
@@ -39920,13 +39929,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="22">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="22" t="s">
         <v>2284</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="22" t="s">
         <v>2285</v>
       </c>
       <c r="D13" s="32" t="s">
@@ -40032,13 +40041,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="22">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="22" t="s">
         <v>3445</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="22" t="s">
         <v>3446</v>
       </c>
       <c r="D21" s="32" t="s">
@@ -40046,13 +40055,13 @@
       </c>
     </row>
     <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="22" t="s">
         <v>2848</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="22" t="s">
         <v>2847</v>
       </c>
       <c r="D22" s="32" t="s">
@@ -40116,13 +40125,13 @@
       </c>
     </row>
     <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="22">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="22" t="s">
         <v>2840</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="22" t="s">
         <v>2839</v>
       </c>
       <c r="D27" s="21" t="s">
@@ -40186,13 +40195,13 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="22">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="22" t="s">
         <v>3461</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="22" t="s">
         <v>3462</v>
       </c>
       <c r="D32" s="22" t="s">
@@ -40200,13 +40209,13 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="22">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="22" t="s">
         <v>3463</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="22" t="s">
         <v>3464</v>
       </c>
       <c r="D33" s="22" t="s">
@@ -40228,13 +40237,13 @@
       </c>
     </row>
     <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="22">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="22" t="s">
         <v>2838</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="22" t="s">
         <v>2837</v>
       </c>
       <c r="D35" s="32" t="s">
@@ -40298,14 +40307,14 @@
       </c>
     </row>
     <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="31">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="31" t="s">
+        <v>3654</v>
+      </c>
+      <c r="C40" s="31" t="s">
         <v>3475</v>
-      </c>
-      <c r="C40" t="s">
-        <v>3476</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>7</v>
@@ -40316,10 +40325,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>3476</v>
+      </c>
+      <c r="C41" t="s">
         <v>3477</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3478</v>
       </c>
       <c r="D41" s="21" t="s">
         <v>10</v>
@@ -40330,10 +40339,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
+        <v>3478</v>
+      </c>
+      <c r="C42" t="s">
         <v>3479</v>
-      </c>
-      <c r="C42" t="s">
-        <v>3480</v>
       </c>
       <c r="D42" s="32" t="s">
         <v>7</v>
@@ -40358,10 +40367,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>3480</v>
+      </c>
+      <c r="C44" t="s">
         <v>3481</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3482</v>
       </c>
       <c r="D44" s="22" t="s">
         <v>5</v>
@@ -40372,10 +40381,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>3482</v>
+      </c>
+      <c r="C45" t="s">
         <v>3483</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3484</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>7</v>
@@ -40386,10 +40395,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="22" t="s">
+        <v>3484</v>
+      </c>
+      <c r="C46" s="22" t="s">
         <v>3485</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>3486</v>
       </c>
       <c r="D46" s="22" t="s">
         <v>5</v>
@@ -40400,10 +40409,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C47" t="s">
         <v>3487</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3488</v>
       </c>
       <c r="D47" s="32" t="s">
         <v>7</v>
@@ -40414,10 +40423,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>3488</v>
+      </c>
+      <c r="C48" t="s">
         <v>3489</v>
-      </c>
-      <c r="C48" t="s">
-        <v>3490</v>
       </c>
       <c r="D48" s="21" t="s">
         <v>10</v>
@@ -40428,10 +40437,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>3490</v>
+      </c>
+      <c r="C49" t="s">
         <v>3491</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3492</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>7</v>
@@ -40442,10 +40451,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>3492</v>
+      </c>
+      <c r="C50" t="s">
         <v>3493</v>
-      </c>
-      <c r="C50" t="s">
-        <v>3494</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>7</v>
@@ -40470,10 +40479,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>3494</v>
+      </c>
+      <c r="C52" t="s">
         <v>3495</v>
-      </c>
-      <c r="C52" t="s">
-        <v>3496</v>
       </c>
       <c r="D52" s="32" t="s">
         <v>7</v>
@@ -40484,10 +40493,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C53" t="s">
         <v>3497</v>
-      </c>
-      <c r="C53" t="s">
-        <v>3498</v>
       </c>
       <c r="D53" s="32" t="s">
         <v>7</v>
@@ -40540,10 +40549,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>3498</v>
+      </c>
+      <c r="C57" t="s">
         <v>3499</v>
-      </c>
-      <c r="C57" t="s">
-        <v>3500</v>
       </c>
       <c r="D57" s="32" t="s">
         <v>7</v>
@@ -40554,10 +40563,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>3500</v>
+      </c>
+      <c r="C58" t="s">
         <v>3501</v>
-      </c>
-      <c r="C58" t="s">
-        <v>3502</v>
       </c>
       <c r="D58" s="32" t="s">
         <v>7</v>
@@ -40568,10 +40577,10 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
+        <v>3502</v>
+      </c>
+      <c r="C59" t="s">
         <v>3503</v>
-      </c>
-      <c r="C59" t="s">
-        <v>3504</v>
       </c>
       <c r="D59" s="22" t="s">
         <v>5</v>
@@ -40582,10 +40591,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>3504</v>
+      </c>
+      <c r="C60" t="s">
         <v>3505</v>
-      </c>
-      <c r="C60" t="s">
-        <v>3506</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>7</v>
@@ -40596,10 +40605,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>3506</v>
+      </c>
+      <c r="C61" t="s">
         <v>3507</v>
-      </c>
-      <c r="C61" t="s">
-        <v>3508</v>
       </c>
       <c r="D61" s="22" t="s">
         <v>5</v>
@@ -40610,10 +40619,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>3508</v>
+      </c>
+      <c r="C62" t="s">
         <v>3509</v>
-      </c>
-      <c r="C62" t="s">
-        <v>3510</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>5</v>
@@ -40624,10 +40633,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
+        <v>3510</v>
+      </c>
+      <c r="C63" t="s">
         <v>3511</v>
-      </c>
-      <c r="C63" t="s">
-        <v>3512</v>
       </c>
       <c r="D63" s="32" t="s">
         <v>7</v>
@@ -40638,10 +40647,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>3512</v>
+      </c>
+      <c r="C64" t="s">
         <v>3513</v>
-      </c>
-      <c r="C64" t="s">
-        <v>3514</v>
       </c>
       <c r="D64" s="32" t="s">
         <v>7</v>
@@ -40652,10 +40661,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>3514</v>
+      </c>
+      <c r="C65" t="s">
         <v>3515</v>
-      </c>
-      <c r="C65" t="s">
-        <v>3516</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>10</v>
@@ -40666,10 +40675,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>3516</v>
+      </c>
+      <c r="C66" t="s">
         <v>3517</v>
-      </c>
-      <c r="C66" t="s">
-        <v>3518</v>
       </c>
       <c r="D66" s="32" t="s">
         <v>7</v>
@@ -40680,10 +40689,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>3518</v>
+      </c>
+      <c r="C67" t="s">
         <v>3519</v>
-      </c>
-      <c r="C67" t="s">
-        <v>3520</v>
       </c>
       <c r="D67" s="32" t="s">
         <v>7</v>
@@ -40694,10 +40703,10 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
+        <v>3520</v>
+      </c>
+      <c r="C68" t="s">
         <v>3521</v>
-      </c>
-      <c r="C68" t="s">
-        <v>3522</v>
       </c>
       <c r="D68" s="32" t="s">
         <v>7</v>
@@ -40722,10 +40731,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>3522</v>
+      </c>
+      <c r="C70" t="s">
         <v>3523</v>
-      </c>
-      <c r="C70" t="s">
-        <v>3524</v>
       </c>
       <c r="D70" s="32" t="s">
         <v>7</v>
@@ -40736,10 +40745,10 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
+        <v>3524</v>
+      </c>
+      <c r="C71" t="s">
         <v>3525</v>
-      </c>
-      <c r="C71" t="s">
-        <v>3526</v>
       </c>
       <c r="D71" s="32" t="s">
         <v>7</v>
@@ -40750,10 +40759,10 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
+        <v>3526</v>
+      </c>
+      <c r="C72" t="s">
         <v>3527</v>
-      </c>
-      <c r="C72" t="s">
-        <v>3528</v>
       </c>
       <c r="D72" s="32" t="s">
         <v>7</v>
@@ -40764,10 +40773,10 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
+        <v>3528</v>
+      </c>
+      <c r="C73" t="s">
         <v>3529</v>
-      </c>
-      <c r="C73" t="s">
-        <v>3530</v>
       </c>
       <c r="D73" s="32" t="s">
         <v>7</v>
@@ -40792,10 +40801,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
+        <v>3530</v>
+      </c>
+      <c r="C75" t="s">
         <v>3531</v>
-      </c>
-      <c r="C75" t="s">
-        <v>3532</v>
       </c>
       <c r="D75" s="32" t="s">
         <v>7</v>
@@ -40820,10 +40829,10 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
+        <v>3532</v>
+      </c>
+      <c r="C77" t="s">
         <v>3533</v>
-      </c>
-      <c r="C77" t="s">
-        <v>3534</v>
       </c>
       <c r="D77" s="32" t="s">
         <v>7</v>
@@ -40834,10 +40843,10 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
+        <v>3534</v>
+      </c>
+      <c r="C78" t="s">
         <v>3535</v>
-      </c>
-      <c r="C78" t="s">
-        <v>3536</v>
       </c>
       <c r="D78" s="32" t="s">
         <v>7</v>
@@ -40862,10 +40871,10 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
+        <v>3536</v>
+      </c>
+      <c r="C80" t="s">
         <v>3537</v>
-      </c>
-      <c r="C80" t="s">
-        <v>3538</v>
       </c>
       <c r="D80" s="32" t="s">
         <v>7</v>
@@ -40876,10 +40885,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
+        <v>3538</v>
+      </c>
+      <c r="C81" t="s">
         <v>3539</v>
-      </c>
-      <c r="C81" t="s">
-        <v>3540</v>
       </c>
       <c r="D81" s="32" t="s">
         <v>7</v>
@@ -40904,10 +40913,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
+        <v>3540</v>
+      </c>
+      <c r="C83" t="s">
         <v>3541</v>
-      </c>
-      <c r="C83" t="s">
-        <v>3542</v>
       </c>
       <c r="D83" s="32" t="s">
         <v>7</v>
@@ -40918,10 +40927,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
+        <v>3542</v>
+      </c>
+      <c r="C84" t="s">
         <v>3543</v>
-      </c>
-      <c r="C84" t="s">
-        <v>3544</v>
       </c>
       <c r="D84" s="32" t="s">
         <v>7</v>
@@ -41102,7 +41111,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -41127,10 +41136,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3545</v>
+      </c>
+      <c r="C3" t="s">
         <v>3546</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3547</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>10</v>
@@ -41225,10 +41234,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>3547</v>
+      </c>
+      <c r="C10" t="s">
         <v>3548</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3549</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>10</v>
@@ -41267,10 +41276,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>3549</v>
+      </c>
+      <c r="C13" t="s">
         <v>3550</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3551</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>7</v>
@@ -41295,10 +41304,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>3551</v>
+      </c>
+      <c r="C15" t="s">
         <v>3552</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3553</v>
       </c>
       <c r="D15" s="32" t="s">
         <v>7</v>
@@ -41309,10 +41318,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>3553</v>
+      </c>
+      <c r="C16" t="s">
         <v>3554</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3555</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>7</v>
@@ -41337,10 +41346,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C18" t="s">
         <v>3556</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3557</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>10</v>
@@ -41435,10 +41444,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>3557</v>
+      </c>
+      <c r="C25" t="s">
         <v>3558</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3559</v>
       </c>
       <c r="D25" s="32" t="s">
         <v>7</v>
@@ -41463,10 +41472,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>3559</v>
+      </c>
+      <c r="C27" t="s">
         <v>3560</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3561</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>7</v>
@@ -41491,10 +41500,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>3561</v>
+      </c>
+      <c r="C29" t="s">
         <v>3562</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3563</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>10</v>
@@ -41505,10 +41514,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>3563</v>
+      </c>
+      <c r="C30" t="s">
         <v>3564</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3565</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>7</v>
@@ -41547,10 +41556,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>3476</v>
+      </c>
+      <c r="C33" t="s">
         <v>3477</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3478</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>10</v>
@@ -41561,10 +41570,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>3478</v>
+      </c>
+      <c r="C34" t="s">
         <v>3479</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3480</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>7</v>
@@ -41575,10 +41584,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>3565</v>
+      </c>
+      <c r="C35" t="s">
         <v>3566</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3567</v>
       </c>
       <c r="D35" s="32" t="s">
         <v>7</v>
@@ -41589,10 +41598,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C36" t="s">
         <v>3487</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3488</v>
       </c>
       <c r="D36" s="32" t="s">
         <v>7</v>
@@ -41603,10 +41612,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
+        <v>3567</v>
+      </c>
+      <c r="C37" t="s">
         <v>3568</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3569</v>
       </c>
       <c r="D37" s="32" t="s">
         <v>7</v>
@@ -41617,10 +41626,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>3569</v>
+      </c>
+      <c r="C38" t="s">
         <v>3570</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3571</v>
       </c>
       <c r="D38" s="22" t="s">
         <v>5</v>
@@ -41631,10 +41640,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
+        <v>3492</v>
+      </c>
+      <c r="C39" t="s">
         <v>3493</v>
-      </c>
-      <c r="C39" t="s">
-        <v>3494</v>
       </c>
       <c r="D39" s="32" t="s">
         <v>7</v>
@@ -41645,10 +41654,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
+        <v>3571</v>
+      </c>
+      <c r="C40" t="s">
         <v>3572</v>
-      </c>
-      <c r="C40" t="s">
-        <v>3573</v>
       </c>
       <c r="D40" s="32" t="s">
         <v>7</v>
@@ -41659,10 +41668,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
+        <v>3496</v>
+      </c>
+      <c r="C41" t="s">
         <v>3497</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3498</v>
       </c>
       <c r="D41" s="32" t="s">
         <v>7</v>
@@ -41701,10 +41710,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
+        <v>3573</v>
+      </c>
+      <c r="C44" t="s">
         <v>3574</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3575</v>
       </c>
       <c r="D44" s="32" t="s">
         <v>7</v>
@@ -41715,10 +41724,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
+        <v>3575</v>
+      </c>
+      <c r="C45" t="s">
         <v>3576</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3577</v>
       </c>
       <c r="D45" s="32" t="s">
         <v>7</v>
@@ -41729,10 +41738,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C46" t="s">
         <v>3578</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3579</v>
       </c>
       <c r="D46" s="32" t="s">
         <v>7</v>
@@ -41757,10 +41766,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
+        <v>3498</v>
+      </c>
+      <c r="C48" t="s">
         <v>3499</v>
-      </c>
-      <c r="C48" t="s">
-        <v>3500</v>
       </c>
       <c r="D48" s="32" t="s">
         <v>7</v>
@@ -41771,10 +41780,10 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
+        <v>3504</v>
+      </c>
+      <c r="C49" t="s">
         <v>3505</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3506</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>7</v>
@@ -41785,10 +41794,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>3579</v>
+      </c>
+      <c r="C50" t="s">
         <v>3580</v>
-      </c>
-      <c r="C50" t="s">
-        <v>3581</v>
       </c>
       <c r="D50" s="32" t="s">
         <v>7</v>
@@ -41799,10 +41808,10 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
+        <v>3581</v>
+      </c>
+      <c r="C51" t="s">
         <v>3582</v>
-      </c>
-      <c r="C51" t="s">
-        <v>3583</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>7</v>
@@ -41841,10 +41850,10 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
+        <v>3514</v>
+      </c>
+      <c r="C54" t="s">
         <v>3515</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3516</v>
       </c>
       <c r="D54" s="21" t="s">
         <v>10</v>
@@ -41869,10 +41878,10 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
+        <v>3583</v>
+      </c>
+      <c r="C56" t="s">
         <v>3584</v>
-      </c>
-      <c r="C56" t="s">
-        <v>3585</v>
       </c>
       <c r="D56" s="32" t="s">
         <v>7</v>
@@ -41883,10 +41892,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
+        <v>3585</v>
+      </c>
+      <c r="C57" t="s">
         <v>3586</v>
-      </c>
-      <c r="C57" t="s">
-        <v>3587</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>5</v>
@@ -41897,10 +41906,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
+        <v>3518</v>
+      </c>
+      <c r="C58" t="s">
         <v>3519</v>
-      </c>
-      <c r="C58" t="s">
-        <v>3520</v>
       </c>
       <c r="D58" s="32" t="s">
         <v>7</v>
@@ -41925,10 +41934,10 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
+        <v>3587</v>
+      </c>
+      <c r="C60" t="s">
         <v>3588</v>
-      </c>
-      <c r="C60" t="s">
-        <v>3589</v>
       </c>
       <c r="D60" s="32" t="s">
         <v>7</v>
@@ -41939,10 +41948,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
+        <v>3589</v>
+      </c>
+      <c r="C61" t="s">
         <v>3590</v>
-      </c>
-      <c r="C61" t="s">
-        <v>3591</v>
       </c>
       <c r="D61" s="32" t="s">
         <v>7</v>
@@ -41953,10 +41962,10 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
+        <v>3526</v>
+      </c>
+      <c r="C62" t="s">
         <v>3527</v>
-      </c>
-      <c r="C62" t="s">
-        <v>3528</v>
       </c>
       <c r="D62" s="32" t="s">
         <v>7</v>
@@ -41981,10 +41990,10 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
+        <v>3591</v>
+      </c>
+      <c r="C64" t="s">
         <v>3592</v>
-      </c>
-      <c r="C64" t="s">
-        <v>3593</v>
       </c>
       <c r="D64" s="32" t="s">
         <v>7</v>
@@ -41995,10 +42004,10 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
+        <v>3593</v>
+      </c>
+      <c r="C65" t="s">
         <v>3594</v>
-      </c>
-      <c r="C65" t="s">
-        <v>3595</v>
       </c>
       <c r="D65" s="21" t="s">
         <v>10</v>
@@ -42009,10 +42018,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
+        <v>3595</v>
+      </c>
+      <c r="C66" t="s">
         <v>3596</v>
-      </c>
-      <c r="C66" t="s">
-        <v>3597</v>
       </c>
       <c r="D66" s="32" t="s">
         <v>7</v>
@@ -42023,10 +42032,10 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
+        <v>3597</v>
+      </c>
+      <c r="C67" t="s">
         <v>3598</v>
-      </c>
-      <c r="C67" t="s">
-        <v>3599</v>
       </c>
       <c r="D67" s="32" t="s">
         <v>7</v>
@@ -42051,10 +42060,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
+        <v>3538</v>
+      </c>
+      <c r="C69" t="s">
         <v>3539</v>
-      </c>
-      <c r="C69" t="s">
-        <v>3540</v>
       </c>
       <c r="D69" s="32" t="s">
         <v>7</v>
@@ -42065,10 +42074,10 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
+        <v>3599</v>
+      </c>
+      <c r="C70" t="s">
         <v>3600</v>
-      </c>
-      <c r="C70" t="s">
-        <v>3601</v>
       </c>
       <c r="D70" s="32" t="s">
         <v>7</v>
@@ -42113,7 +42122,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>3602</v>
+        <v>3601</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -42194,10 +42203,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>3549</v>
+      </c>
+      <c r="C7" t="s">
         <v>3550</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3551</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>7</v>
@@ -42222,10 +42231,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>3553</v>
+      </c>
+      <c r="C9" t="s">
         <v>3554</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3555</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>7</v>
@@ -42236,10 +42245,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>3555</v>
+      </c>
+      <c r="C10" t="s">
         <v>3556</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3557</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>10</v>
@@ -42278,10 +42287,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>3557</v>
+      </c>
+      <c r="C13" t="s">
         <v>3558</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3559</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>7</v>
@@ -42292,10 +42301,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>3559</v>
+      </c>
+      <c r="C14" t="s">
         <v>3560</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3561</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>7</v>
@@ -42306,10 +42315,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>3602</v>
+      </c>
+      <c r="C15" t="s">
         <v>3603</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3604</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>10</v>
@@ -42320,10 +42329,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>3604</v>
+      </c>
+      <c r="C16" t="s">
         <v>3605</v>
-      </c>
-      <c r="C16" t="s">
-        <v>3606</v>
       </c>
       <c r="D16" s="32" t="s">
         <v>7</v>
@@ -42348,10 +42357,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>3563</v>
+      </c>
+      <c r="C18" t="s">
         <v>3564</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3565</v>
       </c>
       <c r="D18" s="32" t="s">
         <v>7</v>
@@ -42376,10 +42385,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
+        <v>3486</v>
+      </c>
+      <c r="C20" t="s">
         <v>3487</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3488</v>
       </c>
       <c r="D20" s="32" t="s">
         <v>7</v>
@@ -42390,10 +42399,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
+        <v>3492</v>
+      </c>
+      <c r="C21" t="s">
         <v>3493</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3494</v>
       </c>
       <c r="D21" s="32" t="s">
         <v>7</v>
@@ -42404,10 +42413,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
+        <v>3606</v>
+      </c>
+      <c r="C22" t="s">
         <v>3607</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3608</v>
       </c>
       <c r="D22" s="32" t="s">
         <v>7</v>
@@ -42418,10 +42427,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
+        <v>3573</v>
+      </c>
+      <c r="C23" t="s">
         <v>3574</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3575</v>
       </c>
       <c r="D23" s="32" t="s">
         <v>7</v>
@@ -42432,10 +42441,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>3577</v>
+      </c>
+      <c r="C24" t="s">
         <v>3578</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3579</v>
       </c>
       <c r="D24" s="32" t="s">
         <v>7</v>
@@ -42446,10 +42455,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
+        <v>3608</v>
+      </c>
+      <c r="C25" t="s">
         <v>3609</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3610</v>
       </c>
       <c r="D25" s="21" t="s">
         <v>10</v>
@@ -42460,10 +42469,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
+        <v>3610</v>
+      </c>
+      <c r="C26" t="s">
         <v>3611</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3612</v>
       </c>
       <c r="D26" s="32" t="s">
         <v>7</v>
@@ -42488,10 +42497,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>3581</v>
+      </c>
+      <c r="C28" t="s">
         <v>3582</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3583</v>
       </c>
       <c r="D28" s="32" t="s">
         <v>7</v>
@@ -42502,10 +42511,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
+        <v>3612</v>
+      </c>
+      <c r="C29" t="s">
         <v>3613</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3614</v>
       </c>
       <c r="D29" s="21" t="s">
         <v>10</v>
@@ -42516,10 +42525,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
+        <v>3587</v>
+      </c>
+      <c r="C30" t="s">
         <v>3588</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3589</v>
       </c>
       <c r="D30" s="32" t="s">
         <v>7</v>
@@ -42530,10 +42539,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
+        <v>3614</v>
+      </c>
+      <c r="C31" t="s">
         <v>3615</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3616</v>
       </c>
       <c r="D31" s="32" t="s">
         <v>7</v>
@@ -42544,10 +42553,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
+        <v>3589</v>
+      </c>
+      <c r="C32" t="s">
         <v>3590</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3591</v>
       </c>
       <c r="D32" s="32" t="s">
         <v>7</v>
@@ -42558,10 +42567,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
+        <v>3616</v>
+      </c>
+      <c r="C33" t="s">
         <v>3617</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3618</v>
       </c>
       <c r="D33" s="21" t="s">
         <v>10</v>
@@ -42572,10 +42581,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>3591</v>
+      </c>
+      <c r="C34" t="s">
         <v>3592</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3593</v>
       </c>
       <c r="D34" s="32" t="s">
         <v>7</v>
@@ -42586,10 +42595,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
+        <v>3593</v>
+      </c>
+      <c r="C35" t="s">
         <v>3594</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3595</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>10</v>
@@ -42600,10 +42609,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
+        <v>3595</v>
+      </c>
+      <c r="C36" t="s">
         <v>3596</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3597</v>
       </c>
       <c r="D36" s="32" t="s">
         <v>7</v>
@@ -42634,7 +42643,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
-        <v>3619</v>
+        <v>3618</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -42659,10 +42668,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>3619</v>
+      </c>
+      <c r="C3" t="s">
         <v>3620</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3621</v>
       </c>
       <c r="D3" s="32" t="s">
         <v>7</v>
@@ -42673,10 +42682,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>3557</v>
+      </c>
+      <c r="C4" t="s">
         <v>3558</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3559</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>7</v>
@@ -42687,10 +42696,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>3559</v>
+      </c>
+      <c r="C5" t="s">
         <v>3560</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3561</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>7</v>
@@ -42701,10 +42710,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>3565</v>
+      </c>
+      <c r="C6" t="s">
         <v>3566</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3567</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>7</v>
@@ -42715,10 +42724,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>3482</v>
+      </c>
+      <c r="C7" t="s">
         <v>3483</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3484</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>7</v>
@@ -42729,10 +42738,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>3610</v>
+      </c>
+      <c r="C8" t="s">
         <v>3611</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3612</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>7</v>
@@ -42743,10 +42752,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>3581</v>
+      </c>
+      <c r="C9" t="s">
         <v>3582</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3583</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>7</v>
@@ -42757,10 +42766,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>3514</v>
+      </c>
+      <c r="C10" t="s">
         <v>3515</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3516</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>10</v>
@@ -42771,10 +42780,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>3621</v>
+      </c>
+      <c r="C11" t="s">
         <v>3622</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3623</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>10</v>
@@ -42785,10 +42794,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>3623</v>
+      </c>
+      <c r="C12" t="s">
         <v>3624</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3625</v>
       </c>
       <c r="D12" s="32" t="s">
         <v>7</v>
@@ -42799,10 +42808,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>3591</v>
+      </c>
+      <c r="C13" t="s">
         <v>3592</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3593</v>
       </c>
       <c r="D13" s="32" t="s">
         <v>7</v>
@@ -42813,10 +42822,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
+        <v>3595</v>
+      </c>
+      <c r="C14" t="s">
         <v>3596</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3597</v>
       </c>
       <c r="D14" s="32" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
add  488&546&679 update Q459
</commit_message>
<xml_diff>
--- a/LeetCode 题目.xlsx
+++ b/LeetCode 题目.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\N-5CG82730HK-Data\fuyao\Desktop\cpp\FLY\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7263CF-9535-4BF9-BFF5-0571C6275480}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6874141F-7C21-4F1F-844F-53D20E926A56}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13245" yWindow="735" windowWidth="13395" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode 题目" sheetId="3" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6939" uniqueCount="3464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6945" uniqueCount="3465">
   <si>
     <t>LeetCode 题目</t>
   </si>
@@ -10470,6 +10470,9 @@
   </si>
   <si>
     <t>2020.8.23(self)</t>
+  </si>
+  <si>
+    <t>2020.8.25</t>
   </si>
 </sst>
 </file>
@@ -11905,8 +11908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1701"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="D223" sqref="D223"/>
+    <sheetView tabSelected="1" topLeftCell="A489" workbookViewId="0">
+      <selection activeCell="D489" sqref="D489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18127,7 +18130,9 @@
       <c r="C489" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D489" s="4"/>
+      <c r="D489" s="4" t="s">
+        <v>3464</v>
+      </c>
     </row>
     <row r="490" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A490" s="10" t="s">
@@ -18851,7 +18856,9 @@
       <c r="C547" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D547" s="4"/>
+      <c r="D547" s="4" t="s">
+        <v>3464</v>
+      </c>
     </row>
     <row r="548" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A548" s="10">
@@ -20515,7 +20522,9 @@
       <c r="C680" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D680" s="3"/>
+      <c r="D680" s="3" t="s">
+        <v>3464</v>
+      </c>
     </row>
     <row r="681" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A681" s="10">
@@ -32514,7 +32523,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32840,7 +32849,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33660,7 +33669,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34821,7 +34830,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35050,7 +35059,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35114,7 +35123,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35310,7 +35319,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35418,7 +35427,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35659,7 +35668,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36021,7 +36030,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37710,7 +37719,7 @@
   <dimension ref="A1:D69"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38647,7 +38656,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38679,18 +38688,21 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="22" t="s">
         <v>3363</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="21" t="s">
         <v>3364</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="41" t="s">
+        <v>3459</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="22" t="s">
         <v>3258</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -38704,7 +38716,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="22" t="s">
         <v>3260</v>
       </c>
       <c r="B5" s="22" t="s">
@@ -38718,18 +38730,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="22" t="s">
         <v>3044</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="21" t="s">
         <v>3045</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>10</v>
       </c>
+      <c r="D6" s="41" t="s">
+        <v>3459</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="30" t="s">
         <v>2792</v>
       </c>
       <c r="B7" s="30" t="s">
@@ -38743,7 +38758,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="30" t="s">
         <v>3268</v>
       </c>
       <c r="B8" s="30" t="s">
@@ -38757,7 +38772,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="30" t="s">
         <v>2284</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -38771,18 +38786,21 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="22" t="s">
         <v>3365</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="21" t="s">
         <v>3366</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>10</v>
       </c>
+      <c r="D10" s="41" t="s">
+        <v>3459</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="22" t="s">
         <v>3270</v>
       </c>
       <c r="B11" s="22" t="s">
@@ -38807,7 +38825,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="30" t="s">
         <v>3367</v>
       </c>
       <c r="B13" s="30" t="s">
@@ -38821,7 +38839,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="30" t="s">
         <v>3278</v>
       </c>
       <c r="B14" s="30" t="s">
@@ -38846,7 +38864,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="30" t="s">
         <v>3371</v>
       </c>
       <c r="B16" s="30" t="s">
@@ -38860,7 +38878,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="22" t="s">
         <v>3280</v>
       </c>
       <c r="B17" s="22" t="s">
@@ -38885,7 +38903,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="21" t="s">
         <v>3288</v>
       </c>
       <c r="B19" s="21" t="s">
@@ -38910,7 +38928,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="22" t="s">
         <v>3290</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -38946,7 +38964,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="22" t="s">
         <v>2940</v>
       </c>
       <c r="B24" s="22" t="s">
@@ -38971,7 +38989,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="22" t="s">
         <v>3294</v>
       </c>
       <c r="B26" s="22" t="s">
@@ -38985,7 +39003,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="30" t="s">
         <v>3377</v>
       </c>
       <c r="B27" s="30" t="s">
@@ -38999,7 +39017,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="22" t="s">
         <v>3298</v>
       </c>
       <c r="B28" s="22" t="s">
@@ -39046,7 +39064,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="22" t="s">
         <v>3310</v>
       </c>
       <c r="B32" s="22" t="s">
@@ -39115,7 +39133,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="22" t="s">
         <v>3387</v>
       </c>
       <c r="B38" s="22" t="s">
@@ -39151,7 +39169,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="30" t="s">
         <v>3332</v>
       </c>
       <c r="B41" s="30" t="s">
@@ -39165,7 +39183,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="30" t="s">
         <v>2390</v>
       </c>
       <c r="B42" s="30" t="s">
@@ -39223,7 +39241,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="30" t="s">
         <v>3134</v>
       </c>
       <c r="B47" s="30" t="s">
@@ -39248,7 +39266,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="30" t="s">
         <v>3340</v>
       </c>
       <c r="B49" s="30" t="s">
@@ -39328,7 +39346,7 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="30" t="s">
         <v>3352</v>
       </c>
       <c r="B56" s="30" t="s">
@@ -39342,7 +39360,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="30" t="s">
         <v>3358</v>
       </c>
       <c r="B57" s="30" t="s">
@@ -40929,7 +40947,7 @@
   <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42495,7 +42513,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43484,7 +43502,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43958,7 +43976,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31:B31"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44336,7 +44354,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44721,7 +44739,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="I228" sqref="I228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>